<commit_message>
Kinovorführung Harold 3.11.24, Verleiherrechnung Margini & Monk, Shows bis Ende 2024 eingespeist.
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72657B64-45A4-4FC1-9C4C-1AF4C6E6F6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AF58E0-999F-4C66-B9CC-4CA8DE8EC983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="256">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -785,6 +785,27 @@
   </si>
   <si>
     <t>26 27680 00000 00000 01005 30821</t>
+  </si>
+  <si>
+    <t>Film: Monk and the Gun</t>
+  </si>
+  <si>
+    <t>00 00000 00000 00000 04400 51932</t>
+  </si>
+  <si>
+    <t>44005193</t>
+  </si>
+  <si>
+    <t>Film: Margini</t>
+  </si>
+  <si>
+    <t>Noah Film Sagl</t>
+  </si>
+  <si>
+    <t>Via Ronchetto 7, 6900 Lugano</t>
+  </si>
+  <si>
+    <t>DS-42.24</t>
   </si>
 </sst>
 </file>
@@ -883,8 +904,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{27287C1A-B7AC-49C2-89D9-0074BB2DB80A}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -947,8 +968,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K71" totalsRowShown="0">
-  <autoFilter ref="A1:K71" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K73" totalsRowShown="0">
+  <autoFilter ref="A1:K73" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K47">
     <sortCondition ref="A1:A47"/>
   </sortState>
@@ -983,9 +1004,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1023,7 +1044,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1129,7 +1150,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1285,18 +1306,18 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.42578125" customWidth="1"/>
+    <col min="7" max="7" width="42.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1319,7 +1340,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -1339,7 +1360,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -1356,7 +1377,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -1373,7 +1394,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -1390,7 +1411,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -1407,7 +1428,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1424,7 +1445,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1441,7 +1462,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1458,7 +1479,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1481,7 +1502,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1504,7 +1525,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1527,7 +1548,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1547,7 +1568,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1570,7 +1591,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1614,26 +1635,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1668,7 +1689,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -1695,7 +1716,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -1722,7 +1743,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -1748,7 +1769,7 @@
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -1772,7 +1793,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -1796,7 +1817,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -1827,7 +1848,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1851,7 +1872,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1875,7 +1896,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1903,7 +1924,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1928,7 +1949,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1953,7 +1974,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1978,7 +1999,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2003,7 +2024,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -2028,7 +2049,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -2056,7 +2077,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2082,7 +2103,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -2106,7 +2127,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -2130,7 +2151,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -2154,7 +2175,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -2178,7 +2199,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -2202,7 +2223,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -2230,7 +2251,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2262,7 +2283,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -2295,7 +2316,7 @@
       </c>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2328,7 +2349,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -2365,7 +2386,7 @@
       <c r="L27" s="11"/>
       <c r="M27" s="11"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -2398,7 +2419,7 @@
       <c r="L28" s="11"/>
       <c r="M28" s="11"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -2431,7 +2452,7 @@
       <c r="L29" s="11"/>
       <c r="M29" s="11"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -2464,7 +2485,7 @@
       <c r="L30" s="11"/>
       <c r="M30" s="11"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -2497,7 +2518,7 @@
       <c r="L31" s="11"/>
       <c r="M31" s="11"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -2534,7 +2555,7 @@
       <c r="L32" s="11"/>
       <c r="M32" s="11"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -2569,7 +2590,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -2604,7 +2625,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -2639,7 +2660,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -2670,7 +2691,7 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -2705,7 +2726,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -2740,7 +2761,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -2764,7 +2785,7 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -2799,7 +2820,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -2830,7 +2851,7 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -2863,7 +2884,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -2898,7 +2919,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -2933,7 +2954,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -2964,7 +2985,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -2994,7 +3015,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -3024,7 +3045,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>24</v>
       </c>
@@ -3056,7 +3077,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>24</v>
       </c>
@@ -3088,7 +3109,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>75</v>
       </c>
@@ -3110,7 +3131,7 @@
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -3134,7 +3155,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -3169,7 +3190,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>22</v>
       </c>
@@ -3204,7 +3225,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>22</v>
       </c>
@@ -3239,7 +3260,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>22</v>
       </c>
@@ -3274,7 +3295,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -3306,7 +3327,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>24</v>
       </c>
@@ -3336,7 +3357,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>24</v>
       </c>
@@ -3368,7 +3389,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -3400,7 +3421,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>22</v>
       </c>
@@ -3435,7 +3456,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>75</v>
       </c>
@@ -3458,7 +3479,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>75</v>
       </c>
@@ -3481,7 +3502,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -3504,7 +3525,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>75</v>
       </c>
@@ -3527,7 +3548,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>75</v>
       </c>
@@ -3562,7 +3583,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>75</v>
       </c>
@@ -3585,7 +3606,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>75</v>
       </c>
@@ -3608,7 +3629,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>22</v>
       </c>
@@ -3641,7 +3662,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>22</v>
       </c>
@@ -3676,7 +3697,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>22</v>
       </c>
@@ -3711,7 +3732,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>22</v>
       </c>
@@ -3746,394 +3767,456 @@
         <v>115</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E72" s="4"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E73" s="4"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>22</v>
+      </c>
+      <c r="B72" s="1">
+        <v>45583</v>
+      </c>
+      <c r="C72" t="s">
+        <v>249</v>
+      </c>
+      <c r="D72" s="1">
+        <v>45596</v>
+      </c>
+      <c r="E72" s="4">
+        <v>194.6</v>
+      </c>
+      <c r="F72" t="s">
+        <v>52</v>
+      </c>
+      <c r="G72" t="s">
+        <v>53</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K72" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>22</v>
+      </c>
+      <c r="B73" s="1">
+        <v>45590</v>
+      </c>
+      <c r="C73" t="s">
+        <v>252</v>
+      </c>
+      <c r="D73" s="1">
+        <v>45593</v>
+      </c>
+      <c r="E73" s="4">
+        <v>218.05</v>
+      </c>
+      <c r="F73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G73" t="s">
+        <v>254</v>
+      </c>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E74" s="4"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E75" s="4"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E76" s="4"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E77" s="4"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E78" s="4"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E79" s="4"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E80" s="4"/>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E81" s="4"/>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E82" s="4"/>
     </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E83" s="4"/>
     </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E84" s="4"/>
     </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E85" s="4"/>
     </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E86" s="4"/>
     </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E87" s="4"/>
     </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E88" s="4"/>
     </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E89" s="4"/>
     </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E90" s="4"/>
     </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E91" s="4"/>
     </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E92" s="4"/>
     </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E93" s="4"/>
     </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E94" s="4"/>
     </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E95" s="4"/>
     </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E96" s="4"/>
     </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E97" s="4"/>
     </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E98" s="4"/>
     </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E99" s="4"/>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E100" s="4"/>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E101" s="4"/>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E102" s="4"/>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E103" s="4"/>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E104" s="4"/>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E105" s="4"/>
     </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E106" s="4"/>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E107" s="4"/>
     </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E108" s="4"/>
     </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E109" s="4"/>
     </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E110" s="4"/>
     </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E111" s="4"/>
     </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E112" s="4"/>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E113" s="4"/>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E114" s="4"/>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E115" s="4"/>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E116" s="4"/>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E117" s="4"/>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E118" s="4"/>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E119" s="4"/>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E120" s="4"/>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E121" s="4"/>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E122" s="4"/>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E123" s="4"/>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E124" s="4"/>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E125" s="4"/>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E126" s="4"/>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E127" s="4"/>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E128" s="4"/>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E129" s="4"/>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E130" s="4"/>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E131" s="4"/>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E132" s="4"/>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E133" s="4"/>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E134" s="4"/>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E135" s="4"/>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E136" s="4"/>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E137" s="4"/>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E138" s="4"/>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E139" s="4"/>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E140" s="4"/>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E141" s="4"/>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E142" s="4"/>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E143" s="4"/>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E144" s="4"/>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E145" s="4"/>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E146" s="4"/>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E147" s="4"/>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E148" s="4"/>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E149" s="4"/>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E150" s="4"/>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E151" s="4"/>
     </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E152" s="4"/>
     </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E153" s="4"/>
     </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E154" s="4"/>
     </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E155" s="4"/>
     </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E156" s="4"/>
     </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E157" s="4"/>
     </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E158" s="4"/>
     </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E159" s="4"/>
     </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E160" s="4"/>
     </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E161" s="4"/>
     </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E162" s="4"/>
     </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E163" s="4"/>
     </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E164" s="4"/>
     </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E165" s="4"/>
     </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E166" s="4"/>
     </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E167" s="4"/>
     </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E168" s="4"/>
     </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E169" s="4"/>
     </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E170" s="4"/>
     </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E171" s="4"/>
     </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E172" s="4"/>
     </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E173" s="4"/>
     </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E174" s="4"/>
     </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E175" s="4"/>
     </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E176" s="4"/>
     </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E177" s="4"/>
     </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E178" s="4"/>
     </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E179" s="4"/>
     </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E180" s="4"/>
     </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E181" s="4"/>
     </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E182" s="4"/>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E183" s="4"/>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E184" s="4"/>
     </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E185" s="4"/>
     </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E186" s="4"/>
     </row>
-    <row r="187" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E187" s="4"/>
     </row>
-    <row r="188" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E188" s="4"/>
     </row>
-    <row r="189" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E189" s="4"/>
     </row>
-    <row r="190" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E190" s="4"/>
     </row>
-    <row r="191" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E191" s="4"/>
     </row>
-    <row r="192" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E192" s="4"/>
     </row>
-    <row r="193" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E193" s="4"/>
     </row>
-    <row r="194" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E194" s="4"/>
     </row>
-    <row r="195" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E195" s="4"/>
     </row>
-    <row r="196" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E196" s="4"/>
     </row>
-    <row r="197" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E197" s="4"/>
     </row>
-    <row r="198" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E198" s="4"/>
     </row>
-    <row r="199" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E199" s="4"/>
     </row>
-    <row r="200" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E200" s="4"/>
     </row>
-    <row r="201" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E201" s="4"/>
     </row>
   </sheetData>
@@ -4174,47 +4257,47 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
neue Filmvorführung Scent of fear 10.11.24
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BF1010-37B3-4934-AAA9-3E91FD67F3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09963854-9D87-4914-A97C-EF8E3BEE44F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="261">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -818,6 +818,9 @@
   </si>
   <si>
     <t>10053217</t>
+  </si>
+  <si>
+    <t>Verpflegung Podium DenkAnstoss</t>
   </si>
 </sst>
 </file>
@@ -980,8 +983,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K74" totalsRowShown="0">
-  <autoFilter ref="A1:K74" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K75" totalsRowShown="0">
+  <autoFilter ref="A1:K75" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K47">
     <sortCondition ref="A1:A47"/>
   </sortState>
@@ -1664,8 +1667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G55" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3900,7 +3903,28 @@
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E75" s="4"/>
+      <c r="A75" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75" s="1">
+        <v>45606</v>
+      </c>
+      <c r="C75" t="s">
+        <v>260</v>
+      </c>
+      <c r="D75" s="1">
+        <v>45606</v>
+      </c>
+      <c r="E75" s="4">
+        <v>100</v>
+      </c>
+      <c r="F75" t="s">
+        <v>162</v>
+      </c>
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
+      <c r="J75" s="2"/>
+      <c r="K75" s="2"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E76" s="4"/>

</xml_diff>

<commit_message>
Gewinn aus dem lezten Jahr aus den Einnahmen entfehrt
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0D9E10-1222-46BE-AB0C-E5C36172D8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292A36B6-F809-4CCF-BB27-9879223B4929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="283">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -431,9 +431,6 @@
   </si>
   <si>
     <t>240370TS</t>
-  </si>
-  <si>
-    <t>Gewinn 2023</t>
   </si>
   <si>
     <t>Atelierkino</t>
@@ -980,8 +977,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{27287C1A-B7AC-49C2-89D9-0074BB2DB80A}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -1025,10 +1022,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}" name="Table3" displayName="Table3" ref="A1:G18" totalsRowShown="0">
-  <autoFilter ref="A1:G18" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G13">
-    <sortCondition ref="A1:A13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}" name="Table3" displayName="Table3" ref="A1:G17" totalsRowShown="0">
+  <autoFilter ref="A1:G17" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">
+    <sortCondition ref="A1:A12"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{3D23B81F-00E6-4787-9893-D2AE611E1A32}" name="Kategorie"/>
@@ -1080,9 +1077,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1120,7 +1117,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1226,7 +1223,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1376,24 +1373,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.44140625" customWidth="1"/>
+    <col min="7" max="7" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1416,7 +1413,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1436,7 +1433,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -1453,7 +1450,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1470,12 +1467,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C5" s="5">
         <v>45368</v>
@@ -1484,15 +1481,15 @@
         <v>1000</v>
       </c>
       <c r="E5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C6" s="5">
         <v>45371</v>
@@ -1501,10 +1498,10 @@
         <v>1000</v>
       </c>
       <c r="E6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1521,52 +1518,58 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>131</v>
+      <c r="B8" t="s">
+        <v>165</v>
       </c>
       <c r="C8" s="5">
-        <v>45322</v>
+        <v>45439</v>
       </c>
       <c r="D8" s="4">
-        <v>4001.43</v>
+        <v>977.6</v>
       </c>
       <c r="E8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>166</v>
+        <v>107</v>
       </c>
       <c r="C9" s="5">
-        <v>45439</v>
+        <v>45390</v>
       </c>
       <c r="D9" s="4">
-        <v>977.6</v>
+        <v>16.29</v>
       </c>
       <c r="E9" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="F9" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10" s="5">
-        <v>45390</v>
+        <v>45357</v>
       </c>
       <c r="D10" s="4">
-        <v>16.29</v>
+        <v>65.25</v>
       </c>
       <c r="E10" t="s">
         <v>103</v>
@@ -1575,21 +1578,21 @@
         <v>104</v>
       </c>
       <c r="G10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="C11" s="5">
-        <v>45357</v>
+        <v>45418</v>
       </c>
       <c r="D11" s="4">
-        <v>65.25</v>
+        <v>25.77</v>
       </c>
       <c r="E11" t="s">
         <v>103</v>
@@ -1598,144 +1601,121 @@
         <v>104</v>
       </c>
       <c r="G11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="C12" s="5">
-        <v>45418</v>
+        <v>45443</v>
       </c>
       <c r="D12" s="4">
-        <v>25.77</v>
+        <v>1020</v>
       </c>
       <c r="E12" t="s">
-        <v>103</v>
+        <v>167</v>
       </c>
       <c r="F12" t="s">
-        <v>104</v>
-      </c>
-      <c r="G12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C13" s="5">
-        <v>45443</v>
+        <v>45448</v>
       </c>
       <c r="D13" s="4">
-        <v>1020</v>
+        <v>26.01</v>
       </c>
       <c r="E13" t="s">
-        <v>168</v>
+        <v>103</v>
       </c>
       <c r="F13" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="G13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>234</v>
+      </c>
+      <c r="C14" s="5">
+        <v>45592</v>
+      </c>
+      <c r="D14" s="4">
+        <v>600</v>
+      </c>
+      <c r="E14" t="s">
+        <v>236</v>
+      </c>
+      <c r="F14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
-        <v>172</v>
-      </c>
-      <c r="C14" s="5">
-        <v>45448</v>
-      </c>
-      <c r="D14" s="4">
-        <v>26.01</v>
-      </c>
-      <c r="E14" t="s">
-        <v>103</v>
-      </c>
-      <c r="F14" t="s">
-        <v>104</v>
-      </c>
-      <c r="G14" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
       <c r="B15" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="C15" s="5">
-        <v>45592</v>
+        <v>45603</v>
       </c>
       <c r="D15" s="4">
-        <v>600</v>
+        <v>14.7</v>
       </c>
       <c r="E15" t="s">
-        <v>237</v>
-      </c>
-      <c r="F15" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>250</v>
+        <v>18</v>
       </c>
       <c r="C16" s="5">
-        <v>45603</v>
+        <v>45612</v>
       </c>
       <c r="D16" s="4">
-        <v>14.7</v>
+        <v>15000</v>
       </c>
       <c r="E16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>263</v>
       </c>
       <c r="C17" s="5">
-        <v>45612</v>
+        <v>45580</v>
       </c>
       <c r="D17" s="4">
-        <v>15000</v>
+        <v>10000</v>
       </c>
       <c r="E17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" t="s">
         <v>264</v>
-      </c>
-      <c r="C18" s="5">
-        <v>45580</v>
-      </c>
-      <c r="D18" s="4">
-        <v>10000</v>
-      </c>
-      <c r="E18" t="s">
-        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -1750,7 +1730,7 @@
           <x14:formula1>
             <xm:f>dropdown!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A18</xm:sqref>
+          <xm:sqref>A2:A17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1762,26 +1742,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M220"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1816,7 +1796,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1843,7 +1823,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -1870,7 +1850,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1903,7 +1883,7 @@
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -1927,7 +1907,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -1951,7 +1931,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -1959,7 +1939,7 @@
         <v>45332</v>
       </c>
       <c r="C7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D7" s="1">
         <v>45332</v>
@@ -1968,11 +1948,11 @@
         <v>37.25</v>
       </c>
       <c r="F7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -1996,7 +1976,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>73</v>
       </c>
@@ -2004,7 +1984,7 @@
         <v>45576</v>
       </c>
       <c r="C9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D9" s="1">
         <v>45576</v>
@@ -2016,10 +1996,10 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -2027,7 +2007,7 @@
         <v>45576</v>
       </c>
       <c r="C10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D10" s="1">
         <v>45576</v>
@@ -2039,10 +2019,10 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -2050,7 +2030,7 @@
         <v>45576</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D11" s="1">
         <v>45576</v>
@@ -2062,10 +2042,10 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -2073,7 +2053,7 @@
         <v>45576</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D12" s="1">
         <v>45576</v>
@@ -2085,10 +2065,10 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -2096,7 +2076,7 @@
         <v>45576</v>
       </c>
       <c r="C13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D13" s="1">
         <v>45576</v>
@@ -2108,10 +2088,10 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -2119,7 +2099,7 @@
         <v>45578</v>
       </c>
       <c r="C14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D14" s="1">
         <v>45578</v>
@@ -2131,10 +2111,10 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -2142,7 +2122,7 @@
         <v>45576</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D15" s="1">
         <v>45579</v>
@@ -2151,16 +2131,16 @@
         <v>279.89999999999998</v>
       </c>
       <c r="F15" t="s">
+        <v>222</v>
+      </c>
+      <c r="G15" t="s">
         <v>223</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>226</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>111</v>
@@ -2169,7 +2149,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -2177,7 +2157,7 @@
         <v>45606</v>
       </c>
       <c r="C16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D16" s="1">
         <v>45606</v>
@@ -2186,14 +2166,14 @@
         <v>100</v>
       </c>
       <c r="F16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -2217,7 +2197,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2241,7 +2221,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2269,12 +2249,12 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D20" s="1">
         <v>45527</v>
@@ -2289,10 +2269,10 @@
         <v>30</v>
       </c>
       <c r="H20" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>111</v>
@@ -2301,12 +2281,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D21" s="1">
         <v>45322</v>
@@ -2324,12 +2304,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D22" s="1">
         <v>45316</v>
@@ -2349,12 +2329,12 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D23" s="1">
         <v>45347</v>
@@ -2374,12 +2354,12 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D24" s="1">
         <v>45376</v>
@@ -2399,12 +2379,12 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D25" s="1">
         <v>45407</v>
@@ -2424,12 +2404,12 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D26" s="1">
         <v>45437</v>
@@ -2449,12 +2429,12 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D27" s="1">
         <v>45468</v>
@@ -2473,12 +2453,12 @@
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D28" s="1">
         <v>45498</v>
@@ -2497,12 +2477,12 @@
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D29" s="1">
         <v>45529</v>
@@ -2524,12 +2504,12 @@
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>17</v>
       </c>
       <c r="C30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D30" s="1">
         <v>45560</v>
@@ -2551,12 +2531,12 @@
       <c r="L30" s="10"/>
       <c r="M30" s="10"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>17</v>
       </c>
       <c r="C31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D31" s="1">
         <v>45590</v>
@@ -2578,12 +2558,12 @@
       <c r="L31" s="10"/>
       <c r="M31" s="10"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>17</v>
       </c>
       <c r="C32" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D32" s="1">
         <v>45621</v>
@@ -2605,12 +2585,12 @@
       <c r="L32" s="10"/>
       <c r="M32" s="10"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D33" s="1">
         <v>45651</v>
@@ -2632,12 +2612,12 @@
       <c r="L33" s="10"/>
       <c r="M33" s="10"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>17</v>
       </c>
       <c r="C34" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D34" s="1">
         <v>45498</v>
@@ -2647,22 +2627,22 @@
         <v>1254</v>
       </c>
       <c r="F34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G34" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>17</v>
       </c>
       <c r="C35" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D35" s="1">
         <v>45529</v>
@@ -2672,22 +2652,22 @@
         <v>1254</v>
       </c>
       <c r="F35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G35" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>17</v>
       </c>
       <c r="C36" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D36" s="1">
         <v>45560</v>
@@ -2697,22 +2677,22 @@
         <v>1254</v>
       </c>
       <c r="F36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G36" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>17</v>
       </c>
       <c r="C37" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D37" s="1">
         <v>45590</v>
@@ -2722,22 +2702,22 @@
         <v>1254</v>
       </c>
       <c r="F37" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G37" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>17</v>
       </c>
       <c r="C38" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D38" s="1">
         <v>45621</v>
@@ -2747,22 +2727,22 @@
         <v>1254</v>
       </c>
       <c r="F38" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G38" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>17</v>
       </c>
       <c r="C39" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D39" s="1">
         <v>45651</v>
@@ -2772,17 +2752,17 @@
         <v>1254</v>
       </c>
       <c r="F39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G39" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>24</v>
       </c>
@@ -2808,12 +2788,12 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D41" s="1">
         <v>45316</v>
@@ -2832,7 +2812,7 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>24</v>
       </c>
@@ -2860,7 +2840,7 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -2888,12 +2868,12 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>24</v>
       </c>
       <c r="C44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D44" s="1">
         <v>45347</v>
@@ -2912,12 +2892,12 @@
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>24</v>
       </c>
       <c r="C45" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D45" s="1">
         <v>45352</v>
@@ -2932,10 +2912,10 @@
         <v>39</v>
       </c>
       <c r="H45" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="I45" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>90</v>
@@ -2944,12 +2924,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>24</v>
       </c>
       <c r="C46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D46" s="1">
         <v>45376</v>
@@ -2968,7 +2948,7 @@
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>24</v>
       </c>
@@ -3000,12 +2980,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>24</v>
       </c>
       <c r="C48" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D48" s="1">
         <v>45407</v>
@@ -3024,12 +3004,12 @@
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>24</v>
       </c>
       <c r="C49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D49" s="1">
         <v>45437</v>
@@ -3048,12 +3028,12 @@
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>24</v>
       </c>
       <c r="C50" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D50" s="1">
         <v>45468</v>
@@ -3072,12 +3052,12 @@
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>24</v>
       </c>
       <c r="C51" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D51" s="1">
         <v>45498</v>
@@ -3096,12 +3076,12 @@
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>24</v>
       </c>
       <c r="C52" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D52" s="1">
         <v>45529</v>
@@ -3120,12 +3100,12 @@
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>24</v>
       </c>
       <c r="C53" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D53" s="1">
         <v>45560</v>
@@ -3144,12 +3124,12 @@
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>24</v>
       </c>
       <c r="C54" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D54" s="1">
         <v>45590</v>
@@ -3168,12 +3148,12 @@
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>24</v>
       </c>
       <c r="C55" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D55" s="1">
         <v>45621</v>
@@ -3192,12 +3172,12 @@
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>24</v>
       </c>
       <c r="C56" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D56" s="1">
         <v>45651</v>
@@ -3216,12 +3196,12 @@
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>24</v>
       </c>
       <c r="C57" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D57" s="1">
         <v>45444</v>
@@ -3236,10 +3216,10 @@
         <v>39</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>90</v>
@@ -3248,12 +3228,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>24</v>
       </c>
       <c r="C58" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D58" s="1">
         <v>45505</v>
@@ -3262,30 +3242,30 @@
         <v>879.4</v>
       </c>
       <c r="F58" t="s">
+        <v>204</v>
+      </c>
+      <c r="G58" t="s">
         <v>205</v>
       </c>
-      <c r="G58" t="s">
+      <c r="H58" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="H58" s="2" t="s">
+      <c r="I58" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="I58" s="2" t="s">
-        <v>208</v>
-      </c>
       <c r="J58" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="K58" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="K58" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>24</v>
       </c>
       <c r="C59" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D59" s="1">
         <v>45562</v>
@@ -3294,30 +3274,30 @@
         <v>263.89999999999998</v>
       </c>
       <c r="F59" t="s">
+        <v>209</v>
+      </c>
+      <c r="G59" t="s">
         <v>210</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H59" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="I59" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="I59" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="J59" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="K59" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="K59" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>24</v>
       </c>
       <c r="C60" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D60" s="1">
         <v>45534</v>
@@ -3332,10 +3312,10 @@
         <v>39</v>
       </c>
       <c r="H60" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="I60" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="I60" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>90</v>
@@ -3344,7 +3324,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>22</v>
       </c>
@@ -3375,7 +3355,7 @@
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>22</v>
       </c>
@@ -3406,7 +3386,7 @@
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>22</v>
       </c>
@@ -3438,7 +3418,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="6"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>22</v>
       </c>
@@ -3469,7 +3449,7 @@
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>22</v>
       </c>
@@ -3500,7 +3480,7 @@
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>22</v>
       </c>
@@ -3524,7 +3504,7 @@
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>22</v>
       </c>
@@ -3559,7 +3539,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>22</v>
       </c>
@@ -3590,7 +3570,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>22</v>
       </c>
@@ -3625,7 +3605,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>22</v>
       </c>
@@ -3660,7 +3640,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>22</v>
       </c>
@@ -3695,7 +3675,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>22</v>
       </c>
@@ -3730,7 +3710,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>22</v>
       </c>
@@ -3763,7 +3743,7 @@
       </c>
       <c r="K73" s="2"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>22</v>
       </c>
@@ -3798,7 +3778,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>22</v>
       </c>
@@ -3806,7 +3786,7 @@
         <v>45400</v>
       </c>
       <c r="C75" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D75" s="1">
         <v>45400</v>
@@ -3822,7 +3802,7 @@
       </c>
       <c r="H75" s="2"/>
       <c r="I75" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J75" s="2" t="s">
         <v>90</v>
@@ -3831,7 +3811,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>22</v>
       </c>
@@ -3866,7 +3846,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>22</v>
       </c>
@@ -3874,7 +3854,7 @@
         <v>45319</v>
       </c>
       <c r="C77" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D77" s="1">
         <v>45421</v>
@@ -3883,10 +3863,10 @@
         <v>179.08</v>
       </c>
       <c r="F77" t="s">
+        <v>146</v>
+      </c>
+      <c r="G77" t="s">
         <v>147</v>
-      </c>
-      <c r="G77" t="s">
-        <v>148</v>
       </c>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
@@ -3897,7 +3877,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>22</v>
       </c>
@@ -3905,7 +3885,7 @@
         <v>45371</v>
       </c>
       <c r="C78" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D78" s="1">
         <v>45422</v>
@@ -3920,10 +3900,10 @@
         <v>76</v>
       </c>
       <c r="H78" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I78" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="I78" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="J78" s="2" t="s">
         <v>90</v>
@@ -3932,7 +3912,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>22</v>
       </c>
@@ -3940,7 +3920,7 @@
         <v>45415</v>
       </c>
       <c r="C79" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D79" s="1">
         <v>45426</v>
@@ -3955,10 +3935,10 @@
         <v>62</v>
       </c>
       <c r="H79" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I79" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="J79" s="2" t="s">
         <v>90</v>
@@ -3967,7 +3947,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>22</v>
       </c>
@@ -3975,7 +3955,7 @@
         <v>45431</v>
       </c>
       <c r="C80" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D80" s="1">
         <v>45435</v>
@@ -3984,14 +3964,14 @@
         <v>227.55</v>
       </c>
       <c r="F80" t="s">
+        <v>149</v>
+      </c>
+      <c r="G80" t="s">
         <v>150</v>
-      </c>
-      <c r="G80" t="s">
-        <v>151</v>
       </c>
       <c r="H80" s="2"/>
       <c r="I80" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J80" s="2" t="s">
         <v>90</v>
@@ -4000,7 +3980,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>22</v>
       </c>
@@ -4008,7 +3988,7 @@
         <v>45435</v>
       </c>
       <c r="C81" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D81" s="1">
         <v>45439</v>
@@ -4023,10 +4003,10 @@
         <v>34</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J81" s="2" t="s">
         <v>90</v>
@@ -4035,7 +4015,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>22</v>
       </c>
@@ -4043,7 +4023,7 @@
         <v>45412</v>
       </c>
       <c r="C82" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D82" s="1">
         <v>45460</v>
@@ -4052,16 +4032,16 @@
         <v>214</v>
       </c>
       <c r="F82" t="s">
+        <v>178</v>
+      </c>
+      <c r="G82" t="s">
+        <v>182</v>
+      </c>
+      <c r="H82" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="G82" t="s">
+      <c r="I82" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="H82" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="I82" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="J82" s="2" t="s">
         <v>90</v>
@@ -4070,7 +4050,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>22</v>
       </c>
@@ -4078,7 +4058,7 @@
         <v>45438</v>
       </c>
       <c r="C83" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D83" s="1">
         <v>45475</v>
@@ -4087,16 +4067,16 @@
         <v>174.6</v>
       </c>
       <c r="F83" t="s">
+        <v>185</v>
+      </c>
+      <c r="G83" t="s">
         <v>186</v>
       </c>
-      <c r="G83" t="s">
+      <c r="H83" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H83" s="2" t="s">
+      <c r="I83" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="I83" s="2" t="s">
-        <v>189</v>
       </c>
       <c r="J83" s="2" t="s">
         <v>90</v>
@@ -4105,7 +4085,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>22</v>
       </c>
@@ -4113,7 +4093,7 @@
         <v>45555</v>
       </c>
       <c r="C84" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D84" s="1">
         <v>45562</v>
@@ -4128,10 +4108,10 @@
         <v>62</v>
       </c>
       <c r="H84" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I84" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="I84" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="J84" s="2" t="s">
         <v>90</v>
@@ -4140,7 +4120,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>22</v>
       </c>
@@ -4148,7 +4128,7 @@
         <v>45557</v>
       </c>
       <c r="C85" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D85" s="1">
         <v>45566</v>
@@ -4157,16 +4137,16 @@
         <v>178.35</v>
       </c>
       <c r="F85" t="s">
+        <v>185</v>
+      </c>
+      <c r="G85" t="s">
         <v>186</v>
       </c>
-      <c r="G85" t="s">
-        <v>187</v>
-      </c>
       <c r="H85" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="I85" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="I85" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="J85" s="2" t="s">
         <v>90</v>
@@ -4175,7 +4155,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>22</v>
       </c>
@@ -4183,7 +4163,7 @@
         <v>45562</v>
       </c>
       <c r="C86" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D86" s="1">
         <v>45568</v>
@@ -4198,10 +4178,10 @@
         <v>62</v>
       </c>
       <c r="H86" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="I86" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="I86" s="2" t="s">
-        <v>216</v>
       </c>
       <c r="J86" s="2" t="s">
         <v>90</v>
@@ -4210,7 +4190,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>22</v>
       </c>
@@ -4218,7 +4198,7 @@
         <v>45581</v>
       </c>
       <c r="C87" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D87" s="1">
         <v>45583</v>
@@ -4233,17 +4213,17 @@
         <v>62</v>
       </c>
       <c r="H87" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="I87" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="I87" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="J87" s="2"/>
       <c r="K87" s="2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>22</v>
       </c>
@@ -4251,7 +4231,7 @@
         <v>45577</v>
       </c>
       <c r="C88" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D88" s="1">
         <v>45583</v>
@@ -4266,10 +4246,10 @@
         <v>76</v>
       </c>
       <c r="H88" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="I88" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="I88" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="J88" s="2" t="s">
         <v>90</v>
@@ -4278,7 +4258,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>22</v>
       </c>
@@ -4286,7 +4266,7 @@
         <v>45571</v>
       </c>
       <c r="C89" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D89" s="1">
         <v>45588</v>
@@ -4295,13 +4275,13 @@
         <v>181.6</v>
       </c>
       <c r="F89" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G89" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H89" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I89" s="2">
         <v>10053082</v>
@@ -4313,7 +4293,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>22</v>
       </c>
@@ -4321,7 +4301,7 @@
         <v>45578</v>
       </c>
       <c r="C90" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D90" s="1">
         <v>45589</v>
@@ -4336,10 +4316,10 @@
         <v>34</v>
       </c>
       <c r="H90" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="I90" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="J90" s="2" t="s">
         <v>90</v>
@@ -4348,7 +4328,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>22</v>
       </c>
@@ -4356,7 +4336,7 @@
         <v>45590</v>
       </c>
       <c r="C91" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D91" s="1">
         <v>45593</v>
@@ -4365,14 +4345,14 @@
         <v>218.05</v>
       </c>
       <c r="F91" t="s">
+        <v>246</v>
+      </c>
+      <c r="G91" t="s">
         <v>247</v>
-      </c>
-      <c r="G91" t="s">
-        <v>248</v>
       </c>
       <c r="H91" s="2"/>
       <c r="I91" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J91" s="2" t="s">
         <v>90</v>
@@ -4381,7 +4361,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>22</v>
       </c>
@@ -4389,7 +4369,7 @@
         <v>45583</v>
       </c>
       <c r="C92" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D92" s="1">
         <v>45596</v>
@@ -4404,10 +4384,10 @@
         <v>53</v>
       </c>
       <c r="H92" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="I92" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="I92" s="2" t="s">
-        <v>245</v>
       </c>
       <c r="J92" s="2" t="s">
         <v>90</v>
@@ -4416,7 +4396,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>22</v>
       </c>
@@ -4424,7 +4404,7 @@
         <v>45585</v>
       </c>
       <c r="C93" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D93" s="1">
         <v>45603</v>
@@ -4433,16 +4413,16 @@
         <v>181.6</v>
       </c>
       <c r="F93" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G93" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H93" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="I93" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="I93" s="2" t="s">
-        <v>253</v>
       </c>
       <c r="J93" s="2" t="s">
         <v>90</v>
@@ -4451,12 +4431,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>14</v>
       </c>
       <c r="C94" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D94" s="1">
         <v>45435</v>
@@ -4465,28 +4445,28 @@
         <v>479.5</v>
       </c>
       <c r="F94" t="s">
+        <v>156</v>
+      </c>
+      <c r="G94" t="s">
         <v>157</v>
-      </c>
-      <c r="G94" t="s">
-        <v>158</v>
       </c>
       <c r="H94" s="2"/>
       <c r="I94" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J94" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="K94" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K94" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>14</v>
       </c>
       <c r="C95" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D95" s="1">
         <v>45435</v>
@@ -4495,395 +4475,395 @@
         <v>420</v>
       </c>
       <c r="F95" t="s">
+        <v>156</v>
+      </c>
+      <c r="G95" t="s">
         <v>157</v>
-      </c>
-      <c r="G95" t="s">
-        <v>158</v>
       </c>
       <c r="H95" s="2"/>
       <c r="I95" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J95" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="J95" s="6" t="s">
+      <c r="K95" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K95" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E96" s="4"/>
     </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E97" s="4"/>
     </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E98" s="4"/>
     </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E99" s="4"/>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E100" s="4"/>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E101" s="4"/>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E102" s="4"/>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E103" s="4"/>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E104" s="4"/>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E105" s="4"/>
     </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E106" s="4"/>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E107" s="4"/>
     </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E108" s="4"/>
     </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E109" s="4"/>
     </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E110" s="4"/>
     </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E111" s="4"/>
     </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E112" s="4"/>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E113" s="4"/>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E114" s="4"/>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E115" s="4"/>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E116" s="4"/>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E117" s="4"/>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E118" s="4"/>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E119" s="4"/>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E120" s="4"/>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E121" s="4"/>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E122" s="4"/>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E123" s="4"/>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E124" s="4"/>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E125" s="4"/>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E126" s="4"/>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E127" s="4"/>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E128" s="4"/>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E129" s="4"/>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E130" s="4"/>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E131" s="4"/>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E132" s="4"/>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E133" s="4"/>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E134" s="4"/>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E135" s="4"/>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E136" s="4"/>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E137" s="4"/>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E138" s="4"/>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E139" s="4"/>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E140" s="4"/>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E141" s="4"/>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E142" s="4"/>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E143" s="4"/>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E144" s="4"/>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E145" s="4"/>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E146" s="4"/>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E147" s="4"/>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E148" s="4"/>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E149" s="4"/>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E150" s="4"/>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E151" s="4"/>
     </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E152" s="4"/>
     </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E153" s="4"/>
     </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E154" s="4"/>
     </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E155" s="4"/>
     </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E156" s="4"/>
     </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E157" s="4"/>
     </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E158" s="4"/>
     </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E159" s="4"/>
     </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E160" s="4"/>
     </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E161" s="4"/>
     </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E162" s="4"/>
     </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E163" s="4"/>
     </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E164" s="4"/>
     </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E165" s="4"/>
     </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E166" s="4"/>
     </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E167" s="4"/>
     </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E168" s="4"/>
     </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E169" s="4"/>
     </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E170" s="4"/>
     </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E171" s="4"/>
     </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E172" s="4"/>
     </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E173" s="4"/>
     </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E174" s="4"/>
     </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E175" s="4"/>
     </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E176" s="4"/>
     </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E177" s="4"/>
     </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E178" s="4"/>
     </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E179" s="4"/>
     </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E180" s="4"/>
     </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E181" s="4"/>
     </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E182" s="4"/>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E183" s="4"/>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E184" s="4"/>
     </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E185" s="4"/>
     </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E186" s="4"/>
     </row>
-    <row r="187" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E187" s="4"/>
     </row>
-    <row r="188" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="188" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E188" s="4"/>
     </row>
-    <row r="189" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="189" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E189" s="4"/>
     </row>
-    <row r="190" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="190" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E190" s="4"/>
     </row>
-    <row r="191" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="191" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E191" s="4"/>
     </row>
-    <row r="192" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E192" s="4"/>
     </row>
-    <row r="193" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E193" s="4"/>
     </row>
-    <row r="194" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E194" s="4"/>
     </row>
-    <row r="195" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E195" s="4"/>
     </row>
-    <row r="196" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E196" s="4"/>
     </row>
-    <row r="197" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E197" s="4"/>
     </row>
-    <row r="198" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E198" s="4"/>
     </row>
-    <row r="199" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E199" s="4"/>
     </row>
-    <row r="200" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E200" s="4"/>
     </row>
-    <row r="201" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E201" s="4"/>
     </row>
-    <row r="202" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E202" s="4"/>
     </row>
-    <row r="203" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="203" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E203" s="4"/>
     </row>
-    <row r="204" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E204" s="4"/>
     </row>
-    <row r="205" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="205" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E205" s="4"/>
     </row>
-    <row r="206" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E206" s="4"/>
     </row>
-    <row r="207" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E207" s="4"/>
     </row>
-    <row r="208" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E208" s="4"/>
     </row>
-    <row r="209" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="209" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E209" s="4"/>
     </row>
-    <row r="210" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="210" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E210" s="4"/>
     </row>
-    <row r="211" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="211" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E211" s="4"/>
     </row>
-    <row r="212" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="212" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E212" s="4"/>
     </row>
-    <row r="213" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="213" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E213" s="4"/>
     </row>
-    <row r="214" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="214" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E214" s="4"/>
     </row>
-    <row r="215" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="215" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E215" s="4"/>
     </row>
-    <row r="216" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="216" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E216" s="4"/>
     </row>
-    <row r="217" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="217" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E217" s="4"/>
     </row>
-    <row r="218" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="218" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E218" s="4"/>
     </row>
-    <row r="219" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="219" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E219" s="4"/>
     </row>
-    <row r="220" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="220" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E220" s="4"/>
     </row>
   </sheetData>
@@ -4924,47 +4904,47 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Neue Rechnung - scent of fear 14.11.24
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292A36B6-F809-4CCF-BB27-9879223B4929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E6D84D-072C-4B78-AFA6-B2FBBEC2FBBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="286">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -887,6 +887,15 @@
   </si>
   <si>
     <t xml:space="preserve">Gehaltszahlung Betriebsleitung Januar 24 </t>
+  </si>
+  <si>
+    <t>Film: Scent of Fear</t>
+  </si>
+  <si>
+    <t>00 00000 00000 00000 00004 24145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00042414 </t>
   </si>
 </sst>
 </file>
@@ -918,15 +927,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -958,12 +973,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -975,10 +1021,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{27287C1A-B7AC-49C2-89D9-0074BB2DB80A}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -1041,10 +1098,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K95" totalsRowShown="0">
-  <autoFilter ref="A1:K95" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K95">
-    <sortCondition ref="A1:A95"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K96" totalsRowShown="0">
+  <autoFilter ref="A1:K96" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K96">
+    <sortCondition ref="D1:D96"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="9" xr3:uid="{7720D0EA-5763-4F4F-82DA-8D34884933A7}" name="Kategorie"/>
@@ -1077,9 +1134,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1117,7 +1174,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1223,7 +1280,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1375,22 +1432,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.42578125" customWidth="1"/>
+    <col min="7" max="7" width="42.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1413,7 +1470,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1433,7 +1490,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -1450,7 +1507,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1467,7 +1524,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -1484,7 +1541,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -1501,7 +1558,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1518,7 +1575,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1535,7 +1592,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1558,7 +1615,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1581,7 +1638,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1604,7 +1661,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1624,7 +1681,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1647,7 +1704,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1667,7 +1724,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1684,7 +1741,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1701,7 +1758,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1742,26 +1799,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M220"/>
   <sheetViews>
-    <sheetView zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96:K96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1796,432 +1853,468 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1">
-        <v>45311</v>
+        <v>45332</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="D2" s="1">
-        <v>45311</v>
+        <v>37308</v>
       </c>
       <c r="E2" s="4">
-        <v>75.849999999999994</v>
+        <v>417.7</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="1">
-        <v>45311</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1">
-        <v>45311</v>
+        <v>44895</v>
       </c>
       <c r="E3" s="4">
-        <v>60</v>
+        <v>15.75</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="I3" s="2">
+        <v>42491</v>
+      </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>73</v>
       </c>
       <c r="B4" s="1">
-        <v>45312</v>
+        <v>45311</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1">
-        <v>45312</v>
+        <v>45311</v>
       </c>
       <c r="E4" s="4">
-        <v>52.45</v>
+        <v>75.849999999999994</v>
       </c>
       <c r="F4" t="s">
-        <v>109</v>
+        <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>110</v>
+        <v>8</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>112</v>
-      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="5">
-        <v>45319</v>
+      <c r="B5" s="1">
+        <v>45311</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="5">
-        <v>45319</v>
+        <v>72</v>
+      </c>
+      <c r="D5" s="1">
+        <v>45311</v>
       </c>
       <c r="E5" s="4">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>56</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>73</v>
       </c>
       <c r="B6" s="1">
-        <v>45340</v>
+        <v>45312</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1">
-        <v>45323</v>
+        <v>45312</v>
       </c>
       <c r="E6" s="4">
-        <v>400</v>
+        <v>52.45</v>
       </c>
       <c r="F6" t="s">
-        <v>68</v>
+        <v>109</v>
+      </c>
+      <c r="G6" t="s">
+        <v>110</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J6" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="1">
-        <v>45332</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>177</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1">
-        <v>45332</v>
+        <v>45316</v>
       </c>
       <c r="E7" s="4">
-        <v>37.25</v>
+        <v>34.5</v>
       </c>
       <c r="F7" t="s">
-        <v>177</v>
-      </c>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" s="1">
-        <v>45354</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1">
-        <v>45354</v>
+        <v>45316</v>
       </c>
       <c r="E8" s="4">
-        <v>10</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="F8" t="s">
-        <v>79</v>
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" s="1">
-        <v>45576</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>216</v>
+        <v>282</v>
       </c>
       <c r="D9" s="1">
-        <v>45576</v>
+        <v>45316</v>
       </c>
       <c r="E9" s="4">
-        <v>37.700000000000003</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="1">
-        <v>45576</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>217</v>
+        <v>132</v>
       </c>
       <c r="D10" s="1">
-        <v>45576</v>
+        <v>45316</v>
       </c>
       <c r="E10" s="4">
-        <v>116.1</v>
+        <v>1200</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>56</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="1">
-        <v>45576</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="D11" s="1">
-        <v>45576</v>
+      <c r="B11" s="5">
+        <v>45319</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="5">
+        <v>45319</v>
       </c>
       <c r="E11" s="4">
-        <v>154.80000000000001</v>
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>27</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1">
-        <v>45576</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>218</v>
+        <v>45316</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
       </c>
       <c r="D12" s="1">
-        <v>45576</v>
+        <v>45321</v>
       </c>
       <c r="E12" s="4">
-        <v>102.2</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+        <v>194.6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="J12" s="2"/>
-      <c r="K12" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="1">
-        <v>45576</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>254</v>
+        <v>180</v>
       </c>
       <c r="D13" s="1">
-        <v>45576</v>
+        <v>45322</v>
       </c>
       <c r="E13" s="4">
-        <v>30.7</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+        <v>276</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>111</v>
+      </c>
       <c r="K13" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>73</v>
       </c>
       <c r="B14" s="1">
-        <v>45578</v>
+        <v>45340</v>
       </c>
       <c r="C14" t="s">
-        <v>220</v>
+        <v>67</v>
       </c>
       <c r="D14" s="1">
-        <v>45578</v>
+        <v>45323</v>
       </c>
       <c r="E14" s="4">
-        <v>50.25</v>
+        <v>400</v>
+      </c>
+      <c r="F14" t="s">
+        <v>68</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="1">
-        <v>45576</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>221</v>
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
       </c>
       <c r="D15" s="1">
-        <v>45579</v>
+        <v>45329</v>
       </c>
       <c r="E15" s="4">
-        <v>279.89999999999998</v>
+        <v>35.049999999999997</v>
       </c>
       <c r="F15" t="s">
-        <v>222</v>
+        <v>38</v>
       </c>
       <c r="G15" t="s">
-        <v>223</v>
+        <v>39</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>224</v>
+        <v>47</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1">
-        <v>45606</v>
+        <v>45312</v>
       </c>
       <c r="C16" t="s">
-        <v>253</v>
+        <v>58</v>
       </c>
       <c r="D16" s="1">
-        <v>45606</v>
+        <v>45329</v>
       </c>
       <c r="E16" s="4">
-        <v>100</v>
+        <v>276.3</v>
       </c>
       <c r="F16" t="s">
-        <v>156</v>
-      </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="G16" t="s">
+        <v>43</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D17" s="1">
-        <v>45316</v>
+        <v>45330</v>
       </c>
       <c r="E17" s="4">
-        <v>34.5</v>
+        <v>100</v>
       </c>
       <c r="F17" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="G17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45311</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="D18" s="1">
-        <v>45316</v>
+        <v>45330</v>
       </c>
       <c r="E18" s="4">
-        <v>32.700000000000003</v>
+        <v>423.5</v>
       </c>
       <c r="F18" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="G18" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2249,87 +2342,83 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>73</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45332</v>
       </c>
       <c r="C20" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="D20" s="1">
-        <v>45527</v>
+        <v>45332</v>
       </c>
       <c r="E20" s="4">
-        <v>159</v>
+        <v>37.25</v>
       </c>
       <c r="F20" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45333</v>
       </c>
       <c r="C21" t="s">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="D21" s="1">
-        <v>45322</v>
+        <v>45337</v>
       </c>
       <c r="E21" s="4">
-        <v>276</v>
+        <v>192.45</v>
       </c>
       <c r="F21" t="s">
-        <v>9</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="G21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H21" t="s">
+        <v>63</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45340</v>
       </c>
       <c r="C22" t="s">
-        <v>282</v>
+        <v>65</v>
       </c>
       <c r="D22" s="1">
-        <v>45316</v>
+        <v>45341</v>
       </c>
       <c r="E22" s="4">
-        <f t="shared" ref="E22:E39" si="0">1140*1.1</f>
-        <v>1254</v>
+        <v>1000</v>
       </c>
       <c r="F22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -2340,7 +2429,7 @@
         <v>45347</v>
       </c>
       <c r="E23" s="4">
-        <f t="shared" si="0"/>
+        <f>1140*1.1</f>
         <v>1254</v>
       </c>
       <c r="F23" t="s">
@@ -2354,97 +2443,105 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>280</v>
+        <v>133</v>
       </c>
       <c r="D24" s="1">
-        <v>45376</v>
+        <v>45347</v>
       </c>
       <c r="E24" s="4">
-        <f t="shared" si="0"/>
-        <v>1254</v>
+        <v>1200</v>
       </c>
       <c r="F24" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G24" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>265</v>
+        <v>173</v>
       </c>
       <c r="D25" s="1">
-        <v>45407</v>
+        <v>45352</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" si="0"/>
-        <v>1254</v>
+        <v>51.45</v>
       </c>
       <c r="F25" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="G25" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>73</v>
+      </c>
+      <c r="B26" s="1">
+        <v>45354</v>
       </c>
       <c r="C26" t="s">
-        <v>266</v>
+        <v>26</v>
       </c>
       <c r="D26" s="1">
-        <v>45437</v>
+        <v>45354</v>
       </c>
       <c r="E26" s="4">
-        <f t="shared" si="0"/>
-        <v>1254</v>
+        <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>267</v>
+        <v>280</v>
       </c>
       <c r="D27" s="1">
-        <v>45468</v>
+        <v>45376</v>
       </c>
       <c r="E27" s="4">
-        <f t="shared" si="0"/>
+        <f>1140*1.1</f>
         <v>1254</v>
       </c>
       <c r="F27" t="s">
         <v>7</v>
+      </c>
+      <c r="G27" t="s">
+        <v>8</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -2453,22 +2550,24 @@
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>268</v>
+        <v>134</v>
       </c>
       <c r="D28" s="1">
-        <v>45498</v>
+        <v>45376</v>
       </c>
       <c r="E28" s="4">
-        <f t="shared" si="0"/>
-        <v>1254</v>
+        <v>1200</v>
       </c>
       <c r="F28" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="G28" t="s">
+        <v>56</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -2477,326 +2576,424 @@
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>269</v>
+        <v>81</v>
       </c>
       <c r="D29" s="1">
-        <v>45529</v>
+        <v>45376</v>
       </c>
       <c r="E29" s="4">
-        <f t="shared" si="0"/>
-        <v>1254</v>
+        <v>25.1</v>
       </c>
       <c r="F29" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="G29" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="B30" s="1">
+        <v>45344</v>
       </c>
       <c r="C30" t="s">
-        <v>270</v>
+        <v>84</v>
       </c>
       <c r="D30" s="1">
-        <v>45560</v>
+        <v>45387</v>
       </c>
       <c r="E30" s="4">
-        <f t="shared" si="0"/>
-        <v>1254</v>
+        <v>205.4</v>
       </c>
       <c r="F30" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="G30" t="s">
-        <v>8</v>
-      </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="L30" s="10"/>
       <c r="M30" s="10"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="B31" s="1">
+        <v>45418</v>
       </c>
       <c r="C31" t="s">
-        <v>271</v>
+        <v>126</v>
       </c>
       <c r="D31" s="1">
-        <v>45590</v>
+        <v>45387</v>
       </c>
       <c r="E31" s="4">
-        <f t="shared" si="0"/>
-        <v>1254</v>
+        <v>170</v>
       </c>
       <c r="F31" t="s">
-        <v>7</v>
+        <v>127</v>
       </c>
       <c r="G31" t="s">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
+      <c r="J31" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="L31" s="10"/>
       <c r="M31" s="10"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="B32" s="1">
+        <v>45386</v>
       </c>
       <c r="C32" t="s">
-        <v>272</v>
+        <v>94</v>
       </c>
       <c r="D32" s="1">
-        <v>45621</v>
+        <v>45387</v>
       </c>
       <c r="E32" s="4">
-        <f t="shared" si="0"/>
-        <v>1254</v>
+        <v>139.75</v>
       </c>
       <c r="F32" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="G32" t="s">
-        <v>8</v>
-      </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="L32" s="10"/>
       <c r="M32" s="10"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="B33" s="1">
+        <v>45358</v>
       </c>
       <c r="C33" t="s">
-        <v>273</v>
+        <v>100</v>
       </c>
       <c r="D33" s="1">
-        <v>45651</v>
+        <v>45387</v>
       </c>
       <c r="E33" s="4">
-        <f t="shared" si="0"/>
-        <v>1254</v>
+        <v>104</v>
       </c>
       <c r="F33" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="G33" t="s">
-        <v>8</v>
-      </c>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="L33" s="10"/>
       <c r="M33" s="10"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="1">
+        <v>45368</v>
+      </c>
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="1">
+        <v>45387</v>
+      </c>
+      <c r="E34" s="4">
+        <v>178.35</v>
+      </c>
+      <c r="F34" t="s">
+        <v>61</v>
+      </c>
+      <c r="G34" t="s">
+        <v>62</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J34" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="K34" s="20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="1">
+        <v>45354</v>
+      </c>
+      <c r="C35" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="1">
+        <v>45387</v>
+      </c>
+      <c r="E35" s="4">
+        <v>137.9</v>
+      </c>
+      <c r="F35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G35" t="s">
+        <v>62</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="1">
+        <v>45339</v>
+      </c>
+      <c r="C36" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" s="1">
+        <v>45392</v>
+      </c>
+      <c r="E36" s="4">
+        <v>461.95</v>
+      </c>
+      <c r="F36" t="s">
+        <v>75</v>
+      </c>
+      <c r="G36" t="s">
+        <v>76</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="1">
+        <v>45383</v>
+      </c>
+      <c r="C37" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37" s="1">
+        <v>45394</v>
+      </c>
+      <c r="E37" s="4">
+        <v>211.9</v>
+      </c>
+      <c r="F37" t="s">
+        <v>61</v>
+      </c>
+      <c r="G37" t="s">
+        <v>62</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="1">
+        <v>45400</v>
+      </c>
+      <c r="C38" t="s">
+        <v>143</v>
+      </c>
+      <c r="D38" s="1">
+        <v>45400</v>
+      </c>
+      <c r="E38" s="4">
+        <v>211.85</v>
+      </c>
+      <c r="F38" t="s">
+        <v>50</v>
+      </c>
+      <c r="G38" t="s">
+        <v>51</v>
+      </c>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="1">
+        <v>45403</v>
+      </c>
+      <c r="C39" t="s">
+        <v>121</v>
+      </c>
+      <c r="D39" s="1">
+        <v>45403</v>
+      </c>
+      <c r="E39" s="4">
+        <v>447.55</v>
+      </c>
+      <c r="F39" t="s">
+        <v>123</v>
+      </c>
+      <c r="G39" t="s">
+        <v>124</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J39" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="K39" s="20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>17</v>
       </c>
-      <c r="C34" t="s">
-        <v>274</v>
-      </c>
-      <c r="D34" s="1">
-        <v>45498</v>
-      </c>
-      <c r="E34" s="4">
-        <f t="shared" si="0"/>
+      <c r="C40" t="s">
+        <v>265</v>
+      </c>
+      <c r="D40" s="1">
+        <v>45407</v>
+      </c>
+      <c r="E40" s="4">
+        <f>1140*1.1</f>
         <v>1254</v>
       </c>
-      <c r="F34" t="s">
-        <v>156</v>
-      </c>
-      <c r="G34" t="s">
-        <v>255</v>
-      </c>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" t="s">
-        <v>275</v>
-      </c>
-      <c r="D35" s="1">
-        <v>45529</v>
-      </c>
-      <c r="E35" s="4">
-        <f t="shared" si="0"/>
-        <v>1254</v>
-      </c>
-      <c r="F35" t="s">
-        <v>156</v>
-      </c>
-      <c r="G35" t="s">
-        <v>255</v>
-      </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36" t="s">
-        <v>276</v>
-      </c>
-      <c r="D36" s="1">
-        <v>45560</v>
-      </c>
-      <c r="E36" s="4">
-        <f t="shared" si="0"/>
-        <v>1254</v>
-      </c>
-      <c r="F36" t="s">
-        <v>156</v>
-      </c>
-      <c r="G36" t="s">
-        <v>255</v>
-      </c>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>17</v>
-      </c>
-      <c r="C37" t="s">
-        <v>277</v>
-      </c>
-      <c r="D37" s="1">
-        <v>45590</v>
-      </c>
-      <c r="E37" s="4">
-        <f t="shared" si="0"/>
-        <v>1254</v>
-      </c>
-      <c r="F37" t="s">
-        <v>156</v>
-      </c>
-      <c r="G37" t="s">
-        <v>255</v>
-      </c>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>17</v>
-      </c>
-      <c r="C38" t="s">
-        <v>278</v>
-      </c>
-      <c r="D38" s="1">
-        <v>45621</v>
-      </c>
-      <c r="E38" s="4">
-        <f t="shared" si="0"/>
-        <v>1254</v>
-      </c>
-      <c r="F38" t="s">
-        <v>156</v>
-      </c>
-      <c r="G38" t="s">
-        <v>255</v>
-      </c>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>17</v>
-      </c>
-      <c r="C39" t="s">
-        <v>279</v>
-      </c>
-      <c r="D39" s="1">
-        <v>45651</v>
-      </c>
-      <c r="E39" s="4">
-        <f t="shared" si="0"/>
-        <v>1254</v>
-      </c>
-      <c r="F39" t="s">
-        <v>156</v>
-      </c>
-      <c r="G39" t="s">
-        <v>255</v>
-      </c>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>24</v>
-      </c>
-      <c r="C40" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40" s="1">
-        <v>44895</v>
-      </c>
-      <c r="E40" s="4">
-        <v>15.75</v>
-      </c>
       <c r="F40" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G40" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="H40" s="2"/>
-      <c r="I40" s="2">
-        <v>42491</v>
-      </c>
+      <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D41" s="1">
-        <v>45316</v>
+        <v>45407</v>
       </c>
       <c r="E41" s="4">
         <v>1200</v>
@@ -2812,110 +3009,132 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B42" s="1">
+        <v>45319</v>
       </c>
       <c r="C42" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
       <c r="D42" s="1">
-        <v>45329</v>
+        <v>45421</v>
       </c>
       <c r="E42" s="4">
-        <v>35.049999999999997</v>
+        <v>179.08</v>
       </c>
       <c r="F42" t="s">
-        <v>38</v>
+        <v>146</v>
       </c>
       <c r="G42" t="s">
-        <v>39</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B43" s="1">
+        <v>45371</v>
       </c>
       <c r="C43" t="s">
-        <v>37</v>
+        <v>140</v>
       </c>
       <c r="D43" s="1">
-        <v>45330</v>
+        <v>45422</v>
       </c>
       <c r="E43" s="4">
-        <v>100</v>
+        <v>162.15</v>
       </c>
       <c r="F43" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="G43" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B44" s="1">
+        <v>45415</v>
       </c>
       <c r="C44" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D44" s="1">
-        <v>45347</v>
+        <v>45426</v>
       </c>
       <c r="E44" s="4">
-        <v>1200</v>
+        <v>137.9</v>
       </c>
       <c r="F44" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="G44" t="s">
-        <v>56</v>
-      </c>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B45" s="1">
+        <v>45431</v>
       </c>
       <c r="C45" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="D45" s="1">
-        <v>45352</v>
+        <v>45435</v>
       </c>
       <c r="E45" s="4">
-        <v>51.45</v>
+        <v>227.55</v>
       </c>
       <c r="F45" t="s">
-        <v>38</v>
+        <v>149</v>
       </c>
       <c r="G45" t="s">
-        <v>39</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>169</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="H45" s="2"/>
       <c r="I45" s="2" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>90</v>
@@ -2924,87 +3143,92 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C46" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="D46" s="1">
-        <v>45376</v>
+        <v>45435</v>
       </c>
       <c r="E46" s="4">
-        <v>1200</v>
+        <v>479.5</v>
       </c>
       <c r="F46" t="s">
-        <v>11</v>
+        <v>156</v>
       </c>
       <c r="G46" t="s">
-        <v>56</v>
+        <v>157</v>
       </c>
       <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I46" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C47" t="s">
-        <v>81</v>
+        <v>158</v>
       </c>
       <c r="D47" s="1">
-        <v>45376</v>
+        <v>45435</v>
       </c>
       <c r="E47" s="4">
-        <v>25.1</v>
+        <v>420</v>
       </c>
       <c r="F47" t="s">
-        <v>38</v>
+        <v>156</v>
       </c>
       <c r="G47" t="s">
-        <v>39</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>82</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="H47" s="2"/>
       <c r="I47" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>90</v>
+        <v>160</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>161</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C48" t="s">
-        <v>135</v>
+        <v>266</v>
       </c>
       <c r="D48" s="1">
-        <v>45407</v>
+        <v>45437</v>
       </c>
       <c r="E48" s="4">
-        <v>1200</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F48" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G48" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>24</v>
       </c>
@@ -3028,111 +3252,139 @@
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B50" s="1">
+        <v>45435</v>
       </c>
       <c r="C50" t="s">
-        <v>256</v>
+        <v>152</v>
       </c>
       <c r="D50" s="1">
-        <v>45468</v>
+        <v>45439</v>
       </c>
       <c r="E50" s="4">
-        <v>1200</v>
+        <v>253.55</v>
       </c>
       <c r="F50" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="G50" t="s">
-        <v>56</v>
-      </c>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>24</v>
       </c>
       <c r="C51" t="s">
-        <v>257</v>
+        <v>174</v>
       </c>
       <c r="D51" s="1">
-        <v>45498</v>
+        <v>45444</v>
       </c>
       <c r="E51" s="4">
-        <v>1200</v>
+        <v>80.150000000000006</v>
       </c>
       <c r="F51" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="G51" t="s">
-        <v>56</v>
-      </c>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B52" s="1">
+        <v>45412</v>
       </c>
       <c r="C52" t="s">
-        <v>258</v>
+        <v>181</v>
       </c>
       <c r="D52" s="1">
-        <v>45529</v>
+        <v>45460</v>
       </c>
       <c r="E52" s="4">
-        <v>1200</v>
+        <v>214</v>
       </c>
       <c r="F52" t="s">
-        <v>11</v>
+        <v>178</v>
       </c>
       <c r="G52" t="s">
-        <v>56</v>
-      </c>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C53" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="D53" s="1">
-        <v>45560</v>
+        <v>45468</v>
       </c>
       <c r="E53" s="4">
-        <v>1200</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F53" t="s">
-        <v>11</v>
-      </c>
-      <c r="G53" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>24</v>
       </c>
       <c r="C54" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D54" s="1">
-        <v>45590</v>
+        <v>45468</v>
       </c>
       <c r="E54" s="4">
         <v>1200</v>
@@ -3148,142 +3400,136 @@
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B55" s="1">
+        <v>45438</v>
       </c>
       <c r="C55" t="s">
-        <v>261</v>
+        <v>184</v>
       </c>
       <c r="D55" s="1">
-        <v>45621</v>
+        <v>45475</v>
       </c>
       <c r="E55" s="4">
-        <v>1200</v>
+        <v>174.6</v>
       </c>
       <c r="F55" t="s">
-        <v>11</v>
+        <v>185</v>
       </c>
       <c r="G55" t="s">
-        <v>56</v>
-      </c>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C56" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="D56" s="1">
-        <v>45651</v>
+        <v>45498</v>
       </c>
       <c r="E56" s="4">
-        <v>1200</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F56" t="s">
-        <v>11</v>
-      </c>
-      <c r="G56" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C57" t="s">
-        <v>174</v>
+        <v>274</v>
       </c>
       <c r="D57" s="1">
-        <v>45444</v>
+        <v>45498</v>
       </c>
       <c r="E57" s="4">
-        <v>80.150000000000006</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F57" t="s">
-        <v>38</v>
+        <v>156</v>
       </c>
       <c r="G57" t="s">
-        <v>39</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="J57" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K57" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>24</v>
       </c>
       <c r="C58" t="s">
-        <v>203</v>
+        <v>257</v>
       </c>
       <c r="D58" s="1">
-        <v>45505</v>
+        <v>45498</v>
       </c>
       <c r="E58" s="4">
-        <v>879.4</v>
+        <v>1200</v>
       </c>
       <c r="F58" t="s">
-        <v>204</v>
+        <v>11</v>
       </c>
       <c r="G58" t="s">
-        <v>205</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="K58" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>24</v>
       </c>
       <c r="C59" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D59" s="1">
-        <v>45562</v>
+        <v>45505</v>
       </c>
       <c r="E59" s="4">
-        <v>263.89999999999998</v>
+        <v>879.4</v>
       </c>
       <c r="F59" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="G59" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>201</v>
@@ -3292,299 +3538,266 @@
         <v>202</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C60" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D60" s="1">
-        <v>45534</v>
+        <v>45527</v>
       </c>
       <c r="E60" s="4">
-        <v>13.15</v>
+        <v>159</v>
       </c>
       <c r="F60" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G60" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="J60" s="2" t="s">
-        <v>90</v>
+        <v>197</v>
+      </c>
+      <c r="J60" s="6" t="s">
+        <v>111</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>22</v>
-      </c>
-      <c r="B61" s="1">
-        <v>45332</v>
+        <v>17</v>
       </c>
       <c r="C61" t="s">
-        <v>74</v>
+        <v>269</v>
       </c>
       <c r="D61" s="1">
-        <v>37308</v>
+        <v>45529</v>
       </c>
       <c r="E61" s="4">
-        <v>417.7</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F61" t="s">
-        <v>75</v>
+        <v>7</v>
       </c>
       <c r="G61" t="s">
-        <v>76</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I61" s="2" t="s">
-        <v>78</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>22</v>
-      </c>
-      <c r="B62" s="1">
-        <v>45316</v>
+        <v>17</v>
       </c>
       <c r="C62" t="s">
-        <v>59</v>
+        <v>275</v>
       </c>
       <c r="D62" s="1">
-        <v>45321</v>
+        <v>45529</v>
       </c>
       <c r="E62" s="4">
-        <v>194.6</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F62" t="s">
-        <v>52</v>
+        <v>156</v>
       </c>
       <c r="G62" t="s">
-        <v>53</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I62" s="2" t="s">
-        <v>55</v>
-      </c>
+        <v>255</v>
+      </c>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>22</v>
-      </c>
-      <c r="B63" s="1">
-        <v>45312</v>
+        <v>24</v>
       </c>
       <c r="C63" t="s">
-        <v>58</v>
+        <v>258</v>
       </c>
       <c r="D63" s="1">
-        <v>45329</v>
+        <v>45529</v>
       </c>
       <c r="E63" s="4">
-        <v>276.3</v>
+        <v>1200</v>
       </c>
       <c r="F63" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="G63" t="s">
-        <v>43</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I63" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
       <c r="L63" s="6"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>22</v>
-      </c>
-      <c r="B64" s="1">
-        <v>45311</v>
+        <v>24</v>
       </c>
       <c r="C64" t="s">
-        <v>57</v>
+        <v>198</v>
       </c>
       <c r="D64" s="1">
-        <v>45330</v>
+        <v>45534</v>
       </c>
       <c r="E64" s="4">
-        <v>423.5</v>
+        <v>13.15</v>
       </c>
       <c r="F64" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G64" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>35</v>
+        <v>199</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>22</v>
-      </c>
-      <c r="B65" s="1">
-        <v>45333</v>
+        <v>17</v>
       </c>
       <c r="C65" t="s">
-        <v>60</v>
+        <v>270</v>
       </c>
       <c r="D65" s="1">
-        <v>45337</v>
+        <v>45560</v>
       </c>
       <c r="E65" s="4">
-        <v>192.45</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F65" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="G65" t="s">
-        <v>62</v>
-      </c>
-      <c r="H65" t="s">
-        <v>63</v>
-      </c>
-      <c r="I65" s="2" t="s">
-        <v>64</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>22</v>
-      </c>
-      <c r="B66" s="1">
-        <v>45340</v>
+        <v>17</v>
       </c>
       <c r="C66" t="s">
-        <v>65</v>
+        <v>276</v>
       </c>
       <c r="D66" s="1">
-        <v>45341</v>
+        <v>45560</v>
       </c>
       <c r="E66" s="4">
-        <v>1000</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F66" t="s">
-        <v>66</v>
+        <v>156</v>
+      </c>
+      <c r="G66" t="s">
+        <v>255</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>22</v>
-      </c>
-      <c r="B67" s="1">
-        <v>45344</v>
+        <v>24</v>
       </c>
       <c r="C67" t="s">
-        <v>84</v>
+        <v>259</v>
       </c>
       <c r="D67" s="1">
-        <v>45387</v>
+        <v>45560</v>
       </c>
       <c r="E67" s="4">
-        <v>205.4</v>
+        <v>1200</v>
       </c>
       <c r="F67" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="G67" t="s">
-        <v>86</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I67" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="J67" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K67" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>22</v>
-      </c>
-      <c r="B68" s="1">
-        <v>45418</v>
+        <v>24</v>
       </c>
       <c r="C68" t="s">
-        <v>126</v>
+        <v>208</v>
       </c>
       <c r="D68" s="1">
-        <v>45387</v>
+        <v>45562</v>
       </c>
       <c r="E68" s="4">
-        <v>170</v>
+        <v>263.89999999999998</v>
       </c>
       <c r="F68" t="s">
-        <v>127</v>
+        <v>209</v>
       </c>
       <c r="G68" t="s">
-        <v>128</v>
-      </c>
-      <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
+        <v>210</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>212</v>
+      </c>
       <c r="J68" s="2" t="s">
-        <v>90</v>
+        <v>201</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>22</v>
       </c>
       <c r="B69" s="1">
-        <v>45386</v>
+        <v>45555</v>
       </c>
       <c r="C69" t="s">
-        <v>94</v>
+        <v>189</v>
       </c>
       <c r="D69" s="1">
-        <v>45387</v>
+        <v>45562</v>
       </c>
       <c r="E69" s="4">
-        <v>139.75</v>
+        <v>180.9</v>
       </c>
       <c r="F69" t="s">
         <v>61</v>
@@ -3593,10 +3806,10 @@
         <v>62</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>95</v>
+        <v>190</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>96</v>
+        <v>191</v>
       </c>
       <c r="J69" s="2" t="s">
         <v>90</v>
@@ -3605,33 +3818,33 @@
         <v>113</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>22</v>
       </c>
       <c r="B70" s="1">
-        <v>45358</v>
+        <v>45557</v>
       </c>
       <c r="C70" t="s">
-        <v>100</v>
+        <v>192</v>
       </c>
       <c r="D70" s="1">
-        <v>45387</v>
+        <v>45566</v>
       </c>
       <c r="E70" s="4">
-        <v>104</v>
+        <v>178.35</v>
       </c>
       <c r="F70" t="s">
-        <v>61</v>
+        <v>185</v>
       </c>
       <c r="G70" t="s">
-        <v>62</v>
+        <v>186</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>101</v>
+        <v>193</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>102</v>
+        <v>194</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>90</v>
@@ -3640,21 +3853,21 @@
         <v>113</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>22</v>
       </c>
       <c r="B71" s="1">
-        <v>45368</v>
+        <v>45562</v>
       </c>
       <c r="C71" t="s">
-        <v>91</v>
+        <v>213</v>
       </c>
       <c r="D71" s="1">
-        <v>45387</v>
+        <v>45568</v>
       </c>
       <c r="E71" s="4">
-        <v>178.35</v>
+        <v>88.85</v>
       </c>
       <c r="F71" t="s">
         <v>61</v>
@@ -3663,10 +3876,10 @@
         <v>62</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>92</v>
+        <v>214</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>93</v>
+        <v>215</v>
       </c>
       <c r="J71" s="9" t="s">
         <v>90</v>
@@ -3675,258 +3888,194 @@
         <v>113</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B72" s="1">
-        <v>45354</v>
+        <v>45576</v>
       </c>
       <c r="C72" t="s">
-        <v>97</v>
+        <v>216</v>
       </c>
       <c r="D72" s="1">
-        <v>45387</v>
+        <v>45576</v>
       </c>
       <c r="E72" s="4">
-        <v>137.9</v>
-      </c>
-      <c r="F72" t="s">
-        <v>61</v>
-      </c>
-      <c r="G72" t="s">
-        <v>62</v>
-      </c>
-      <c r="H72" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="I72" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="J72" s="2" t="s">
-        <v>90</v>
-      </c>
+        <v>37.700000000000003</v>
+      </c>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2"/>
       <c r="K72" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B73" s="1">
-        <v>45339</v>
+        <v>45576</v>
       </c>
       <c r="C73" t="s">
-        <v>114</v>
+        <v>217</v>
       </c>
       <c r="D73" s="1">
-        <v>45392</v>
+        <v>45576</v>
       </c>
       <c r="E73" s="4">
-        <v>461.95</v>
-      </c>
-      <c r="F73" t="s">
-        <v>75</v>
-      </c>
-      <c r="G73" t="s">
-        <v>76</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="I73" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="J73" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K73" s="2"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+        <v>116.1</v>
+      </c>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B74" s="1">
-        <v>45383</v>
-      </c>
-      <c r="C74" t="s">
-        <v>118</v>
+        <v>45576</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>219</v>
       </c>
       <c r="D74" s="1">
-        <v>45394</v>
+        <v>45576</v>
       </c>
       <c r="E74" s="4">
-        <v>211.9</v>
-      </c>
-      <c r="F74" t="s">
-        <v>61</v>
-      </c>
-      <c r="G74" t="s">
-        <v>62</v>
-      </c>
-      <c r="H74" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>90</v>
-      </c>
+        <v>154.80000000000001</v>
+      </c>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
       <c r="K74" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B75" s="1">
-        <v>45400</v>
-      </c>
-      <c r="C75" t="s">
-        <v>143</v>
+        <v>45576</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>218</v>
       </c>
       <c r="D75" s="1">
-        <v>45400</v>
+        <v>45576</v>
       </c>
       <c r="E75" s="4">
-        <v>211.85</v>
-      </c>
-      <c r="F75" t="s">
-        <v>50</v>
-      </c>
-      <c r="G75" t="s">
-        <v>51</v>
+        <v>102.2</v>
       </c>
       <c r="H75" s="2"/>
-      <c r="I75" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="J75" s="2" t="s">
-        <v>90</v>
-      </c>
+      <c r="I75" s="2"/>
+      <c r="J75" s="2"/>
       <c r="K75" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B76" s="1">
-        <v>45403</v>
+        <v>45576</v>
       </c>
       <c r="C76" t="s">
-        <v>121</v>
+        <v>254</v>
       </c>
       <c r="D76" s="1">
-        <v>45403</v>
+        <v>45576</v>
       </c>
       <c r="E76" s="4">
-        <v>447.55</v>
-      </c>
-      <c r="F76" t="s">
-        <v>123</v>
-      </c>
-      <c r="G76" t="s">
-        <v>124</v>
-      </c>
-      <c r="H76" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I76" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="J76" s="9" t="s">
-        <v>90</v>
-      </c>
+        <v>30.7</v>
+      </c>
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="9"/>
       <c r="K76" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B77" s="1">
-        <v>45319</v>
+        <v>45578</v>
       </c>
       <c r="C77" t="s">
-        <v>145</v>
+        <v>220</v>
       </c>
       <c r="D77" s="1">
-        <v>45421</v>
+        <v>45578</v>
       </c>
       <c r="E77" s="4">
-        <v>179.08</v>
-      </c>
-      <c r="F77" t="s">
-        <v>146</v>
-      </c>
-      <c r="G77" t="s">
-        <v>147</v>
+        <v>50.25</v>
       </c>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
-      <c r="J77" s="2" t="s">
-        <v>90</v>
-      </c>
+      <c r="J77" s="2"/>
       <c r="K77" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B78" s="1">
-        <v>45371</v>
-      </c>
-      <c r="C78" t="s">
-        <v>140</v>
+        <v>45576</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>221</v>
       </c>
       <c r="D78" s="1">
-        <v>45422</v>
+        <v>45579</v>
       </c>
       <c r="E78" s="4">
-        <v>162.15</v>
+        <v>279.89999999999998</v>
       </c>
       <c r="F78" t="s">
-        <v>75</v>
+        <v>222</v>
       </c>
       <c r="G78" t="s">
-        <v>76</v>
+        <v>223</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>141</v>
+        <v>224</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>142</v>
+        <v>225</v>
       </c>
       <c r="J78" s="2" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>22</v>
       </c>
       <c r="B79" s="1">
-        <v>45415</v>
+        <v>45581</v>
       </c>
       <c r="C79" t="s">
-        <v>137</v>
+        <v>227</v>
       </c>
       <c r="D79" s="1">
-        <v>45426</v>
+        <v>45583</v>
       </c>
       <c r="E79" s="4">
-        <v>137.9</v>
+        <v>232.4</v>
       </c>
       <c r="F79" t="s">
         <v>61</v>
@@ -3935,43 +4084,43 @@
         <v>62</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>138</v>
+        <v>228</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J79" s="2" t="s">
-        <v>90</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="J79" s="2"/>
       <c r="K79" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>22</v>
       </c>
       <c r="B80" s="1">
-        <v>45431</v>
+        <v>45577</v>
       </c>
       <c r="C80" t="s">
-        <v>148</v>
+        <v>231</v>
       </c>
       <c r="D80" s="1">
-        <v>45435</v>
+        <v>45583</v>
       </c>
       <c r="E80" s="4">
-        <v>227.55</v>
+        <v>924.65</v>
       </c>
       <c r="F80" t="s">
-        <v>149</v>
+        <v>75</v>
       </c>
       <c r="G80" t="s">
-        <v>150</v>
-      </c>
-      <c r="H80" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>232</v>
+      </c>
       <c r="I80" s="2" t="s">
-        <v>151</v>
+        <v>233</v>
       </c>
       <c r="J80" s="2" t="s">
         <v>90</v>
@@ -3980,33 +4129,33 @@
         <v>113</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>22</v>
       </c>
       <c r="B81" s="1">
-        <v>45435</v>
+        <v>45571</v>
       </c>
       <c r="C81" t="s">
-        <v>152</v>
+        <v>240</v>
       </c>
       <c r="D81" s="1">
-        <v>45439</v>
+        <v>45588</v>
       </c>
       <c r="E81" s="4">
-        <v>253.55</v>
+        <v>181.6</v>
       </c>
       <c r="F81" t="s">
-        <v>33</v>
+        <v>178</v>
       </c>
       <c r="G81" t="s">
-        <v>34</v>
-      </c>
-      <c r="H81" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="I81" s="2" t="s">
-        <v>153</v>
+        <v>182</v>
+      </c>
+      <c r="H81" t="s">
+        <v>241</v>
+      </c>
+      <c r="I81" s="2">
+        <v>10053082</v>
       </c>
       <c r="J81" s="2" t="s">
         <v>90</v>
@@ -4015,33 +4164,33 @@
         <v>113</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>22</v>
       </c>
       <c r="B82" s="1">
-        <v>45412</v>
+        <v>45578</v>
       </c>
       <c r="C82" t="s">
-        <v>181</v>
+        <v>237</v>
       </c>
       <c r="D82" s="1">
-        <v>45460</v>
+        <v>45589</v>
       </c>
       <c r="E82" s="4">
-        <v>214</v>
+        <v>194.6</v>
       </c>
       <c r="F82" t="s">
-        <v>178</v>
+        <v>33</v>
       </c>
       <c r="G82" t="s">
-        <v>182</v>
+        <v>34</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>179</v>
+        <v>238</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>183</v>
+        <v>239</v>
       </c>
       <c r="J82" s="2" t="s">
         <v>90</v>
@@ -4050,138 +4199,105 @@
         <v>113</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>22</v>
-      </c>
-      <c r="B83" s="1">
-        <v>45438</v>
+        <v>17</v>
       </c>
       <c r="C83" t="s">
-        <v>184</v>
+        <v>271</v>
       </c>
       <c r="D83" s="1">
-        <v>45475</v>
+        <v>45590</v>
       </c>
       <c r="E83" s="4">
-        <v>174.6</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F83" t="s">
-        <v>185</v>
+        <v>7</v>
       </c>
       <c r="G83" t="s">
-        <v>186</v>
-      </c>
-      <c r="H83" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="I83" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="J83" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K83" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
+      <c r="J83" s="2"/>
+      <c r="K83" s="2"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>22</v>
-      </c>
-      <c r="B84" s="1">
-        <v>45555</v>
+        <v>17</v>
       </c>
       <c r="C84" t="s">
-        <v>189</v>
+        <v>277</v>
       </c>
       <c r="D84" s="1">
-        <v>45562</v>
+        <v>45590</v>
       </c>
       <c r="E84" s="4">
-        <v>180.9</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F84" t="s">
-        <v>61</v>
+        <v>156</v>
       </c>
       <c r="G84" t="s">
-        <v>62</v>
-      </c>
-      <c r="H84" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="I84" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="J84" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K84" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+      <c r="H84" s="2"/>
+      <c r="I84" s="2"/>
+      <c r="J84" s="2"/>
+      <c r="K84" s="2"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>22</v>
-      </c>
-      <c r="B85" s="1">
-        <v>45557</v>
+        <v>24</v>
       </c>
       <c r="C85" t="s">
-        <v>192</v>
+        <v>260</v>
       </c>
       <c r="D85" s="1">
-        <v>45566</v>
+        <v>45590</v>
       </c>
       <c r="E85" s="4">
-        <v>178.35</v>
+        <v>1200</v>
       </c>
       <c r="F85" t="s">
-        <v>185</v>
+        <v>11</v>
       </c>
       <c r="G85" t="s">
-        <v>186</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="I85" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="J85" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K85" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>22</v>
       </c>
       <c r="B86" s="1">
-        <v>45562</v>
+        <v>45590</v>
       </c>
       <c r="C86" t="s">
-        <v>213</v>
+        <v>245</v>
       </c>
       <c r="D86" s="1">
-        <v>45568</v>
+        <v>45593</v>
       </c>
       <c r="E86" s="4">
-        <v>88.85</v>
+        <v>218.05</v>
       </c>
       <c r="F86" t="s">
-        <v>61</v>
+        <v>246</v>
       </c>
       <c r="G86" t="s">
-        <v>62</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>214</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="H86" s="2"/>
       <c r="I86" s="2" t="s">
-        <v>215</v>
+        <v>248</v>
       </c>
       <c r="J86" s="2" t="s">
         <v>90</v>
@@ -4190,66 +4306,68 @@
         <v>113</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>22</v>
       </c>
       <c r="B87" s="1">
-        <v>45581</v>
+        <v>45583</v>
       </c>
       <c r="C87" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="D87" s="1">
-        <v>45583</v>
+        <v>45596</v>
       </c>
       <c r="E87" s="4">
-        <v>232.4</v>
+        <v>194.6</v>
       </c>
       <c r="F87" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G87" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="J87" s="2"/>
+        <v>244</v>
+      </c>
+      <c r="J87" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="K87" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>22</v>
       </c>
       <c r="B88" s="1">
-        <v>45577</v>
+        <v>45585</v>
       </c>
       <c r="C88" t="s">
-        <v>231</v>
+        <v>250</v>
       </c>
       <c r="D88" s="1">
-        <v>45583</v>
+        <v>45603</v>
       </c>
       <c r="E88" s="4">
-        <v>924.65</v>
+        <v>181.6</v>
       </c>
       <c r="F88" t="s">
-        <v>75</v>
+        <v>178</v>
       </c>
       <c r="G88" t="s">
-        <v>76</v>
+        <v>182</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>233</v>
+        <v>252</v>
       </c>
       <c r="J88" s="2" t="s">
         <v>90</v>
@@ -4258,612 +4376,584 @@
         <v>113</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
+        <v>73</v>
+      </c>
+      <c r="B89" s="1">
+        <v>45606</v>
+      </c>
+      <c r="C89" t="s">
+        <v>253</v>
+      </c>
+      <c r="D89" s="1">
+        <v>45606</v>
+      </c>
+      <c r="E89" s="4">
+        <v>100</v>
+      </c>
+      <c r="F89" t="s">
+        <v>156</v>
+      </c>
+      <c r="H89" s="2"/>
+      <c r="I89" s="2"/>
+      <c r="J89" s="2"/>
+      <c r="K89" s="2"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A90" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B89" s="1">
-        <v>45571</v>
-      </c>
-      <c r="C89" t="s">
-        <v>240</v>
-      </c>
-      <c r="D89" s="1">
-        <v>45588</v>
-      </c>
-      <c r="E89" s="4">
-        <v>181.6</v>
-      </c>
-      <c r="F89" t="s">
-        <v>178</v>
-      </c>
-      <c r="G89" t="s">
-        <v>182</v>
-      </c>
-      <c r="H89" t="s">
-        <v>241</v>
-      </c>
-      <c r="I89" s="2">
-        <v>10053082</v>
-      </c>
-      <c r="J89" s="2" t="s">
+      <c r="B90" s="13">
+        <v>45606</v>
+      </c>
+      <c r="C90" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="D90" s="13">
+        <v>45613</v>
+      </c>
+      <c r="E90" s="16">
+        <v>256.45</v>
+      </c>
+      <c r="F90" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="G90" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="H90" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="I90" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="J90" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="K89" s="2" t="s">
+      <c r="K90" s="18" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>22</v>
-      </c>
-      <c r="B90" s="1">
-        <v>45578</v>
-      </c>
-      <c r="C90" t="s">
-        <v>237</v>
-      </c>
-      <c r="D90" s="1">
-        <v>45589</v>
-      </c>
-      <c r="E90" s="4">
-        <v>194.6</v>
-      </c>
-      <c r="F90" t="s">
-        <v>33</v>
-      </c>
-      <c r="G90" t="s">
-        <v>34</v>
-      </c>
-      <c r="H90" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="J90" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K90" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>22</v>
-      </c>
-      <c r="B91" s="1">
-        <v>45590</v>
+        <v>17</v>
       </c>
       <c r="C91" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="D91" s="1">
-        <v>45593</v>
+        <v>45621</v>
       </c>
       <c r="E91" s="4">
-        <v>218.05</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F91" t="s">
-        <v>246</v>
+        <v>7</v>
       </c>
       <c r="G91" t="s">
-        <v>247</v>
+        <v>8</v>
       </c>
       <c r="H91" s="2"/>
-      <c r="I91" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="J91" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K91" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I91" s="2"/>
+      <c r="J91" s="2"/>
+      <c r="K91" s="2"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>22</v>
-      </c>
-      <c r="B92" s="1">
-        <v>45583</v>
+        <v>17</v>
       </c>
       <c r="C92" t="s">
-        <v>242</v>
+        <v>278</v>
       </c>
       <c r="D92" s="1">
-        <v>45596</v>
+        <v>45621</v>
       </c>
       <c r="E92" s="4">
-        <v>194.6</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F92" t="s">
-        <v>52</v>
+        <v>156</v>
       </c>
       <c r="G92" t="s">
-        <v>53</v>
-      </c>
-      <c r="H92" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="I92" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="J92" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K92" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+      <c r="K92" s="2"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>22</v>
-      </c>
-      <c r="B93" s="1">
-        <v>45585</v>
+        <v>24</v>
       </c>
       <c r="C93" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="D93" s="1">
-        <v>45603</v>
+        <v>45621</v>
       </c>
       <c r="E93" s="4">
-        <v>181.6</v>
+        <v>1200</v>
       </c>
       <c r="F93" t="s">
-        <v>178</v>
+        <v>11</v>
       </c>
       <c r="G93" t="s">
-        <v>182</v>
-      </c>
-      <c r="H93" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I93" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="J93" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K93" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
+      <c r="J93" s="2"/>
+      <c r="K93" s="2"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C94" t="s">
-        <v>155</v>
+        <v>273</v>
       </c>
       <c r="D94" s="1">
-        <v>45435</v>
+        <v>45651</v>
       </c>
       <c r="E94" s="4">
-        <v>479.5</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F94" t="s">
-        <v>156</v>
+        <v>7</v>
       </c>
       <c r="G94" t="s">
-        <v>157</v>
+        <v>8</v>
       </c>
       <c r="H94" s="2"/>
-      <c r="I94" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J94" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="K94" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I94" s="2"/>
+      <c r="J94" s="2"/>
+      <c r="K94" s="2"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C95" t="s">
-        <v>158</v>
+        <v>279</v>
       </c>
       <c r="D95" s="1">
-        <v>45435</v>
+        <v>45651</v>
       </c>
       <c r="E95" s="4">
-        <v>420</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F95" t="s">
         <v>156</v>
       </c>
       <c r="G95" t="s">
-        <v>157</v>
+        <v>255</v>
       </c>
       <c r="H95" s="2"/>
-      <c r="I95" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="J95" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="K95" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E96" s="4"/>
-    </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="I95" s="2"/>
+      <c r="J95" s="2"/>
+      <c r="K95" s="2"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A96" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B96" s="14"/>
+      <c r="C96" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="D96" s="14">
+        <v>45651</v>
+      </c>
+      <c r="E96" s="17">
+        <v>1200</v>
+      </c>
+      <c r="F96" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G96" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H96" s="19"/>
+      <c r="I96" s="19"/>
+      <c r="J96" s="19"/>
+      <c r="K96" s="21"/>
+    </row>
+    <row r="97" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E97" s="4"/>
     </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E98" s="4"/>
     </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E99" s="4"/>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E100" s="4"/>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E101" s="4"/>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E102" s="4"/>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E103" s="4"/>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E104" s="4"/>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E105" s="4"/>
     </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E106" s="4"/>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E107" s="4"/>
     </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E108" s="4"/>
     </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E109" s="4"/>
     </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E110" s="4"/>
     </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E111" s="4"/>
     </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E112" s="4"/>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E113" s="4"/>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E114" s="4"/>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E115" s="4"/>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E116" s="4"/>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E117" s="4"/>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E118" s="4"/>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E119" s="4"/>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E120" s="4"/>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E121" s="4"/>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E122" s="4"/>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E123" s="4"/>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E124" s="4"/>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E125" s="4"/>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E126" s="4"/>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E127" s="4"/>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E128" s="4"/>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E129" s="4"/>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E130" s="4"/>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E131" s="4"/>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E132" s="4"/>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E133" s="4"/>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E134" s="4"/>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E135" s="4"/>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E136" s="4"/>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E137" s="4"/>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E138" s="4"/>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E139" s="4"/>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E140" s="4"/>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E141" s="4"/>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E142" s="4"/>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E143" s="4"/>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E144" s="4"/>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E145" s="4"/>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E146" s="4"/>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E147" s="4"/>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E148" s="4"/>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E149" s="4"/>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E150" s="4"/>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E151" s="4"/>
     </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E152" s="4"/>
     </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E153" s="4"/>
     </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E154" s="4"/>
     </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E155" s="4"/>
     </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E156" s="4"/>
     </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E157" s="4"/>
     </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E158" s="4"/>
     </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E159" s="4"/>
     </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E160" s="4"/>
     </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E161" s="4"/>
     </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E162" s="4"/>
     </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E163" s="4"/>
     </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E164" s="4"/>
     </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E165" s="4"/>
     </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E166" s="4"/>
     </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E167" s="4"/>
     </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E168" s="4"/>
     </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E169" s="4"/>
     </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E170" s="4"/>
     </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E171" s="4"/>
     </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E172" s="4"/>
     </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E173" s="4"/>
     </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E174" s="4"/>
     </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E175" s="4"/>
     </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E176" s="4"/>
     </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E177" s="4"/>
     </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E178" s="4"/>
     </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E179" s="4"/>
     </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E180" s="4"/>
     </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E181" s="4"/>
     </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E182" s="4"/>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E183" s="4"/>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E184" s="4"/>
     </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E185" s="4"/>
     </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E186" s="4"/>
     </row>
-    <row r="187" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E187" s="4"/>
     </row>
-    <row r="188" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E188" s="4"/>
     </row>
-    <row r="189" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E189" s="4"/>
     </row>
-    <row r="190" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E190" s="4"/>
     </row>
-    <row r="191" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E191" s="4"/>
     </row>
-    <row r="192" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E192" s="4"/>
     </row>
-    <row r="193" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E193" s="4"/>
     </row>
-    <row r="194" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E194" s="4"/>
     </row>
-    <row r="195" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E195" s="4"/>
     </row>
-    <row r="196" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E196" s="4"/>
     </row>
-    <row r="197" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E197" s="4"/>
     </row>
-    <row r="198" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E198" s="4"/>
     </row>
-    <row r="199" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E199" s="4"/>
     </row>
-    <row r="200" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E200" s="4"/>
     </row>
-    <row r="201" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E201" s="4"/>
     </row>
-    <row r="202" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E202" s="4"/>
     </row>
-    <row r="203" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E203" s="4"/>
     </row>
-    <row r="204" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E204" s="4"/>
     </row>
-    <row r="205" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E205" s="4"/>
     </row>
-    <row r="206" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E206" s="4"/>
     </row>
-    <row r="207" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E207" s="4"/>
     </row>
-    <row r="208" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E208" s="4"/>
     </row>
-    <row r="209" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E209" s="4"/>
     </row>
-    <row r="210" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E210" s="4"/>
     </row>
-    <row r="211" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E211" s="4"/>
     </row>
-    <row r="212" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E212" s="4"/>
     </row>
-    <row r="213" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E213" s="4"/>
     </row>
-    <row r="214" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E214" s="4"/>
     </row>
-    <row r="215" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E215" s="4"/>
     </row>
-    <row r="216" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E216" s="4"/>
     </row>
-    <row r="217" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E217" s="4"/>
     </row>
-    <row r="218" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E218" s="4"/>
     </row>
-    <row r="219" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E219" s="4"/>
     </row>
-    <row r="220" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E220" s="4"/>
     </row>
   </sheetData>
@@ -4904,47 +4994,47 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Rechnung SKV Quartal 4, Rechnung Bolero
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E6D84D-072C-4B78-AFA6-B2FBBEC2FBBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5F8815-0223-45FA-A651-C9D8CE8277FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="293">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -896,6 +896,27 @@
   </si>
   <si>
     <t xml:space="preserve">00042414 </t>
+  </si>
+  <si>
+    <t>SKV Suisa Abgaben Akonto 4. Quartal</t>
+  </si>
+  <si>
+    <t>000000000000014423010586707</t>
+  </si>
+  <si>
+    <t>14423</t>
+  </si>
+  <si>
+    <t>Film: Bolero</t>
+  </si>
+  <si>
+    <t>Agora Films Sarl</t>
+  </si>
+  <si>
+    <t>Rue Muzy, 1207 Genf</t>
+  </si>
+  <si>
+    <t>29203</t>
   </si>
 </sst>
 </file>
@@ -1009,7 +1030,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1020,18 +1041,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1098,8 +1118,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K96" totalsRowShown="0">
-  <autoFilter ref="A1:K96" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K98" totalsRowShown="0">
+  <autoFilter ref="A1:K98" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K96">
     <sortCondition ref="D1:D96"/>
   </sortState>
@@ -1799,8 +1819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96:K96"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1936,8 +1956,8 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -2547,8 +2567,8 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -2607,8 +2627,8 @@
       <c r="K29" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -2644,8 +2664,8 @@
       <c r="K30" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -2677,8 +2697,8 @@
       <c r="K31" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -2714,8 +2734,8 @@
       <c r="K32" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
@@ -2751,8 +2771,8 @@
       <c r="K33" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -2782,10 +2802,10 @@
       <c r="I34" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="J34" s="20" t="s">
+      <c r="J34" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="K34" s="20" t="s">
+      <c r="K34" s="2" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2953,10 +2973,10 @@
       <c r="I39" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="J39" s="20" t="s">
+      <c r="J39" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="K39" s="20" t="s">
+      <c r="K39" s="2" t="s">
         <v>113</v>
       </c>
     </row>
@@ -4401,37 +4421,37 @@
       <c r="K89" s="2"/>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A90" s="11" t="s">
+      <c r="A90" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B90" s="13">
+      <c r="B90" s="12">
         <v>45606</v>
       </c>
-      <c r="C90" s="11" t="s">
+      <c r="C90" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="D90" s="13">
+      <c r="D90" s="12">
         <v>45613</v>
       </c>
-      <c r="E90" s="16">
+      <c r="E90" s="15">
         <v>256.45</v>
       </c>
-      <c r="F90" s="11" t="s">
+      <c r="F90" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="G90" s="11" t="s">
+      <c r="G90" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="H90" s="18" t="s">
+      <c r="H90" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="I90" s="18" t="s">
+      <c r="I90" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="J90" s="18" t="s">
+      <c r="J90" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="K90" s="18" t="s">
+      <c r="K90" s="17" t="s">
         <v>113</v>
       </c>
     </row>
@@ -4560,76 +4580,135 @@
       <c r="K95" s="2"/>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A96" s="12" t="s">
+      <c r="A96" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B96" s="14"/>
-      <c r="C96" s="15" t="s">
+      <c r="B96" s="13"/>
+      <c r="C96" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="D96" s="14">
+      <c r="D96" s="13">
         <v>45651</v>
       </c>
-      <c r="E96" s="17">
+      <c r="E96" s="16">
         <v>1200</v>
       </c>
-      <c r="F96" s="15" t="s">
+      <c r="F96" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G96" s="15" t="s">
+      <c r="G96" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="H96" s="19"/>
-      <c r="I96" s="19"/>
-      <c r="J96" s="19"/>
-      <c r="K96" s="21"/>
-    </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E97" s="4"/>
-    </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E98" s="4"/>
-    </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="H96" s="18"/>
+      <c r="I96" s="18"/>
+      <c r="J96" s="18"/>
+      <c r="K96" s="19"/>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>24</v>
+      </c>
+      <c r="C97" t="s">
+        <v>286</v>
+      </c>
+      <c r="D97" s="1">
+        <v>45618</v>
+      </c>
+      <c r="E97" s="4">
+        <v>68.08</v>
+      </c>
+      <c r="F97" t="s">
+        <v>38</v>
+      </c>
+      <c r="G97" t="s">
+        <v>39</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="I97" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="J97" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K97" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>22</v>
+      </c>
+      <c r="B98" s="1">
+        <v>45604</v>
+      </c>
+      <c r="C98" t="s">
+        <v>289</v>
+      </c>
+      <c r="D98" s="1">
+        <v>45615</v>
+      </c>
+      <c r="E98" s="4">
+        <v>101.12</v>
+      </c>
+      <c r="F98" t="s">
+        <v>290</v>
+      </c>
+      <c r="G98" t="s">
+        <v>291</v>
+      </c>
+      <c r="H98" s="2"/>
+      <c r="I98" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="J98" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K98" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E99" s="4"/>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E100" s="4"/>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E101" s="4"/>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E102" s="4"/>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E103" s="4"/>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E104" s="4"/>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E105" s="4"/>
     </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E106" s="4"/>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E107" s="4"/>
     </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E108" s="4"/>
     </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E109" s="4"/>
     </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E110" s="4"/>
     </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E111" s="4"/>
     </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E112" s="4"/>
     </row>
     <row r="113" spans="5:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
SKV Quartal 4, Rechnung Bolero
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5F8815-0223-45FA-A651-C9D8CE8277FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77C791F-B900-4412-A0F7-8E1410F8246D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="2964" yWindow="1884" windowWidth="15684" windowHeight="11832" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -1820,7 +1820,7 @@
   <dimension ref="A1:M220"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A80" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
error in Einnahmen und Ausgaben
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77C791F-B900-4412-A0F7-8E1410F8246D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FFF491-8BC3-4BFA-8C0A-4AFB9E13BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2964" yWindow="1884" windowWidth="15684" windowHeight="11832" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="289">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -905,18 +905,6 @@
   </si>
   <si>
     <t>14423</t>
-  </si>
-  <si>
-    <t>Film: Bolero</t>
-  </si>
-  <si>
-    <t>Agora Films Sarl</t>
-  </si>
-  <si>
-    <t>Rue Muzy, 1207 Genf</t>
-  </si>
-  <si>
-    <t>29203</t>
   </si>
 </sst>
 </file>
@@ -1054,8 +1042,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{27287C1A-B7AC-49C2-89D9-0074BB2DB80A}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -1118,8 +1106,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K98" totalsRowShown="0">
-  <autoFilter ref="A1:K98" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K97" totalsRowShown="0">
+  <autoFilter ref="A1:K97" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K96">
     <sortCondition ref="D1:D96"/>
   </sortState>
@@ -1154,9 +1142,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1194,7 +1182,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1300,7 +1288,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1456,18 +1444,18 @@
       <selection activeCell="A18" sqref="A18:K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.44140625" customWidth="1"/>
+    <col min="7" max="7" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1490,7 +1478,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1510,7 +1498,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -1527,7 +1515,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1544,7 +1532,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -1561,7 +1549,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -1578,7 +1566,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1595,7 +1583,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1612,7 +1600,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1635,7 +1623,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1658,7 +1646,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1681,7 +1669,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1701,7 +1689,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1724,7 +1712,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1744,7 +1732,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1761,7 +1749,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1778,7 +1766,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1817,28 +1805,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
-  <dimension ref="A1:M220"/>
+  <dimension ref="A1:M219"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A80" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+      <selection activeCell="A98" sqref="A98:XFD98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1873,7 +1861,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1904,7 +1892,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1930,7 +1918,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1959,7 +1947,7 @@
       <c r="L4" s="20"/>
       <c r="M4" s="20"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -1986,7 +1974,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -2017,7 +2005,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2041,7 +2029,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2065,7 +2053,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2090,7 +2078,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -2114,7 +2102,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -2138,7 +2126,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2169,7 +2157,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -2192,7 +2180,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -2216,7 +2204,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -2244,7 +2232,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -2275,7 +2263,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2303,7 +2291,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -2334,7 +2322,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2362,7 +2350,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -2383,7 +2371,7 @@
       </c>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -2414,7 +2402,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2438,7 +2426,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -2463,7 +2451,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2487,7 +2475,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2519,7 +2507,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>73</v>
       </c>
@@ -2543,7 +2531,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -2570,7 +2558,7 @@
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2596,7 +2584,7 @@
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -2630,7 +2618,7 @@
       <c r="L29" s="20"/>
       <c r="M29" s="20"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -2667,7 +2655,7 @@
       <c r="L30" s="20"/>
       <c r="M30" s="20"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -2700,7 +2688,7 @@
       <c r="L31" s="20"/>
       <c r="M31" s="20"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -2737,7 +2725,7 @@
       <c r="L32" s="20"/>
       <c r="M32" s="20"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -2774,7 +2762,7 @@
       <c r="L33" s="20"/>
       <c r="M33" s="20"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -2809,7 +2797,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -2844,7 +2832,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -2877,7 +2865,7 @@
       </c>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -2912,7 +2900,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -2945,7 +2933,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -2980,7 +2968,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -3005,7 +2993,7 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -3029,7 +3017,7 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -3060,7 +3048,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -3095,7 +3083,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -3130,7 +3118,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -3163,7 +3151,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -3193,7 +3181,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -3223,7 +3211,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -3248,7 +3236,7 @@
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>24</v>
       </c>
@@ -3272,7 +3260,7 @@
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>22</v>
       </c>
@@ -3307,7 +3295,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>24</v>
       </c>
@@ -3339,7 +3327,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -3374,7 +3362,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>17</v>
       </c>
@@ -3396,7 +3384,7 @@
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>24</v>
       </c>
@@ -3420,7 +3408,7 @@
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>22</v>
       </c>
@@ -3455,7 +3443,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>17</v>
       </c>
@@ -3477,7 +3465,7 @@
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -3502,7 +3490,7 @@
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>24</v>
       </c>
@@ -3526,7 +3514,7 @@
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -3558,7 +3546,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -3590,7 +3578,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>17</v>
       </c>
@@ -3615,7 +3603,7 @@
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>17</v>
       </c>
@@ -3640,7 +3628,7 @@
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>24</v>
       </c>
@@ -3665,7 +3653,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="6"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>24</v>
       </c>
@@ -3697,7 +3685,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>17</v>
       </c>
@@ -3722,7 +3710,7 @@
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>17</v>
       </c>
@@ -3747,7 +3735,7 @@
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>24</v>
       </c>
@@ -3771,7 +3759,7 @@
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>24</v>
       </c>
@@ -3803,7 +3791,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>22</v>
       </c>
@@ -3838,7 +3826,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>22</v>
       </c>
@@ -3873,7 +3861,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>22</v>
       </c>
@@ -3908,7 +3896,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>73</v>
       </c>
@@ -3931,7 +3919,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -3954,7 +3942,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -3977,7 +3965,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -4000,7 +3988,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>73</v>
       </c>
@@ -4023,7 +4011,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>73</v>
       </c>
@@ -4046,7 +4034,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>73</v>
       </c>
@@ -4081,7 +4069,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>22</v>
       </c>
@@ -4114,7 +4102,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>22</v>
       </c>
@@ -4149,7 +4137,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>22</v>
       </c>
@@ -4184,7 +4172,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>22</v>
       </c>
@@ -4219,7 +4207,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>17</v>
       </c>
@@ -4244,7 +4232,7 @@
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>17</v>
       </c>
@@ -4269,7 +4257,7 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>24</v>
       </c>
@@ -4293,7 +4281,7 @@
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>22</v>
       </c>
@@ -4326,7 +4314,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>22</v>
       </c>
@@ -4361,7 +4349,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>22</v>
       </c>
@@ -4396,7 +4384,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>73</v>
       </c>
@@ -4420,7 +4408,7 @@
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="s">
         <v>22</v>
       </c>
@@ -4455,7 +4443,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>17</v>
       </c>
@@ -4480,7 +4468,7 @@
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>17</v>
       </c>
@@ -4505,7 +4493,7 @@
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>24</v>
       </c>
@@ -4529,7 +4517,7 @@
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>17</v>
       </c>
@@ -4554,7 +4542,7 @@
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>17</v>
       </c>
@@ -4579,7 +4567,7 @@
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="11" t="s">
         <v>24</v>
       </c>
@@ -4604,7 +4592,7 @@
       <c r="J96" s="18"/>
       <c r="K96" s="19"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>24</v>
       </c>
@@ -4636,404 +4624,371 @@
         <v>113</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>22</v>
-      </c>
-      <c r="B98" s="1">
-        <v>45604</v>
-      </c>
-      <c r="C98" t="s">
-        <v>289</v>
-      </c>
-      <c r="D98" s="1">
-        <v>45615</v>
-      </c>
-      <c r="E98" s="4">
-        <v>101.12</v>
-      </c>
-      <c r="F98" t="s">
-        <v>290</v>
-      </c>
-      <c r="G98" t="s">
-        <v>291</v>
-      </c>
-      <c r="H98" s="2"/>
-      <c r="I98" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="J98" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K98" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E98" s="4"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E99" s="4"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E100" s="4"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E101" s="4"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E102" s="4"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E103" s="4"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E104" s="4"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E105" s="4"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E106" s="4"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E107" s="4"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E108" s="4"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E109" s="4"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E110" s="4"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E111" s="4"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E112" s="4"/>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E113" s="4"/>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E114" s="4"/>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E115" s="4"/>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E116" s="4"/>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E117" s="4"/>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E118" s="4"/>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E119" s="4"/>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E120" s="4"/>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E121" s="4"/>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E122" s="4"/>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E123" s="4"/>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E124" s="4"/>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E125" s="4"/>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E126" s="4"/>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E127" s="4"/>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E128" s="4"/>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E129" s="4"/>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E130" s="4"/>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E131" s="4"/>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E132" s="4"/>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E133" s="4"/>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E134" s="4"/>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E135" s="4"/>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E136" s="4"/>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E137" s="4"/>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E138" s="4"/>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E139" s="4"/>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E140" s="4"/>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E141" s="4"/>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E142" s="4"/>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E143" s="4"/>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E144" s="4"/>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E145" s="4"/>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E146" s="4"/>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E147" s="4"/>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E148" s="4"/>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E149" s="4"/>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E150" s="4"/>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E151" s="4"/>
     </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E152" s="4"/>
     </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E153" s="4"/>
     </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E154" s="4"/>
     </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E155" s="4"/>
     </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E156" s="4"/>
     </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E157" s="4"/>
     </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E158" s="4"/>
     </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E159" s="4"/>
     </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E160" s="4"/>
     </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E161" s="4"/>
     </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E162" s="4"/>
     </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E163" s="4"/>
     </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E164" s="4"/>
     </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E165" s="4"/>
     </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E166" s="4"/>
     </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E167" s="4"/>
     </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E168" s="4"/>
     </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E169" s="4"/>
     </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E170" s="4"/>
     </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E171" s="4"/>
     </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E172" s="4"/>
     </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E173" s="4"/>
     </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E174" s="4"/>
     </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E175" s="4"/>
     </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E176" s="4"/>
     </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E177" s="4"/>
     </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E178" s="4"/>
     </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E179" s="4"/>
     </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E180" s="4"/>
     </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E181" s="4"/>
     </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E182" s="4"/>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E183" s="4"/>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E184" s="4"/>
     </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E185" s="4"/>
     </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E186" s="4"/>
     </row>
-    <row r="187" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E187" s="4"/>
     </row>
-    <row r="188" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="188" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E188" s="4"/>
     </row>
-    <row r="189" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="189" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E189" s="4"/>
     </row>
-    <row r="190" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="190" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E190" s="4"/>
     </row>
-    <row r="191" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="191" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E191" s="4"/>
     </row>
-    <row r="192" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E192" s="4"/>
     </row>
-    <row r="193" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E193" s="4"/>
     </row>
-    <row r="194" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E194" s="4"/>
     </row>
-    <row r="195" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E195" s="4"/>
     </row>
-    <row r="196" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E196" s="4"/>
     </row>
-    <row r="197" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E197" s="4"/>
     </row>
-    <row r="198" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E198" s="4"/>
     </row>
-    <row r="199" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E199" s="4"/>
     </row>
-    <row r="200" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E200" s="4"/>
     </row>
-    <row r="201" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E201" s="4"/>
     </row>
-    <row r="202" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E202" s="4"/>
     </row>
-    <row r="203" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="203" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E203" s="4"/>
     </row>
-    <row r="204" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E204" s="4"/>
     </row>
-    <row r="205" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="205" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E205" s="4"/>
     </row>
-    <row r="206" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E206" s="4"/>
     </row>
-    <row r="207" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E207" s="4"/>
     </row>
-    <row r="208" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E208" s="4"/>
     </row>
-    <row r="209" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="209" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E209" s="4"/>
     </row>
-    <row r="210" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="210" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E210" s="4"/>
     </row>
-    <row r="211" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="211" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E211" s="4"/>
     </row>
-    <row r="212" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="212" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E212" s="4"/>
     </row>
-    <row r="213" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="213" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E213" s="4"/>
     </row>
-    <row r="214" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="214" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E214" s="4"/>
     </row>
-    <row r="215" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="215" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E215" s="4"/>
     </row>
-    <row r="216" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="216" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E216" s="4"/>
     </row>
-    <row r="217" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="217" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E217" s="4"/>
     </row>
-    <row r="218" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="218" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E218" s="4"/>
     </row>
-    <row r="219" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="219" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E219" s="4"/>
-    </row>
-    <row r="220" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E220" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -5057,7 +5012,7 @@
           <x14:formula1>
             <xm:f>dropdown!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>A62:A95 A97:A190 A3:A59</xm:sqref>
+          <xm:sqref>A62:A95 A3:A59 A97:A189</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5073,47 +5028,47 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Rechnungen Cafe de los maestros, Joan Baez eingetragen
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FFF491-8BC3-4BFA-8C0A-4AFB9E13BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72342951-B9C5-4BFC-A0C0-16A554A5B600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="2964" yWindow="1884" windowWidth="15684" windowHeight="11832" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="297">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -905,6 +905,30 @@
   </si>
   <si>
     <t>14423</t>
+  </si>
+  <si>
+    <t>Film: Cafe de los maestros</t>
+  </si>
+  <si>
+    <t>Pathe Films AG</t>
+  </si>
+  <si>
+    <t>Neugasse 6, Postfach, 8031 Zürich</t>
+  </si>
+  <si>
+    <t>93 88771 00200 00000 06007 10145</t>
+  </si>
+  <si>
+    <t>Film: Joan Baez - I am a Noise</t>
+  </si>
+  <si>
+    <t>47164</t>
+  </si>
+  <si>
+    <t>Werbeweischer November 2024</t>
+  </si>
+  <si>
+    <t>241071TS</t>
   </si>
 </sst>
 </file>
@@ -1042,8 +1066,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{27287C1A-B7AC-49C2-89D9-0074BB2DB80A}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -1106,8 +1130,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K97" totalsRowShown="0">
-  <autoFilter ref="A1:K97" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K99" totalsRowShown="0">
+  <autoFilter ref="A1:K99" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K96">
     <sortCondition ref="D1:D96"/>
   </sortState>
@@ -1142,9 +1166,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1182,7 +1206,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1288,7 +1312,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1438,24 +1462,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:K18"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.42578125" customWidth="1"/>
+    <col min="7" max="7" width="42.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1478,7 +1502,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1498,7 +1522,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -1515,7 +1539,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1532,7 +1556,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -1549,7 +1573,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -1566,7 +1590,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1583,7 +1607,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1600,7 +1624,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1623,7 +1647,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1646,7 +1670,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1669,7 +1693,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1689,7 +1713,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1712,7 +1736,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1732,7 +1756,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1749,7 +1773,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1766,7 +1790,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1781,6 +1805,29 @@
       </c>
       <c r="E17" t="s">
         <v>264</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>295</v>
+      </c>
+      <c r="C18" s="5">
+        <v>45630</v>
+      </c>
+      <c r="D18" s="4">
+        <v>24.76</v>
+      </c>
+      <c r="E18" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" t="s">
+        <v>104</v>
+      </c>
+      <c r="G18" t="s">
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -1795,7 +1842,7 @@
           <x14:formula1>
             <xm:f>dropdown!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A17</xm:sqref>
+          <xm:sqref>A2:A18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1808,25 +1855,25 @@
   <dimension ref="A1:M219"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A80" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98:XFD98"/>
+      <selection activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1861,7 +1908,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1892,7 +1939,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1918,7 +1965,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1947,7 +1994,7 @@
       <c r="L4" s="20"/>
       <c r="M4" s="20"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -1974,7 +2021,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -2005,7 +2052,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2029,7 +2076,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2053,7 +2100,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2078,7 +2125,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -2102,7 +2149,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -2126,7 +2173,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2157,7 +2204,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -2180,7 +2227,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -2204,7 +2251,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -2232,7 +2279,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -2263,7 +2310,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2291,7 +2338,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -2322,7 +2369,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2350,7 +2397,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -2371,7 +2418,7 @@
       </c>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -2402,7 +2449,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2426,7 +2473,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -2451,7 +2498,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2475,7 +2522,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2507,7 +2554,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>73</v>
       </c>
@@ -2531,7 +2578,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -2558,7 +2605,7 @@
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2584,7 +2631,7 @@
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -2618,7 +2665,7 @@
       <c r="L29" s="20"/>
       <c r="M29" s="20"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -2655,7 +2702,7 @@
       <c r="L30" s="20"/>
       <c r="M30" s="20"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -2688,7 +2735,7 @@
       <c r="L31" s="20"/>
       <c r="M31" s="20"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -2725,7 +2772,7 @@
       <c r="L32" s="20"/>
       <c r="M32" s="20"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -2762,7 +2809,7 @@
       <c r="L33" s="20"/>
       <c r="M33" s="20"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -2797,7 +2844,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -2832,7 +2879,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -2865,7 +2912,7 @@
       </c>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -2900,7 +2947,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -2933,7 +2980,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -2968,7 +3015,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -2993,7 +3040,7 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -3017,7 +3064,7 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -3048,7 +3095,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -3083,7 +3130,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -3118,7 +3165,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -3151,7 +3198,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -3181,7 +3228,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -3211,7 +3258,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -3236,7 +3283,7 @@
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>24</v>
       </c>
@@ -3260,7 +3307,7 @@
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>22</v>
       </c>
@@ -3295,7 +3342,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>24</v>
       </c>
@@ -3327,7 +3374,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -3362,7 +3409,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>17</v>
       </c>
@@ -3384,7 +3431,7 @@
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>24</v>
       </c>
@@ -3408,7 +3455,7 @@
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>22</v>
       </c>
@@ -3443,7 +3490,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>17</v>
       </c>
@@ -3465,7 +3512,7 @@
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -3490,7 +3537,7 @@
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>24</v>
       </c>
@@ -3514,7 +3561,7 @@
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -3546,7 +3593,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -3578,7 +3625,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>17</v>
       </c>
@@ -3603,7 +3650,7 @@
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>17</v>
       </c>
@@ -3628,7 +3675,7 @@
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>24</v>
       </c>
@@ -3653,7 +3700,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="6"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>24</v>
       </c>
@@ -3685,7 +3732,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>17</v>
       </c>
@@ -3710,7 +3757,7 @@
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>17</v>
       </c>
@@ -3735,7 +3782,7 @@
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>24</v>
       </c>
@@ -3759,7 +3806,7 @@
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>24</v>
       </c>
@@ -3791,7 +3838,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>22</v>
       </c>
@@ -3826,7 +3873,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>22</v>
       </c>
@@ -3861,7 +3908,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>22</v>
       </c>
@@ -3896,7 +3943,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>73</v>
       </c>
@@ -3919,7 +3966,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -3942,7 +3989,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -3965,7 +4012,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -3988,7 +4035,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>73</v>
       </c>
@@ -4011,7 +4058,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>73</v>
       </c>
@@ -4034,7 +4081,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>73</v>
       </c>
@@ -4069,7 +4116,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>22</v>
       </c>
@@ -4102,7 +4149,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>22</v>
       </c>
@@ -4137,7 +4184,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>22</v>
       </c>
@@ -4172,7 +4219,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>22</v>
       </c>
@@ -4207,7 +4254,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>17</v>
       </c>
@@ -4232,7 +4279,7 @@
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>17</v>
       </c>
@@ -4257,7 +4304,7 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>24</v>
       </c>
@@ -4281,7 +4328,7 @@
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>22</v>
       </c>
@@ -4314,7 +4361,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>22</v>
       </c>
@@ -4349,7 +4396,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>22</v>
       </c>
@@ -4384,7 +4431,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>73</v>
       </c>
@@ -4408,7 +4455,7 @@
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="10" t="s">
         <v>22</v>
       </c>
@@ -4443,7 +4490,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>17</v>
       </c>
@@ -4468,7 +4515,7 @@
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>17</v>
       </c>
@@ -4493,7 +4540,7 @@
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>24</v>
       </c>
@@ -4517,7 +4564,7 @@
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>17</v>
       </c>
@@ -4542,7 +4589,7 @@
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>17</v>
       </c>
@@ -4567,7 +4614,7 @@
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="11" t="s">
         <v>24</v>
       </c>
@@ -4592,7 +4639,7 @@
       <c r="J96" s="18"/>
       <c r="K96" s="19"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>24</v>
       </c>
@@ -4624,370 +4671,432 @@
         <v>113</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E98" s="4"/>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E99" s="4"/>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>22</v>
+      </c>
+      <c r="B98" s="1">
+        <v>45626</v>
+      </c>
+      <c r="C98" t="s">
+        <v>289</v>
+      </c>
+      <c r="D98" s="1">
+        <v>45636</v>
+      </c>
+      <c r="E98" s="4">
+        <v>270.25</v>
+      </c>
+      <c r="F98" t="s">
+        <v>290</v>
+      </c>
+      <c r="G98" t="s">
+        <v>291</v>
+      </c>
+      <c r="H98" t="s">
+        <v>292</v>
+      </c>
+      <c r="I98">
+        <v>60071014</v>
+      </c>
+      <c r="J98" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K98" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>22</v>
+      </c>
+      <c r="B99" s="1">
+        <v>45633</v>
+      </c>
+      <c r="C99" t="s">
+        <v>293</v>
+      </c>
+      <c r="D99" s="1">
+        <v>45635</v>
+      </c>
+      <c r="E99" s="4">
+        <v>219</v>
+      </c>
+      <c r="F99" t="s">
+        <v>50</v>
+      </c>
+      <c r="G99" t="s">
+        <v>51</v>
+      </c>
+      <c r="H99" s="2"/>
+      <c r="I99" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="J99" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K99" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E100" s="4"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E101" s="4"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E102" s="4"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E103" s="4"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E104" s="4"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E105" s="4"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E106" s="4"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E107" s="4"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E108" s="4"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E109" s="4"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E110" s="4"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E111" s="4"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E112" s="4"/>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E113" s="4"/>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E114" s="4"/>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E115" s="4"/>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E116" s="4"/>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E117" s="4"/>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E118" s="4"/>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E119" s="4"/>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E120" s="4"/>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E121" s="4"/>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E122" s="4"/>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E123" s="4"/>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E124" s="4"/>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E125" s="4"/>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E126" s="4"/>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E127" s="4"/>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E128" s="4"/>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E129" s="4"/>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E130" s="4"/>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E131" s="4"/>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E132" s="4"/>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E133" s="4"/>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E134" s="4"/>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E135" s="4"/>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E136" s="4"/>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E137" s="4"/>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E138" s="4"/>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E139" s="4"/>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E140" s="4"/>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E141" s="4"/>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E142" s="4"/>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E143" s="4"/>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E144" s="4"/>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E145" s="4"/>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E146" s="4"/>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E147" s="4"/>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E148" s="4"/>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E149" s="4"/>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E150" s="4"/>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E151" s="4"/>
     </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E152" s="4"/>
     </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E153" s="4"/>
     </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E154" s="4"/>
     </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E155" s="4"/>
     </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E156" s="4"/>
     </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E157" s="4"/>
     </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E158" s="4"/>
     </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E159" s="4"/>
     </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E160" s="4"/>
     </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E161" s="4"/>
     </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E162" s="4"/>
     </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E163" s="4"/>
     </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E164" s="4"/>
     </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E165" s="4"/>
     </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E166" s="4"/>
     </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E167" s="4"/>
     </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E168" s="4"/>
     </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E169" s="4"/>
     </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E170" s="4"/>
     </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E171" s="4"/>
     </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E172" s="4"/>
     </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E173" s="4"/>
     </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E174" s="4"/>
     </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E175" s="4"/>
     </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E176" s="4"/>
     </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E177" s="4"/>
     </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E178" s="4"/>
     </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E179" s="4"/>
     </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E180" s="4"/>
     </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E181" s="4"/>
     </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E182" s="4"/>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E183" s="4"/>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E184" s="4"/>
     </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E185" s="4"/>
     </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E186" s="4"/>
     </row>
-    <row r="187" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E187" s="4"/>
     </row>
-    <row r="188" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E188" s="4"/>
     </row>
-    <row r="189" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E189" s="4"/>
     </row>
-    <row r="190" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E190" s="4"/>
     </row>
-    <row r="191" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E191" s="4"/>
     </row>
-    <row r="192" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E192" s="4"/>
     </row>
-    <row r="193" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E193" s="4"/>
     </row>
-    <row r="194" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E194" s="4"/>
     </row>
-    <row r="195" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E195" s="4"/>
     </row>
-    <row r="196" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E196" s="4"/>
     </row>
-    <row r="197" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E197" s="4"/>
     </row>
-    <row r="198" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E198" s="4"/>
     </row>
-    <row r="199" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E199" s="4"/>
     </row>
-    <row r="200" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E200" s="4"/>
     </row>
-    <row r="201" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E201" s="4"/>
     </row>
-    <row r="202" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E202" s="4"/>
     </row>
-    <row r="203" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E203" s="4"/>
     </row>
-    <row r="204" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E204" s="4"/>
     </row>
-    <row r="205" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E205" s="4"/>
     </row>
-    <row r="206" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E206" s="4"/>
     </row>
-    <row r="207" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E207" s="4"/>
     </row>
-    <row r="208" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E208" s="4"/>
     </row>
-    <row r="209" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E209" s="4"/>
     </row>
-    <row r="210" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E210" s="4"/>
     </row>
-    <row r="211" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E211" s="4"/>
     </row>
-    <row r="212" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E212" s="4"/>
     </row>
-    <row r="213" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E213" s="4"/>
     </row>
-    <row r="214" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E214" s="4"/>
     </row>
-    <row r="215" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E215" s="4"/>
     </row>
-    <row r="216" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E216" s="4"/>
     </row>
-    <row r="217" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E217" s="4"/>
     </row>
-    <row r="218" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E218" s="4"/>
     </row>
-    <row r="219" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E219" s="4"/>
     </row>
   </sheetData>
@@ -5028,47 +5137,47 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Spez Preisen Tabubrecherin und Weihnachten in der Schustergasse eingetragen
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72342951-B9C5-4BFC-A0C0-16A554A5B600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C535A7D-8F08-4495-A231-66FEE8D89E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2964" yWindow="1884" windowWidth="15684" windowHeight="11832" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E99" sqref="E99"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Film: WOW! Nachrichten aus dem All
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EF4C0F-868B-4969-B884-951DF176C004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B32A2D0-E17E-437B-9666-7E097CB21724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="313">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -931,15 +931,6 @@
     <t>241071TS</t>
   </si>
   <si>
-    <t>Kinomagie: Wow! Nachrichten aus dem All</t>
-  </si>
-  <si>
-    <t>Schule Menziken</t>
-  </si>
-  <si>
-    <t>Hauptstrasse 42a, 5737 Menziken</t>
-  </si>
-  <si>
     <t>Film: Der Buchspazierer</t>
   </si>
   <si>
@@ -977,6 +968,15 @@
   </si>
   <si>
     <t>29203</t>
+  </si>
+  <si>
+    <t>Film: WOW! Nachricht aus dem All</t>
+  </si>
+  <si>
+    <t>00 00000 00000 00000 00004 33744</t>
+  </si>
+  <si>
+    <t>00043374</t>
   </si>
 </sst>
 </file>
@@ -1159,8 +1159,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}" name="Table3" displayName="Table3" ref="A1:G17" totalsRowShown="0">
-  <autoFilter ref="A1:G17" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}" name="Table3" displayName="Table3" ref="A1:G18" totalsRowShown="0">
+  <autoFilter ref="A1:G18" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">
     <sortCondition ref="A1:A12"/>
   </sortState>
@@ -1178,8 +1178,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K103" totalsRowShown="0">
-  <autoFilter ref="A1:K103" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K104" totalsRowShown="0">
+  <autoFilter ref="A1:K104" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K96">
     <sortCondition ref="D1:D96"/>
   </sortState>
@@ -1510,10 +1510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1876,23 +1876,6 @@
       </c>
       <c r="G18" t="s">
         <v>296</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>297</v>
-      </c>
-      <c r="C19" s="5">
-        <v>45638</v>
-      </c>
-      <c r="D19" s="4">
-        <v>770</v>
-      </c>
-      <c r="E19" t="s">
-        <v>298</v>
-      </c>
-      <c r="F19" t="s">
-        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -1919,8 +1902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100:XFD100"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1930,7 +1913,7 @@
     <col min="3" max="3" width="45.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
     <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
@@ -4812,7 +4795,7 @@
         <v>45646</v>
       </c>
       <c r="C100" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D100" s="1">
         <v>45650</v>
@@ -4827,10 +4810,10 @@
         <v>62</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="J100" s="2" t="s">
         <v>90</v>
@@ -4844,7 +4827,7 @@
         <v>15</v>
       </c>
       <c r="C101" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D101" s="1">
         <v>45638</v>
@@ -4859,10 +4842,10 @@
         <v>30</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="I101" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="J101" s="6" t="s">
         <v>111</v>
@@ -4879,7 +4862,7 @@
         <v>45646</v>
       </c>
       <c r="C102" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D102" s="1">
         <v>45647</v>
@@ -4894,10 +4877,10 @@
         <v>223</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="I102" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="J102" s="2" t="s">
         <v>90</v>
@@ -4914,7 +4897,7 @@
         <v>45604</v>
       </c>
       <c r="C103" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D103" s="1">
         <v>45615</v>
@@ -4923,14 +4906,14 @@
         <v>101.12</v>
       </c>
       <c r="F103" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G103" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="H103" s="2"/>
       <c r="I103" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="J103" s="2" t="s">
         <v>90</v>
@@ -4940,7 +4923,39 @@
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E104" s="4"/>
+      <c r="A104" t="s">
+        <v>22</v>
+      </c>
+      <c r="B104" s="1">
+        <v>45638</v>
+      </c>
+      <c r="C104" t="s">
+        <v>310</v>
+      </c>
+      <c r="D104" s="1">
+        <v>45653</v>
+      </c>
+      <c r="E104" s="4">
+        <v>262.25</v>
+      </c>
+      <c r="F104" t="s">
+        <v>185</v>
+      </c>
+      <c r="G104" t="s">
+        <v>186</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K104" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E105" s="4"/>

</xml_diff>

<commit_message>
Rechnungen Garfield & Tabubrecherin eingetragen Angaben Förderer eingetragen
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE686B4C-93D2-471F-A666-231744C1B192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF29D95-3F90-446F-9199-93116608897A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="15036" yWindow="3240" windowWidth="15684" windowHeight="11832" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="324">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -977,6 +977,39 @@
   </si>
   <si>
     <t>00043374</t>
+  </si>
+  <si>
+    <t>Film: Garfield</t>
+  </si>
+  <si>
+    <t>Sony Pictures Releasing Switzerland GmbH</t>
+  </si>
+  <si>
+    <t>275862000000000000030626311</t>
+  </si>
+  <si>
+    <t>3062631</t>
+  </si>
+  <si>
+    <t>Förderer Kino</t>
+  </si>
+  <si>
+    <t>Theater am Bahnhof</t>
+  </si>
+  <si>
+    <t>Förderer Firmen Kino</t>
+  </si>
+  <si>
+    <t>Förderer TaB nur Kino-Anteil</t>
+  </si>
+  <si>
+    <t>Film: Tabubrecherin</t>
+  </si>
+  <si>
+    <t>langjahr film GmbH</t>
+  </si>
+  <si>
+    <t>Bahnhofstrasse 7, Zug</t>
   </si>
 </sst>
 </file>
@@ -1114,8 +1147,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{27287C1A-B7AC-49C2-89D9-0074BB2DB80A}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -1159,8 +1192,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}" name="Table3" displayName="Table3" ref="A1:G18" totalsRowShown="0">
-  <autoFilter ref="A1:G18" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}" name="Table3" displayName="Table3" ref="A1:G21" totalsRowShown="0">
+  <autoFilter ref="A1:G21" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">
     <sortCondition ref="A1:A12"/>
   </sortState>
@@ -1178,8 +1211,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K104" totalsRowShown="0">
-  <autoFilter ref="A1:K104" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K106" totalsRowShown="0">
+  <autoFilter ref="A1:K106" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K104">
     <sortCondition ref="D1:D104"/>
   </sortState>
@@ -1214,9 +1247,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1254,7 +1287,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1360,7 +1393,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1510,24 +1543,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.42578125" customWidth="1"/>
+    <col min="7" max="7" width="42.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1550,7 +1583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1570,7 +1603,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -1587,7 +1620,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1604,7 +1637,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -1621,7 +1654,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -1638,7 +1671,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1655,7 +1688,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1672,7 +1705,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1695,7 +1728,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1718,7 +1751,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1741,7 +1774,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1761,7 +1794,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1784,7 +1817,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1804,7 +1837,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1821,7 +1854,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1838,7 +1871,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1855,7 +1888,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1876,6 +1909,57 @@
       </c>
       <c r="G18" t="s">
         <v>296</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>317</v>
+      </c>
+      <c r="C19" s="5">
+        <v>45657</v>
+      </c>
+      <c r="D19" s="4">
+        <v>12800</v>
+      </c>
+      <c r="E19" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>319</v>
+      </c>
+      <c r="C20" s="5">
+        <v>45657</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1750</v>
+      </c>
+      <c r="E20" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>320</v>
+      </c>
+      <c r="C21" s="5">
+        <v>45657</v>
+      </c>
+      <c r="D21" s="4">
+        <v>3306</v>
+      </c>
+      <c r="E21" t="s">
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -1902,26 +1986,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M218"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C120" sqref="C120"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1956,7 +2040,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1982,7 +2066,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -2009,7 +2093,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -2038,7 +2122,7 @@
       <c r="L4" s="20"/>
       <c r="M4" s="20"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -2069,7 +2153,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -2093,7 +2177,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2117,7 +2201,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -2142,7 +2226,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -2166,7 +2250,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -2190,7 +2274,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -2221,7 +2305,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -2244,7 +2328,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -2268,7 +2352,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -2299,7 +2383,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -2327,7 +2411,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -2358,7 +2442,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2386,7 +2470,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2414,7 +2498,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -2435,7 +2519,7 @@
       </c>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -2466,7 +2550,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -2490,7 +2574,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2521,7 +2605,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -2546,7 +2630,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2570,7 +2654,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2602,7 +2686,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>73</v>
       </c>
@@ -2626,7 +2710,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -2653,7 +2737,7 @@
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2679,7 +2763,7 @@
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -2713,7 +2797,7 @@
       <c r="L29" s="20"/>
       <c r="M29" s="20"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -2750,7 +2834,7 @@
       <c r="L30" s="20"/>
       <c r="M30" s="20"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -2787,7 +2871,7 @@
       <c r="L31" s="20"/>
       <c r="M31" s="20"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -2824,7 +2908,7 @@
       <c r="L32" s="20"/>
       <c r="M32" s="20"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -2861,7 +2945,7 @@
       <c r="L33" s="20"/>
       <c r="M33" s="20"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -2896,7 +2980,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -2927,7 +3011,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -2960,7 +3044,7 @@
       </c>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -2995,7 +3079,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -3028,7 +3112,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -3063,7 +3147,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -3088,7 +3172,7 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -3112,7 +3196,7 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -3143,7 +3227,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -3178,7 +3262,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -3213,7 +3297,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -3246,7 +3330,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -3276,7 +3360,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -3306,7 +3390,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -3331,7 +3415,7 @@
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>24</v>
       </c>
@@ -3355,7 +3439,7 @@
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>22</v>
       </c>
@@ -3390,7 +3474,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>24</v>
       </c>
@@ -3422,7 +3506,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -3457,7 +3541,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>17</v>
       </c>
@@ -3479,7 +3563,7 @@
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>24</v>
       </c>
@@ -3503,7 +3587,7 @@
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>22</v>
       </c>
@@ -3538,7 +3622,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>17</v>
       </c>
@@ -3560,7 +3644,7 @@
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -3585,7 +3669,7 @@
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>24</v>
       </c>
@@ -3609,7 +3693,7 @@
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -3641,7 +3725,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -3673,7 +3757,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>17</v>
       </c>
@@ -3698,7 +3782,7 @@
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>17</v>
       </c>
@@ -3723,7 +3807,7 @@
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>24</v>
       </c>
@@ -3748,7 +3832,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="6"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>24</v>
       </c>
@@ -3780,7 +3864,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>17</v>
       </c>
@@ -3805,7 +3889,7 @@
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>17</v>
       </c>
@@ -3830,7 +3914,7 @@
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>24</v>
       </c>
@@ -3854,7 +3938,7 @@
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>22</v>
       </c>
@@ -3889,7 +3973,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>24</v>
       </c>
@@ -3921,7 +4005,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>22</v>
       </c>
@@ -3956,7 +4040,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>22</v>
       </c>
@@ -3991,7 +4075,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>73</v>
       </c>
@@ -4014,7 +4098,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -4037,7 +4121,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -4060,7 +4144,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -4083,7 +4167,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>73</v>
       </c>
@@ -4106,7 +4190,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>73</v>
       </c>
@@ -4129,7 +4213,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>73</v>
       </c>
@@ -4164,7 +4248,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>22</v>
       </c>
@@ -4199,7 +4283,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>22</v>
       </c>
@@ -4232,7 +4316,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>22</v>
       </c>
@@ -4267,7 +4351,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>22</v>
       </c>
@@ -4302,7 +4386,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>17</v>
       </c>
@@ -4327,7 +4411,7 @@
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>17</v>
       </c>
@@ -4352,7 +4436,7 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>24</v>
       </c>
@@ -4376,7 +4460,7 @@
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>22</v>
       </c>
@@ -4409,7 +4493,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>22</v>
       </c>
@@ -4444,7 +4528,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>22</v>
       </c>
@@ -4479,7 +4563,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>73</v>
       </c>
@@ -4503,7 +4587,7 @@
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="10" t="s">
         <v>22</v>
       </c>
@@ -4538,7 +4622,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>22</v>
       </c>
@@ -4571,7 +4655,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>24</v>
       </c>
@@ -4603,7 +4687,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>17</v>
       </c>
@@ -4628,7 +4712,7 @@
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>17</v>
       </c>
@@ -4653,7 +4737,7 @@
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>24</v>
       </c>
@@ -4677,7 +4761,7 @@
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="11" t="s">
         <v>22</v>
       </c>
@@ -4710,7 +4794,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>22</v>
       </c>
@@ -4745,7 +4829,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>15</v>
       </c>
@@ -4777,7 +4861,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>73</v>
       </c>
@@ -4812,7 +4896,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>22</v>
       </c>
@@ -4847,7 +4931,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>17</v>
       </c>
@@ -4872,7 +4956,7 @@
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>17</v>
       </c>
@@ -4897,7 +4981,7 @@
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>24</v>
       </c>
@@ -4921,7 +5005,7 @@
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>22</v>
       </c>
@@ -4956,346 +5040,406 @@
         <v>113</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E105" s="4"/>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E106" s="4"/>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>22</v>
+      </c>
+      <c r="B105" s="1">
+        <v>45543</v>
+      </c>
+      <c r="C105" t="s">
+        <v>313</v>
+      </c>
+      <c r="D105" s="1">
+        <v>45614</v>
+      </c>
+      <c r="E105" s="4">
+        <v>86.75</v>
+      </c>
+      <c r="F105" t="s">
+        <v>314</v>
+      </c>
+      <c r="G105" t="s">
+        <v>43</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="J105" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K105" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>22</v>
+      </c>
+      <c r="B106" s="1">
+        <v>45634</v>
+      </c>
+      <c r="C106" t="s">
+        <v>321</v>
+      </c>
+      <c r="D106" s="1">
+        <v>45665</v>
+      </c>
+      <c r="E106" s="4">
+        <v>172.25</v>
+      </c>
+      <c r="F106" t="s">
+        <v>322</v>
+      </c>
+      <c r="G106" t="s">
+        <v>323</v>
+      </c>
+      <c r="H106" s="2"/>
+      <c r="I106" s="2"/>
+      <c r="J106" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K106" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E107" s="4"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E108" s="4"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E109" s="4"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E110" s="4"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E111" s="4"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E112" s="4"/>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E113" s="4"/>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E114" s="4"/>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E115" s="4"/>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E116" s="4"/>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E117" s="4"/>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E118" s="4"/>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E119" s="4"/>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E120" s="4"/>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E121" s="4"/>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E122" s="4"/>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E123" s="4"/>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E124" s="4"/>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E125" s="4"/>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E126" s="4"/>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E127" s="4"/>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E128" s="4"/>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E129" s="4"/>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E130" s="4"/>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E131" s="4"/>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E132" s="4"/>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E133" s="4"/>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E134" s="4"/>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E135" s="4"/>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E136" s="4"/>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E137" s="4"/>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E138" s="4"/>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E139" s="4"/>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E140" s="4"/>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E141" s="4"/>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E142" s="4"/>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E143" s="4"/>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E144" s="4"/>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E145" s="4"/>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E146" s="4"/>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E147" s="4"/>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E148" s="4"/>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E149" s="4"/>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E150" s="4"/>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E151" s="4"/>
     </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E152" s="4"/>
     </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E153" s="4"/>
     </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E154" s="4"/>
     </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E155" s="4"/>
     </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E156" s="4"/>
     </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E157" s="4"/>
     </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E158" s="4"/>
     </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E159" s="4"/>
     </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E160" s="4"/>
     </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E161" s="4"/>
     </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E162" s="4"/>
     </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E163" s="4"/>
     </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E164" s="4"/>
     </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E165" s="4"/>
     </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E166" s="4"/>
     </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E167" s="4"/>
     </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E168" s="4"/>
     </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E169" s="4"/>
     </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E170" s="4"/>
     </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E171" s="4"/>
     </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E172" s="4"/>
     </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E173" s="4"/>
     </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E174" s="4"/>
     </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E175" s="4"/>
     </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E176" s="4"/>
     </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E177" s="4"/>
     </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E178" s="4"/>
     </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E179" s="4"/>
     </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E180" s="4"/>
     </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E181" s="4"/>
     </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E182" s="4"/>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E183" s="4"/>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E184" s="4"/>
     </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E185" s="4"/>
     </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E186" s="4"/>
     </row>
-    <row r="187" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E187" s="4"/>
     </row>
-    <row r="188" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E188" s="4"/>
     </row>
-    <row r="189" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E189" s="4"/>
     </row>
-    <row r="190" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E190" s="4"/>
     </row>
-    <row r="191" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E191" s="4"/>
     </row>
-    <row r="192" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E192" s="4"/>
     </row>
-    <row r="193" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E193" s="4"/>
     </row>
-    <row r="194" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E194" s="4"/>
     </row>
-    <row r="195" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E195" s="4"/>
     </row>
-    <row r="196" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E196" s="4"/>
     </row>
-    <row r="197" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E197" s="4"/>
     </row>
-    <row r="198" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E198" s="4"/>
     </row>
-    <row r="199" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E199" s="4"/>
     </row>
-    <row r="200" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E200" s="4"/>
     </row>
-    <row r="201" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E201" s="4"/>
     </row>
-    <row r="202" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E202" s="4"/>
     </row>
-    <row r="203" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E203" s="4"/>
     </row>
-    <row r="204" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E204" s="4"/>
     </row>
-    <row r="205" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E205" s="4"/>
     </row>
-    <row r="206" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E206" s="4"/>
     </row>
-    <row r="207" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E207" s="4"/>
     </row>
-    <row r="208" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E208" s="4"/>
     </row>
-    <row r="209" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E209" s="4"/>
     </row>
-    <row r="210" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E210" s="4"/>
     </row>
-    <row r="211" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E211" s="4"/>
     </row>
-    <row r="212" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E212" s="4"/>
     </row>
-    <row r="213" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E213" s="4"/>
     </row>
-    <row r="214" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E214" s="4"/>
     </row>
-    <row r="215" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E215" s="4"/>
     </row>
-    <row r="216" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E216" s="4"/>
     </row>
-    <row r="217" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E217" s="4"/>
     </row>
-    <row r="218" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E218" s="4"/>
     </row>
   </sheetData>
@@ -5336,47 +5480,47 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Rechnungen Garfield & Tabubrecherin, Föderer Einnahmen bis ende 2024
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF29D95-3F90-446F-9199-93116608897A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B138FD-F247-4613-9B1E-8326E01DB88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15036" yWindow="3240" windowWidth="15684" windowHeight="11832" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -1986,7 +1986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ferienspass 8.8.24 eingetragen Rechnung Kalbermatten
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5DD46E-E1C8-4506-8E4E-C422013F5D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1122B7-2BDB-41A0-AF3E-457488843247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="2268" yWindow="2268" windowWidth="15684" windowHeight="11832" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="334">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -1027,10 +1027,19 @@
     <t>Popcornschaufel</t>
   </si>
   <si>
-    <t>Thabo: Tierkekse</t>
-  </si>
-  <si>
     <t>Kaffeemaschinenreiniger</t>
+  </si>
+  <si>
+    <t>Leibniz Kekse Dschungel</t>
+  </si>
+  <si>
+    <t>Kioskeinkauf</t>
+  </si>
+  <si>
+    <t>Film: Kalbermatten</t>
+  </si>
+  <si>
+    <t>MovieBiz Films</t>
   </si>
 </sst>
 </file>
@@ -1232,10 +1241,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K111" totalsRowShown="0">
-  <autoFilter ref="A1:K111" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K104">
-    <sortCondition ref="D1:D104"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K118" totalsRowShown="0">
+  <autoFilter ref="A1:K118" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K111">
+    <sortCondition ref="B1:B111"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="9" xr3:uid="{7720D0EA-5763-4F4F-82DA-8D34884933A7}" name="Kategorie"/>
@@ -2007,8 +2016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2063,29 +2072,32 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>73</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45311</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1">
-        <v>44895</v>
+        <v>45311</v>
       </c>
       <c r="E2" s="4">
-        <v>15.75</v>
+        <v>70.650000000000006</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="H2" s="2"/>
-      <c r="I2" s="2">
-        <v>42491</v>
-      </c>
+      <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -2095,19 +2107,19 @@
         <v>45311</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="D3" s="1">
         <v>45311</v>
       </c>
       <c r="E3" s="4">
-        <v>75.849999999999994</v>
+        <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -2116,28 +2128,32 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1">
         <v>45311</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D4" s="1">
-        <v>45311</v>
+        <v>45330</v>
       </c>
       <c r="E4" s="4">
-        <v>60</v>
+        <v>423.5</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="20"/>
@@ -2176,259 +2192,284 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45312</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="D6" s="1">
-        <v>45316</v>
+        <v>45329</v>
       </c>
       <c r="E6" s="4">
-        <v>34.5</v>
+        <v>276.3</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45316</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="D7" s="1">
-        <v>45316</v>
+        <v>45321</v>
       </c>
       <c r="E7" s="4">
-        <v>32.700000000000003</v>
+        <v>194.6</v>
       </c>
       <c r="F7" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="G7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>73</v>
+      </c>
+      <c r="B8" s="5">
+        <v>45319</v>
       </c>
       <c r="C8" t="s">
-        <v>282</v>
-      </c>
-      <c r="D8" s="1">
-        <v>45316</v>
+        <v>26</v>
+      </c>
+      <c r="D8" s="5">
+        <v>45319</v>
       </c>
       <c r="E8" s="4">
-        <f>1140*1.1</f>
-        <v>1254</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="K8" s="2" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45319</v>
       </c>
       <c r="C9" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="D9" s="1">
-        <v>45316</v>
+        <v>45421</v>
       </c>
       <c r="E9" s="4">
-        <v>1200</v>
+        <v>179.08</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>146</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>147</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="J9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="5">
-        <v>45319</v>
+      <c r="B10" s="1">
+        <v>45332</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="5">
-        <v>45319</v>
+        <v>177</v>
+      </c>
+      <c r="D10" s="1">
+        <v>45332</v>
       </c>
       <c r="E10" s="4">
-        <v>24</v>
+        <v>37.25</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+        <v>177</v>
+      </c>
+      <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="1">
-        <v>45316</v>
+        <v>45332</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D11" s="1">
-        <v>45321</v>
+        <v>45343</v>
       </c>
       <c r="E11" s="4">
-        <v>194.6</v>
+        <v>417.7</v>
       </c>
       <c r="F11" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45333</v>
       </c>
       <c r="C12" t="s">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="D12" s="1">
-        <v>45322</v>
+        <v>45337</v>
       </c>
       <c r="E12" s="4">
-        <v>276</v>
+        <v>192.45</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>112</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="G12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" t="s">
+        <v>63</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1">
-        <v>45340</v>
+        <v>45339</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="D13" s="1">
-        <v>45323</v>
+        <v>45392</v>
       </c>
       <c r="E13" s="4">
-        <v>400</v>
+        <v>461.95</v>
       </c>
       <c r="F13" t="s">
-        <v>68</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="G13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B14" s="1">
-        <v>45312</v>
+        <v>45340</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D14" s="1">
-        <v>45329</v>
+        <v>45323</v>
       </c>
       <c r="E14" s="4">
-        <v>276.3</v>
+        <v>400</v>
       </c>
       <c r="F14" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" t="s">
-        <v>43</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45340</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="D15" s="1">
-        <v>45329</v>
+        <v>45341</v>
       </c>
       <c r="E15" s="4">
-        <v>35.049999999999997</v>
+        <v>1000</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>48</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
@@ -2437,124 +2478,147 @@
         <v>22</v>
       </c>
       <c r="B16" s="1">
-        <v>45311</v>
+        <v>45344</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="D16" s="1">
-        <v>45330</v>
+        <v>45387</v>
       </c>
       <c r="E16" s="4">
-        <v>423.5</v>
+        <v>205.4</v>
       </c>
       <c r="F16" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="G16" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>73</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45354</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D17" s="1">
-        <v>45330</v>
+        <v>45354</v>
       </c>
       <c r="E17" s="4">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
+      <c r="K17" s="2" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45354</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="D18" s="1">
-        <v>45331</v>
+        <v>45387</v>
       </c>
       <c r="E18" s="4">
-        <v>101</v>
+        <v>137.9</v>
       </c>
       <c r="F18" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="G18" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1">
-        <v>45332</v>
+        <v>45358</v>
       </c>
       <c r="C19" t="s">
-        <v>177</v>
+        <v>100</v>
       </c>
       <c r="D19" s="1">
-        <v>45332</v>
+        <v>45387</v>
       </c>
       <c r="E19" s="4">
-        <v>37.25</v>
+        <v>104</v>
       </c>
       <c r="F19" t="s">
-        <v>177</v>
-      </c>
-      <c r="K19" s="6"/>
+        <v>61</v>
+      </c>
+      <c r="G19" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="1">
-        <v>45333</v>
+        <v>45368</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="D20" s="1">
-        <v>45337</v>
+        <v>45387</v>
       </c>
       <c r="E20" s="4">
-        <v>192.45</v>
+        <v>178.35</v>
       </c>
       <c r="F20" t="s">
         <v>61</v>
@@ -2562,143 +2626,169 @@
       <c r="G20" t="s">
         <v>62</v>
       </c>
-      <c r="H20" t="s">
-        <v>63</v>
+      <c r="H20" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
+        <v>93</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="1">
-        <v>45340</v>
+        <v>45371</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>140</v>
       </c>
       <c r="D21" s="1">
-        <v>45341</v>
+        <v>45422</v>
       </c>
       <c r="E21" s="4">
-        <v>1000</v>
+        <v>162.15</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
-      </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="G21" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B22" s="1">
-        <v>45332</v>
+        <v>45371</v>
       </c>
       <c r="C22" t="s">
-        <v>74</v>
+        <v>324</v>
       </c>
       <c r="D22" s="1">
-        <v>45343</v>
+        <v>45323</v>
       </c>
       <c r="E22" s="4">
-        <v>417.7</v>
+        <v>12.9</v>
       </c>
       <c r="F22" t="s">
-        <v>75</v>
-      </c>
-      <c r="G22" t="s">
-        <v>76</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>78</v>
-      </c>
+        <v>325</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
+      <c r="K22" s="2" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>45383</v>
       </c>
       <c r="C23" t="s">
-        <v>281</v>
+        <v>118</v>
       </c>
       <c r="D23" s="1">
-        <v>45347</v>
+        <v>45394</v>
       </c>
       <c r="E23" s="4">
-        <f>1140*1.1</f>
-        <v>1254</v>
+        <v>211.9</v>
       </c>
       <c r="F23" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="G23" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>73</v>
+      </c>
+      <c r="B24" s="1">
+        <v>45383</v>
       </c>
       <c r="C24" t="s">
-        <v>133</v>
+        <v>330</v>
       </c>
       <c r="D24" s="1">
-        <v>45347</v>
+        <v>45330</v>
       </c>
       <c r="E24" s="4">
-        <v>1200</v>
+        <f>36.16-11.6</f>
+        <v>24.559999999999995</v>
       </c>
       <c r="F24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" t="s">
-        <v>56</v>
+        <v>327</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
+      <c r="K24" s="2" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45386</v>
       </c>
       <c r="C25" t="s">
-        <v>173</v>
+        <v>94</v>
       </c>
       <c r="D25" s="1">
-        <v>45352</v>
+        <v>45387</v>
       </c>
       <c r="E25" s="4">
-        <v>51.45</v>
+        <v>139.75</v>
       </c>
       <c r="F25" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="G25" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>169</v>
+        <v>95</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>170</v>
+        <v>96</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>90</v>
@@ -2709,105 +2799,138 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="B26" s="1">
-        <v>45354</v>
+        <v>45400</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>143</v>
       </c>
       <c r="D26" s="1">
-        <v>45354</v>
+        <v>45400</v>
       </c>
       <c r="E26" s="4">
-        <v>10</v>
+        <v>211.85</v>
       </c>
       <c r="F26" t="s">
-        <v>79</v>
+        <v>50</v>
+      </c>
+      <c r="G26" t="s">
+        <v>51</v>
       </c>
       <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
+      <c r="I26" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="B27" s="1">
+        <v>45403</v>
       </c>
       <c r="C27" t="s">
-        <v>280</v>
+        <v>121</v>
       </c>
       <c r="D27" s="1">
-        <v>45376</v>
+        <v>45403</v>
       </c>
       <c r="E27" s="4">
-        <f>1140*1.1</f>
-        <v>1254</v>
+        <v>447.55</v>
       </c>
       <c r="F27" t="s">
-        <v>7</v>
+        <v>123</v>
       </c>
       <c r="G27" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
+        <v>124</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B28" s="1">
+        <v>45412</v>
       </c>
       <c r="C28" t="s">
-        <v>134</v>
+        <v>181</v>
       </c>
       <c r="D28" s="1">
-        <v>45376</v>
+        <v>45460</v>
       </c>
       <c r="E28" s="4">
-        <v>1200</v>
+        <v>214</v>
       </c>
       <c r="F28" t="s">
-        <v>11</v>
+        <v>178</v>
       </c>
       <c r="G28" t="s">
-        <v>56</v>
-      </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
+        <v>182</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B29" s="1">
+        <v>45415</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="D29" s="1">
-        <v>45376</v>
+        <v>45426</v>
       </c>
       <c r="E29" s="4">
-        <v>25.1</v>
+        <v>137.9</v>
       </c>
       <c r="F29" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="G29" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>82</v>
+        <v>138</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>83</v>
+        <v>139</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>90</v>
@@ -2823,29 +2946,25 @@
         <v>22</v>
       </c>
       <c r="B30" s="1">
-        <v>45344</v>
+        <v>45418</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
+        <v>126</v>
       </c>
       <c r="D30" s="1">
         <v>45387</v>
       </c>
       <c r="E30" s="4">
-        <v>205.4</v>
+        <v>170</v>
       </c>
       <c r="F30" t="s">
-        <v>85</v>
+        <v>127</v>
       </c>
       <c r="G30" t="s">
-        <v>86</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>88</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
       <c r="J30" s="2" t="s">
         <v>90</v>
       </c>
@@ -2860,28 +2979,26 @@
         <v>22</v>
       </c>
       <c r="B31" s="1">
-        <v>45354</v>
+        <v>45431</v>
       </c>
       <c r="C31" t="s">
-        <v>97</v>
+        <v>148</v>
       </c>
       <c r="D31" s="1">
-        <v>45387</v>
+        <v>45435</v>
       </c>
       <c r="E31" s="4">
-        <v>137.9</v>
+        <v>227.55</v>
       </c>
       <c r="F31" t="s">
-        <v>61</v>
+        <v>149</v>
       </c>
       <c r="G31" t="s">
-        <v>62</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>98</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="H31" s="2"/>
       <c r="I31" s="2" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>90</v>
@@ -2897,28 +3014,28 @@
         <v>22</v>
       </c>
       <c r="B32" s="1">
-        <v>45358</v>
+        <v>45435</v>
       </c>
       <c r="C32" t="s">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="D32" s="1">
-        <v>45387</v>
+        <v>45439</v>
       </c>
       <c r="E32" s="4">
-        <v>104</v>
+        <v>253.55</v>
       </c>
       <c r="F32" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="G32" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>101</v>
+        <v>154</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>90</v>
@@ -2934,28 +3051,28 @@
         <v>22</v>
       </c>
       <c r="B33" s="1">
-        <v>45368</v>
+        <v>45438</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>184</v>
       </c>
       <c r="D33" s="1">
-        <v>45387</v>
+        <v>45475</v>
       </c>
       <c r="E33" s="4">
-        <v>178.35</v>
+        <v>174.6</v>
       </c>
       <c r="F33" t="s">
-        <v>61</v>
+        <v>185</v>
       </c>
       <c r="G33" t="s">
-        <v>62</v>
+        <v>186</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>92</v>
+        <v>187</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>93</v>
+        <v>188</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>90</v>
@@ -2971,28 +3088,28 @@
         <v>22</v>
       </c>
       <c r="B34" s="1">
-        <v>45386</v>
+        <v>45543</v>
       </c>
       <c r="C34" t="s">
-        <v>94</v>
+        <v>313</v>
       </c>
       <c r="D34" s="1">
-        <v>45387</v>
+        <v>45614</v>
       </c>
       <c r="E34" s="4">
-        <v>139.75</v>
+        <v>86.75</v>
       </c>
       <c r="F34" t="s">
-        <v>61</v>
+        <v>314</v>
       </c>
       <c r="G34" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>95</v>
+        <v>315</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>96</v>
+        <v>316</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>90</v>
@@ -3006,25 +3123,29 @@
         <v>22</v>
       </c>
       <c r="B35" s="1">
-        <v>45418</v>
+        <v>45555</v>
       </c>
       <c r="C35" t="s">
-        <v>126</v>
+        <v>189</v>
       </c>
       <c r="D35" s="1">
-        <v>45387</v>
+        <v>45562</v>
       </c>
       <c r="E35" s="4">
-        <v>170</v>
+        <v>180.9</v>
       </c>
       <c r="F35" t="s">
-        <v>127</v>
+        <v>61</v>
       </c>
       <c r="G35" t="s">
-        <v>128</v>
-      </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>191</v>
+      </c>
       <c r="J35" s="2" t="s">
         <v>90</v>
       </c>
@@ -3037,49 +3158,51 @@
         <v>22</v>
       </c>
       <c r="B36" s="1">
-        <v>45339</v>
+        <v>45557</v>
       </c>
       <c r="C36" t="s">
-        <v>114</v>
+        <v>192</v>
       </c>
       <c r="D36" s="1">
-        <v>45392</v>
+        <v>45566</v>
       </c>
       <c r="E36" s="4">
-        <v>461.95</v>
+        <v>178.35</v>
       </c>
       <c r="F36" t="s">
-        <v>75</v>
+        <v>185</v>
       </c>
       <c r="G36" t="s">
-        <v>76</v>
+        <v>186</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>115</v>
+        <v>193</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>116</v>
+        <v>194</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="K36" s="2"/>
+      <c r="K36" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>22</v>
       </c>
       <c r="B37" s="1">
-        <v>45383</v>
+        <v>45562</v>
       </c>
       <c r="C37" t="s">
-        <v>118</v>
+        <v>213</v>
       </c>
       <c r="D37" s="1">
-        <v>45394</v>
+        <v>45568</v>
       </c>
       <c r="E37" s="4">
-        <v>211.9</v>
+        <v>88.85</v>
       </c>
       <c r="F37" t="s">
         <v>61</v>
@@ -3088,10 +3211,10 @@
         <v>62</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>119</v>
+        <v>214</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>120</v>
+        <v>215</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>90</v>
@@ -3105,26 +3228,28 @@
         <v>22</v>
       </c>
       <c r="B38" s="1">
-        <v>45400</v>
+        <v>45571</v>
       </c>
       <c r="C38" t="s">
-        <v>143</v>
+        <v>240</v>
       </c>
       <c r="D38" s="1">
-        <v>45400</v>
+        <v>45588</v>
       </c>
       <c r="E38" s="4">
-        <v>211.85</v>
+        <v>181.6</v>
       </c>
       <c r="F38" t="s">
-        <v>50</v>
+        <v>178</v>
       </c>
       <c r="G38" t="s">
-        <v>51</v>
-      </c>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2" t="s">
-        <v>144</v>
+        <v>182</v>
+      </c>
+      <c r="H38" t="s">
+        <v>241</v>
+      </c>
+      <c r="I38" s="2">
+        <v>10053082</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>90</v>
@@ -3135,187 +3260,152 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B39" s="1">
-        <v>45403</v>
+        <v>45576</v>
       </c>
       <c r="C39" t="s">
-        <v>121</v>
+        <v>216</v>
       </c>
       <c r="D39" s="1">
-        <v>45403</v>
+        <v>45576</v>
       </c>
       <c r="E39" s="4">
-        <v>447.55</v>
-      </c>
-      <c r="F39" t="s">
-        <v>123</v>
-      </c>
-      <c r="G39" t="s">
-        <v>124</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>90</v>
-      </c>
+        <v>37.700000000000003</v>
+      </c>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
       <c r="K39" s="2" t="s">
-        <v>113</v>
+        <v>226</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>73</v>
+      </c>
+      <c r="B40" s="1">
+        <v>45576</v>
       </c>
       <c r="C40" t="s">
-        <v>265</v>
+        <v>217</v>
       </c>
       <c r="D40" s="1">
-        <v>45407</v>
+        <v>45576</v>
       </c>
       <c r="E40" s="4">
-        <f>1140*1.1</f>
-        <v>1254</v>
-      </c>
-      <c r="F40" t="s">
-        <v>7</v>
-      </c>
-      <c r="G40" t="s">
-        <v>8</v>
+        <v>116.1</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
+      <c r="K40" s="2" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>24</v>
-      </c>
-      <c r="C41" t="s">
-        <v>135</v>
+        <v>73</v>
+      </c>
+      <c r="B41" s="1">
+        <v>45576</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>219</v>
       </c>
       <c r="D41" s="1">
-        <v>45407</v>
+        <v>45576</v>
       </c>
       <c r="E41" s="4">
-        <v>1200</v>
-      </c>
-      <c r="F41" t="s">
-        <v>11</v>
-      </c>
-      <c r="G41" t="s">
-        <v>56</v>
+        <v>154.80000000000001</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
+      <c r="K41" s="2" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B42" s="1">
-        <v>45319</v>
-      </c>
-      <c r="C42" t="s">
-        <v>145</v>
+        <v>45576</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>218</v>
       </c>
       <c r="D42" s="1">
-        <v>45421</v>
+        <v>45576</v>
       </c>
       <c r="E42" s="4">
-        <v>179.08</v>
-      </c>
-      <c r="F42" t="s">
-        <v>146</v>
-      </c>
-      <c r="G42" t="s">
-        <v>147</v>
+        <v>102.2</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
-      <c r="J42" s="2" t="s">
-        <v>90</v>
-      </c>
+      <c r="J42" s="2"/>
       <c r="K42" s="2" t="s">
-        <v>113</v>
+        <v>226</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B43" s="1">
-        <v>45371</v>
+        <v>45576</v>
       </c>
       <c r="C43" t="s">
-        <v>140</v>
+        <v>254</v>
       </c>
       <c r="D43" s="1">
-        <v>45422</v>
+        <v>45576</v>
       </c>
       <c r="E43" s="4">
-        <v>162.15</v>
-      </c>
-      <c r="F43" t="s">
-        <v>75</v>
-      </c>
-      <c r="G43" t="s">
-        <v>76</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>90</v>
-      </c>
+        <v>30.7</v>
+      </c>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
       <c r="K43" s="2" t="s">
-        <v>113</v>
+        <v>226</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B44" s="1">
-        <v>45415</v>
-      </c>
-      <c r="C44" t="s">
-        <v>137</v>
+        <v>45576</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>221</v>
       </c>
       <c r="D44" s="1">
-        <v>45426</v>
+        <v>45579</v>
       </c>
       <c r="E44" s="4">
-        <v>137.9</v>
+        <v>279.89999999999998</v>
       </c>
       <c r="F44" t="s">
-        <v>61</v>
+        <v>222</v>
       </c>
       <c r="G44" t="s">
-        <v>62</v>
+        <v>223</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>138</v>
+        <v>224</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>139</v>
+        <v>225</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
@@ -3323,26 +3413,28 @@
         <v>22</v>
       </c>
       <c r="B45" s="1">
-        <v>45431</v>
+        <v>45577</v>
       </c>
       <c r="C45" t="s">
-        <v>148</v>
+        <v>231</v>
       </c>
       <c r="D45" s="1">
-        <v>45435</v>
+        <v>45583</v>
       </c>
       <c r="E45" s="4">
-        <v>227.55</v>
+        <v>924.65</v>
       </c>
       <c r="F45" t="s">
-        <v>149</v>
+        <v>75</v>
       </c>
       <c r="G45" t="s">
-        <v>150</v>
-      </c>
-      <c r="H45" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>232</v>
+      </c>
       <c r="I45" s="2" t="s">
-        <v>151</v>
+        <v>233</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>90</v>
@@ -3353,140 +3445,157 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>14</v>
+        <v>73</v>
+      </c>
+      <c r="B46" s="1">
+        <v>45578</v>
       </c>
       <c r="C46" t="s">
-        <v>155</v>
+        <v>220</v>
       </c>
       <c r="D46" s="1">
-        <v>45435</v>
+        <v>45578</v>
       </c>
       <c r="E46" s="4">
-        <v>479.5</v>
-      </c>
-      <c r="F46" t="s">
-        <v>156</v>
-      </c>
-      <c r="G46" t="s">
-        <v>157</v>
+        <v>50.25</v>
       </c>
       <c r="H46" s="2"/>
-      <c r="I46" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J46" s="6" t="s">
-        <v>161</v>
-      </c>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
       <c r="K46" s="2" t="s">
-        <v>162</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="B47" s="1">
+        <v>45578</v>
       </c>
       <c r="C47" t="s">
-        <v>158</v>
+        <v>237</v>
       </c>
       <c r="D47" s="1">
-        <v>45435</v>
+        <v>45589</v>
       </c>
       <c r="E47" s="4">
-        <v>420</v>
+        <v>194.6</v>
       </c>
       <c r="F47" t="s">
-        <v>156</v>
+        <v>33</v>
       </c>
       <c r="G47" t="s">
-        <v>157</v>
-      </c>
-      <c r="H47" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>238</v>
+      </c>
       <c r="I47" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>161</v>
+        <v>239</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>162</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="B48" s="1">
+        <v>45581</v>
       </c>
       <c r="C48" t="s">
-        <v>266</v>
+        <v>227</v>
       </c>
       <c r="D48" s="1">
-        <v>45437</v>
+        <v>45583</v>
       </c>
       <c r="E48" s="4">
-        <f>1140*1.1</f>
-        <v>1254</v>
+        <v>232.4</v>
       </c>
       <c r="F48" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="G48" t="s">
-        <v>8</v>
-      </c>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>229</v>
+      </c>
       <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
+      <c r="K48" s="2" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B49" s="1">
+        <v>45583</v>
       </c>
       <c r="C49" t="s">
-        <v>136</v>
+        <v>242</v>
       </c>
       <c r="D49" s="1">
-        <v>45437</v>
+        <v>45596</v>
       </c>
       <c r="E49" s="4">
-        <v>1200</v>
+        <v>194.6</v>
       </c>
       <c r="F49" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="G49" t="s">
-        <v>56</v>
-      </c>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>22</v>
       </c>
       <c r="B50" s="1">
-        <v>45435</v>
+        <v>45585</v>
       </c>
       <c r="C50" t="s">
-        <v>152</v>
+        <v>250</v>
       </c>
       <c r="D50" s="1">
-        <v>45439</v>
+        <v>45603</v>
       </c>
       <c r="E50" s="4">
-        <v>253.55</v>
+        <v>181.6</v>
       </c>
       <c r="F50" t="s">
-        <v>33</v>
+        <v>178</v>
       </c>
       <c r="G50" t="s">
-        <v>34</v>
+        <v>182</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>154</v>
+        <v>251</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>153</v>
+        <v>252</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>90</v>
@@ -3497,28 +3606,29 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B51" s="1">
+        <v>45590</v>
       </c>
       <c r="C51" t="s">
-        <v>174</v>
+        <v>245</v>
       </c>
       <c r="D51" s="1">
-        <v>45444</v>
+        <v>45593</v>
       </c>
       <c r="E51" s="4">
-        <v>80.150000000000006</v>
+        <v>218.05</v>
       </c>
       <c r="F51" t="s">
-        <v>38</v>
+        <v>246</v>
       </c>
       <c r="G51" t="s">
-        <v>39</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>176</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="H51" s="2"/>
       <c r="I51" s="2" t="s">
-        <v>175</v>
+        <v>248</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>90</v>
@@ -3532,28 +3642,26 @@
         <v>22</v>
       </c>
       <c r="B52" s="1">
-        <v>45412</v>
+        <v>45604</v>
       </c>
       <c r="C52" t="s">
-        <v>181</v>
+        <v>306</v>
       </c>
       <c r="D52" s="1">
-        <v>45460</v>
+        <v>45615</v>
       </c>
       <c r="E52" s="4">
-        <v>214</v>
+        <v>101.12</v>
       </c>
       <c r="F52" t="s">
-        <v>178</v>
+        <v>307</v>
       </c>
       <c r="G52" t="s">
-        <v>182</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>179</v>
-      </c>
+        <v>308</v>
+      </c>
+      <c r="H52" s="2"/>
       <c r="I52" s="2" t="s">
-        <v>183</v>
+        <v>309</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>90</v>
@@ -3564,77 +3672,92 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>17</v>
+        <v>73</v>
+      </c>
+      <c r="B53" s="1">
+        <v>45606</v>
       </c>
       <c r="C53" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="D53" s="1">
-        <v>45468</v>
+        <v>45606</v>
       </c>
       <c r="E53" s="4">
-        <f>1140*1.1</f>
-        <v>1254</v>
+        <v>100</v>
       </c>
       <c r="F53" t="s">
-        <v>7</v>
+        <v>156</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
+      <c r="K53" s="2" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>24</v>
-      </c>
-      <c r="C54" t="s">
-        <v>256</v>
-      </c>
-      <c r="D54" s="1">
-        <v>45468</v>
-      </c>
-      <c r="E54" s="4">
-        <v>1200</v>
-      </c>
-      <c r="F54" t="s">
-        <v>11</v>
-      </c>
-      <c r="G54" t="s">
-        <v>56</v>
-      </c>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
+      <c r="A54" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" s="12">
+        <v>45606</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="D54" s="12">
+        <v>45613</v>
+      </c>
+      <c r="E54" s="15">
+        <v>256.45</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="H54" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="I54" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="J54" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="K54" s="17" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>22</v>
       </c>
       <c r="B55" s="1">
-        <v>45438</v>
+        <v>45626</v>
       </c>
       <c r="C55" t="s">
-        <v>184</v>
+        <v>289</v>
       </c>
       <c r="D55" s="1">
-        <v>45475</v>
+        <v>45636</v>
       </c>
       <c r="E55" s="4">
-        <v>174.6</v>
+        <v>270.25</v>
       </c>
       <c r="F55" t="s">
-        <v>185</v>
+        <v>290</v>
       </c>
       <c r="G55" t="s">
-        <v>186</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>188</v>
+        <v>291</v>
+      </c>
+      <c r="H55" t="s">
+        <v>292</v>
+      </c>
+      <c r="I55">
+        <v>60071014</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>90</v>
@@ -3645,183 +3768,217 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="B56" s="1">
+        <v>45633</v>
       </c>
       <c r="C56" t="s">
-        <v>268</v>
+        <v>293</v>
       </c>
       <c r="D56" s="1">
-        <v>45498</v>
+        <v>45635</v>
       </c>
       <c r="E56" s="4">
-        <f>1140*1.1</f>
-        <v>1254</v>
+        <v>219</v>
       </c>
       <c r="F56" t="s">
-        <v>7</v>
+        <v>50</v>
+      </c>
+      <c r="G56" t="s">
+        <v>51</v>
       </c>
       <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
+      <c r="I56" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="B57" s="1">
+        <v>45634</v>
       </c>
       <c r="C57" t="s">
-        <v>274</v>
+        <v>321</v>
       </c>
       <c r="D57" s="1">
-        <v>45498</v>
+        <v>45665</v>
       </c>
       <c r="E57" s="4">
-        <f>1140*1.1</f>
-        <v>1254</v>
+        <v>172.25</v>
       </c>
       <c r="F57" t="s">
-        <v>156</v>
+        <v>322</v>
       </c>
       <c r="G57" t="s">
-        <v>255</v>
+        <v>323</v>
       </c>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
-      <c r="K57" s="2"/>
+      <c r="J57" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B58" s="1">
+        <v>45638</v>
       </c>
       <c r="C58" t="s">
-        <v>257</v>
+        <v>310</v>
       </c>
       <c r="D58" s="1">
-        <v>45498</v>
+        <v>45653</v>
       </c>
       <c r="E58" s="4">
-        <v>1200</v>
+        <v>262.25</v>
       </c>
       <c r="F58" t="s">
-        <v>11</v>
+        <v>185</v>
       </c>
       <c r="G58" t="s">
-        <v>56</v>
-      </c>
-      <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
-      <c r="J58" s="2"/>
-      <c r="K58" s="2"/>
+        <v>186</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>24</v>
+        <v>73</v>
+      </c>
+      <c r="B59" s="1">
+        <v>45646</v>
       </c>
       <c r="C59" t="s">
-        <v>203</v>
+        <v>303</v>
       </c>
       <c r="D59" s="1">
-        <v>45505</v>
+        <v>45647</v>
       </c>
       <c r="E59" s="4">
-        <v>879.4</v>
+        <v>39.950000000000003</v>
       </c>
       <c r="F59" t="s">
-        <v>204</v>
+        <v>177</v>
       </c>
       <c r="G59" t="s">
-        <v>205</v>
+        <v>223</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>206</v>
+        <v>304</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>207</v>
+        <v>305</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>201</v>
+        <v>90</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>202</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="B60" s="1">
+        <v>45646</v>
       </c>
       <c r="C60" t="s">
-        <v>195</v>
+        <v>297</v>
       </c>
       <c r="D60" s="1">
-        <v>45527</v>
+        <v>45650</v>
       </c>
       <c r="E60" s="4">
-        <v>159</v>
+        <v>426.55</v>
       </c>
       <c r="F60" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="G60" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>196</v>
+        <v>298</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="J60" s="6" t="s">
-        <v>111</v>
+        <v>299</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C61" t="s">
-        <v>269</v>
+        <v>49</v>
       </c>
       <c r="D61" s="1">
-        <v>45529</v>
+        <v>44895</v>
       </c>
       <c r="E61" s="4">
-        <f>1140*1.1</f>
-        <v>1254</v>
+        <v>15.75</v>
       </c>
       <c r="F61" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="G61" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
+      <c r="I61" s="2">
+        <v>42491</v>
+      </c>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C62" t="s">
-        <v>275</v>
+        <v>19</v>
       </c>
       <c r="D62" s="1">
-        <v>45529</v>
+        <v>45316</v>
       </c>
       <c r="E62" s="4">
-        <f>1140*1.1</f>
-        <v>1254</v>
+        <v>34.5</v>
       </c>
       <c r="F62" t="s">
-        <v>156</v>
+        <v>9</v>
       </c>
       <c r="G62" t="s">
-        <v>255</v>
+        <v>10</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
@@ -3830,80 +3987,74 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C63" t="s">
-        <v>258</v>
+        <v>25</v>
       </c>
       <c r="D63" s="1">
-        <v>45529</v>
+        <v>45316</v>
       </c>
       <c r="E63" s="4">
-        <v>1200</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="F63" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G63" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
-      <c r="K63" s="2"/>
+      <c r="K63" s="2" t="s">
+        <v>226</v>
+      </c>
       <c r="L63" s="6"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C64" t="s">
-        <v>198</v>
+        <v>282</v>
       </c>
       <c r="D64" s="1">
-        <v>45534</v>
+        <v>45316</v>
       </c>
       <c r="E64" s="4">
-        <v>13.15</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F64" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="G64" t="s">
-        <v>39</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="I64" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="J64" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K64" s="2" t="s">
-        <v>113</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C65" t="s">
-        <v>270</v>
+        <v>132</v>
       </c>
       <c r="D65" s="1">
-        <v>45560</v>
+        <v>45316</v>
       </c>
       <c r="E65" s="4">
-        <f>1140*1.1</f>
-        <v>1254</v>
+        <v>1200</v>
       </c>
       <c r="F65" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G65" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
@@ -3912,493 +4063,455 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C66" t="s">
+        <v>180</v>
+      </c>
+      <c r="D66" s="1">
+        <v>45322</v>
+      </c>
+      <c r="E66" s="4">
         <v>276</v>
       </c>
-      <c r="D66" s="1">
-        <v>45560</v>
-      </c>
-      <c r="E66" s="4">
-        <f>1140*1.1</f>
-        <v>1254</v>
-      </c>
       <c r="F66" t="s">
-        <v>156</v>
-      </c>
-      <c r="G66" t="s">
-        <v>255</v>
-      </c>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
-      <c r="J66" s="2"/>
-      <c r="K66" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="J66" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="K66" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>24</v>
       </c>
       <c r="C67" t="s">
-        <v>259</v>
+        <v>46</v>
       </c>
       <c r="D67" s="1">
-        <v>45560</v>
+        <v>45329</v>
       </c>
       <c r="E67" s="4">
-        <v>1200</v>
+        <v>35.049999999999997</v>
       </c>
       <c r="F67" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="G67" t="s">
-        <v>56</v>
-      </c>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>22</v>
-      </c>
-      <c r="B68" s="1">
-        <v>45555</v>
+        <v>24</v>
       </c>
       <c r="C68" t="s">
-        <v>189</v>
+        <v>37</v>
       </c>
       <c r="D68" s="1">
-        <v>45562</v>
+        <v>45330</v>
       </c>
       <c r="E68" s="4">
-        <v>180.9</v>
+        <v>100</v>
       </c>
       <c r="F68" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="G68" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="I68" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="J68" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K68" s="2" t="s">
-        <v>113</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C69" t="s">
-        <v>208</v>
+        <v>28</v>
       </c>
       <c r="D69" s="1">
-        <v>45562</v>
+        <v>45331</v>
       </c>
       <c r="E69" s="4">
-        <v>263.89999999999998</v>
+        <v>101</v>
       </c>
       <c r="F69" t="s">
-        <v>209</v>
+        <v>29</v>
       </c>
       <c r="G69" t="s">
-        <v>210</v>
+        <v>30</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>211</v>
+        <v>31</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="J69" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="K69" s="2" t="s">
-        <v>202</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>22</v>
-      </c>
-      <c r="B70" s="1">
-        <v>45557</v>
+        <v>17</v>
       </c>
       <c r="C70" t="s">
-        <v>192</v>
+        <v>281</v>
       </c>
       <c r="D70" s="1">
-        <v>45566</v>
+        <v>45347</v>
       </c>
       <c r="E70" s="4">
-        <v>178.35</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F70" t="s">
-        <v>185</v>
+        <v>7</v>
       </c>
       <c r="G70" t="s">
-        <v>186</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="I70" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="J70" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K70" s="2" t="s">
-        <v>113</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>22</v>
-      </c>
-      <c r="B71" s="1">
-        <v>45562</v>
+        <v>24</v>
       </c>
       <c r="C71" t="s">
-        <v>213</v>
+        <v>133</v>
       </c>
       <c r="D71" s="1">
-        <v>45568</v>
+        <v>45347</v>
       </c>
       <c r="E71" s="4">
-        <v>88.85</v>
+        <v>1200</v>
       </c>
       <c r="F71" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="G71" t="s">
-        <v>62</v>
-      </c>
-      <c r="H71" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="I71" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="J71" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="K71" s="7" t="s">
-        <v>113</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="9"/>
+      <c r="K71" s="7"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>73</v>
-      </c>
-      <c r="B72" s="1">
-        <v>45576</v>
+        <v>24</v>
       </c>
       <c r="C72" t="s">
-        <v>216</v>
+        <v>173</v>
       </c>
       <c r="D72" s="1">
-        <v>45576</v>
+        <v>45352</v>
       </c>
       <c r="E72" s="4">
-        <v>37.700000000000003</v>
-      </c>
-      <c r="H72" s="2"/>
-      <c r="I72" s="2"/>
-      <c r="J72" s="2"/>
+        <v>51.45</v>
+      </c>
+      <c r="F72" t="s">
+        <v>38</v>
+      </c>
+      <c r="G72" t="s">
+        <v>39</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="K72" s="2" t="s">
-        <v>226</v>
+        <v>113</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>73</v>
-      </c>
-      <c r="B73" s="1">
-        <v>45576</v>
+        <v>17</v>
       </c>
       <c r="C73" t="s">
-        <v>217</v>
+        <v>280</v>
       </c>
       <c r="D73" s="1">
-        <v>45576</v>
+        <v>45376</v>
       </c>
       <c r="E73" s="4">
-        <v>116.1</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
+      </c>
+      <c r="F73" t="s">
+        <v>7</v>
+      </c>
+      <c r="G73" t="s">
+        <v>8</v>
       </c>
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
-      <c r="K73" s="2" t="s">
-        <v>226</v>
-      </c>
+      <c r="K73" s="2"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>73</v>
-      </c>
-      <c r="B74" s="1">
-        <v>45576</v>
-      </c>
-      <c r="C74" s="8" t="s">
-        <v>219</v>
+        <v>24</v>
+      </c>
+      <c r="C74" t="s">
+        <v>134</v>
       </c>
       <c r="D74" s="1">
-        <v>45576</v>
+        <v>45376</v>
       </c>
       <c r="E74" s="4">
-        <v>154.80000000000001</v>
+        <v>1200</v>
+      </c>
+      <c r="F74" t="s">
+        <v>11</v>
+      </c>
+      <c r="G74" t="s">
+        <v>56</v>
       </c>
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
-      <c r="K74" s="2" t="s">
-        <v>226</v>
-      </c>
+      <c r="K74" s="2"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>73</v>
-      </c>
-      <c r="B75" s="1">
-        <v>45576</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>218</v>
+        <v>24</v>
+      </c>
+      <c r="C75" t="s">
+        <v>81</v>
       </c>
       <c r="D75" s="1">
-        <v>45576</v>
+        <v>45376</v>
       </c>
       <c r="E75" s="4">
-        <v>102.2</v>
-      </c>
-      <c r="H75" s="2"/>
-      <c r="I75" s="2"/>
-      <c r="J75" s="2"/>
+        <v>25.1</v>
+      </c>
+      <c r="F75" t="s">
+        <v>38</v>
+      </c>
+      <c r="G75" t="s">
+        <v>39</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="K75" s="2" t="s">
-        <v>226</v>
+        <v>113</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>73</v>
-      </c>
-      <c r="B76" s="1">
-        <v>45576</v>
+        <v>17</v>
       </c>
       <c r="C76" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="D76" s="1">
-        <v>45576</v>
+        <v>45407</v>
       </c>
       <c r="E76" s="4">
-        <v>30.7</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
+      </c>
+      <c r="F76" t="s">
+        <v>7</v>
+      </c>
+      <c r="G76" t="s">
+        <v>8</v>
       </c>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
       <c r="J76" s="9"/>
-      <c r="K76" s="7" t="s">
-        <v>226</v>
-      </c>
+      <c r="K76" s="7"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>73</v>
-      </c>
-      <c r="B77" s="1">
-        <v>45578</v>
+        <v>24</v>
       </c>
       <c r="C77" t="s">
-        <v>220</v>
+        <v>135</v>
       </c>
       <c r="D77" s="1">
-        <v>45578</v>
+        <v>45407</v>
       </c>
       <c r="E77" s="4">
-        <v>50.25</v>
+        <v>1200</v>
+      </c>
+      <c r="F77" t="s">
+        <v>11</v>
+      </c>
+      <c r="G77" t="s">
+        <v>56</v>
       </c>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
-      <c r="K77" s="2" t="s">
-        <v>226</v>
-      </c>
+      <c r="K77" s="2"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>73</v>
-      </c>
-      <c r="B78" s="1">
-        <v>45576</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>221</v>
+        <v>14</v>
+      </c>
+      <c r="C78" t="s">
+        <v>155</v>
       </c>
       <c r="D78" s="1">
-        <v>45579</v>
+        <v>45435</v>
       </c>
       <c r="E78" s="4">
-        <v>279.89999999999998</v>
+        <v>479.5</v>
       </c>
       <c r="F78" t="s">
-        <v>222</v>
+        <v>156</v>
       </c>
       <c r="G78" t="s">
-        <v>223</v>
-      </c>
-      <c r="H78" s="2" t="s">
-        <v>224</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="H78" s="2"/>
       <c r="I78" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="J78" s="2" t="s">
-        <v>111</v>
+        <v>159</v>
+      </c>
+      <c r="J78" s="6" t="s">
+        <v>161</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>112</v>
+        <v>162</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>22</v>
-      </c>
-      <c r="B79" s="1">
-        <v>45577</v>
+        <v>14</v>
       </c>
       <c r="C79" t="s">
-        <v>231</v>
+        <v>158</v>
       </c>
       <c r="D79" s="1">
-        <v>45583</v>
+        <v>45435</v>
       </c>
       <c r="E79" s="4">
-        <v>924.65</v>
+        <v>420</v>
       </c>
       <c r="F79" t="s">
-        <v>75</v>
+        <v>156</v>
       </c>
       <c r="G79" t="s">
-        <v>76</v>
-      </c>
-      <c r="H79" s="2" t="s">
-        <v>232</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="H79" s="2"/>
       <c r="I79" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="J79" s="2" t="s">
-        <v>90</v>
+        <v>160</v>
+      </c>
+      <c r="J79" s="6" t="s">
+        <v>161</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>22</v>
-      </c>
-      <c r="B80" s="1">
-        <v>45581</v>
+        <v>17</v>
       </c>
       <c r="C80" t="s">
-        <v>227</v>
+        <v>266</v>
       </c>
       <c r="D80" s="1">
-        <v>45583</v>
+        <v>45437</v>
       </c>
       <c r="E80" s="4">
-        <v>232.4</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F80" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="G80" t="s">
-        <v>62</v>
-      </c>
-      <c r="H80" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="I80" s="2" t="s">
-        <v>229</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
       <c r="J80" s="2"/>
-      <c r="K80" s="2" t="s">
-        <v>230</v>
-      </c>
+      <c r="K80" s="2"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>22</v>
-      </c>
-      <c r="B81" s="1">
-        <v>45571</v>
+        <v>24</v>
       </c>
       <c r="C81" t="s">
-        <v>240</v>
+        <v>136</v>
       </c>
       <c r="D81" s="1">
-        <v>45588</v>
+        <v>45437</v>
       </c>
       <c r="E81" s="4">
-        <v>181.6</v>
+        <v>1200</v>
       </c>
       <c r="F81" t="s">
-        <v>178</v>
+        <v>11</v>
       </c>
       <c r="G81" t="s">
-        <v>182</v>
-      </c>
-      <c r="H81" t="s">
-        <v>241</v>
-      </c>
-      <c r="I81" s="2">
-        <v>10053082</v>
-      </c>
-      <c r="J81" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K81" s="2" t="s">
-        <v>113</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+      <c r="J81" s="2"/>
+      <c r="K81" s="2"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>22</v>
-      </c>
-      <c r="B82" s="1">
-        <v>45578</v>
+        <v>24</v>
       </c>
       <c r="C82" t="s">
-        <v>237</v>
+        <v>174</v>
       </c>
       <c r="D82" s="1">
-        <v>45589</v>
+        <v>45444</v>
       </c>
       <c r="E82" s="4">
-        <v>194.6</v>
+        <v>80.150000000000006</v>
       </c>
       <c r="F82" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G82" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>238</v>
+        <v>176</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>239</v>
+        <v>175</v>
       </c>
       <c r="J82" s="2" t="s">
         <v>90</v>
@@ -4412,10 +4525,10 @@
         <v>17</v>
       </c>
       <c r="C83" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D83" s="1">
-        <v>45590</v>
+        <v>45468</v>
       </c>
       <c r="E83" s="4">
         <f>1140*1.1</f>
@@ -4423,9 +4536,6 @@
       </c>
       <c r="F83" t="s">
         <v>7</v>
-      </c>
-      <c r="G83" t="s">
-        <v>8</v>
       </c>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
@@ -4434,23 +4544,22 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C84" t="s">
-        <v>277</v>
+        <v>256</v>
       </c>
       <c r="D84" s="1">
-        <v>45590</v>
+        <v>45468</v>
       </c>
       <c r="E84" s="4">
-        <f>1140*1.1</f>
-        <v>1254</v>
+        <v>1200</v>
       </c>
       <c r="F84" t="s">
-        <v>156</v>
+        <v>11</v>
       </c>
       <c r="G84" t="s">
-        <v>255</v>
+        <v>56</v>
       </c>
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
@@ -4459,22 +4568,20 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C85" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="D85" s="1">
-        <v>45590</v>
+        <v>45498</v>
       </c>
       <c r="E85" s="4">
-        <v>1200</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F85" t="s">
-        <v>11</v>
-      </c>
-      <c r="G85" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
@@ -4483,275 +4590,242 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>22</v>
-      </c>
-      <c r="B86" s="1">
-        <v>45590</v>
+        <v>17</v>
       </c>
       <c r="C86" t="s">
-        <v>245</v>
+        <v>274</v>
       </c>
       <c r="D86" s="1">
-        <v>45593</v>
+        <v>45498</v>
       </c>
       <c r="E86" s="4">
-        <v>218.05</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F86" t="s">
-        <v>246</v>
+        <v>156</v>
       </c>
       <c r="G86" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="H86" s="2"/>
-      <c r="I86" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="J86" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K86" s="2" t="s">
-        <v>113</v>
-      </c>
+      <c r="I86" s="2"/>
+      <c r="J86" s="2"/>
+      <c r="K86" s="2"/>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>22</v>
-      </c>
-      <c r="B87" s="1">
-        <v>45583</v>
+        <v>24</v>
       </c>
       <c r="C87" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="D87" s="1">
-        <v>45596</v>
+        <v>45498</v>
       </c>
       <c r="E87" s="4">
-        <v>194.6</v>
+        <v>1200</v>
       </c>
       <c r="F87" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="G87" t="s">
-        <v>53</v>
-      </c>
-      <c r="H87" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="I87" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="J87" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K87" s="2" t="s">
-        <v>113</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2"/>
+      <c r="K87" s="2"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>22</v>
-      </c>
-      <c r="B88" s="1">
-        <v>45585</v>
+        <v>24</v>
       </c>
       <c r="C88" t="s">
-        <v>250</v>
+        <v>203</v>
       </c>
       <c r="D88" s="1">
-        <v>45603</v>
+        <v>45505</v>
       </c>
       <c r="E88" s="4">
-        <v>181.6</v>
+        <v>879.4</v>
       </c>
       <c r="F88" t="s">
-        <v>178</v>
+        <v>204</v>
       </c>
       <c r="G88" t="s">
-        <v>182</v>
+        <v>205</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>251</v>
+        <v>206</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>252</v>
+        <v>207</v>
       </c>
       <c r="J88" s="2" t="s">
-        <v>90</v>
+        <v>201</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>73</v>
-      </c>
-      <c r="B89" s="1">
-        <v>45606</v>
+        <v>15</v>
       </c>
       <c r="C89" t="s">
-        <v>253</v>
+        <v>195</v>
       </c>
       <c r="D89" s="1">
-        <v>45606</v>
+        <v>45527</v>
       </c>
       <c r="E89" s="4">
-        <v>100</v>
+        <v>159</v>
       </c>
       <c r="F89" t="s">
-        <v>156</v>
-      </c>
-      <c r="H89" s="2"/>
-      <c r="I89" s="2"/>
-      <c r="J89" s="2"/>
-      <c r="K89" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="G89" t="s">
+        <v>30</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="J89" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A90" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B90" s="12">
-        <v>45606</v>
-      </c>
-      <c r="C90" s="10" t="s">
-        <v>283</v>
-      </c>
-      <c r="D90" s="12">
-        <v>45613</v>
-      </c>
-      <c r="E90" s="15">
-        <v>256.45</v>
-      </c>
-      <c r="F90" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="G90" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="H90" s="17" t="s">
-        <v>284</v>
-      </c>
-      <c r="I90" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="J90" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="K90" s="17" t="s">
-        <v>113</v>
-      </c>
+      <c r="A90" t="s">
+        <v>17</v>
+      </c>
+      <c r="C90" t="s">
+        <v>269</v>
+      </c>
+      <c r="D90" s="1">
+        <v>45529</v>
+      </c>
+      <c r="E90" s="4">
+        <f>1140*1.1</f>
+        <v>1254</v>
+      </c>
+      <c r="F90" t="s">
+        <v>7</v>
+      </c>
+      <c r="G90" t="s">
+        <v>8</v>
+      </c>
+      <c r="H90" s="2"/>
+      <c r="I90" s="2"/>
+      <c r="J90" s="2"/>
+      <c r="K90" s="2"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>22</v>
-      </c>
-      <c r="B91" s="1">
-        <v>45604</v>
+        <v>17</v>
       </c>
       <c r="C91" t="s">
-        <v>306</v>
+        <v>275</v>
       </c>
       <c r="D91" s="1">
-        <v>45615</v>
+        <v>45529</v>
       </c>
       <c r="E91" s="4">
-        <v>101.12</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F91" t="s">
-        <v>307</v>
+        <v>156</v>
       </c>
       <c r="G91" t="s">
-        <v>308</v>
+        <v>255</v>
       </c>
       <c r="H91" s="2"/>
-      <c r="I91" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="J91" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K91" s="2" t="s">
-        <v>113</v>
-      </c>
+      <c r="I91" s="2"/>
+      <c r="J91" s="2"/>
+      <c r="K91" s="2"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>24</v>
       </c>
       <c r="C92" t="s">
-        <v>286</v>
+        <v>258</v>
       </c>
       <c r="D92" s="1">
-        <v>45618</v>
+        <v>45529</v>
       </c>
       <c r="E92" s="4">
-        <v>68.08</v>
+        <v>1200</v>
       </c>
       <c r="F92" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="G92" t="s">
-        <v>39</v>
-      </c>
-      <c r="H92" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="I92" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="J92" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K92" s="2" t="s">
-        <v>113</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+      <c r="K92" s="2"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C93" t="s">
-        <v>272</v>
+        <v>198</v>
       </c>
       <c r="D93" s="1">
-        <v>45621</v>
+        <v>45534</v>
       </c>
       <c r="E93" s="4">
-        <f>1140*1.1</f>
-        <v>1254</v>
+        <v>13.15</v>
       </c>
       <c r="F93" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="G93" t="s">
-        <v>8</v>
-      </c>
-      <c r="H93" s="2"/>
-      <c r="I93" s="2"/>
-      <c r="J93" s="2"/>
-      <c r="K93" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="I93" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="J93" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K93" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>17</v>
       </c>
       <c r="C94" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="D94" s="1">
-        <v>45621</v>
+        <v>45560</v>
       </c>
       <c r="E94" s="4">
         <f>1140*1.1</f>
         <v>1254</v>
       </c>
       <c r="F94" t="s">
-        <v>156</v>
+        <v>7</v>
       </c>
       <c r="G94" t="s">
-        <v>255</v>
+        <v>8</v>
       </c>
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
@@ -4760,22 +4834,23 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C95" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
       <c r="D95" s="1">
-        <v>45621</v>
+        <v>45560</v>
       </c>
       <c r="E95" s="4">
-        <v>1200</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F95" t="s">
-        <v>11</v>
+        <v>156</v>
       </c>
       <c r="G95" t="s">
-        <v>56</v>
+        <v>255</v>
       </c>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
@@ -4784,218 +4859,186 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B96" s="13">
-        <v>45633</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B96" s="13"/>
       <c r="C96" s="14" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
       <c r="D96" s="13">
-        <v>45635</v>
+        <v>45560</v>
       </c>
       <c r="E96" s="16">
-        <v>219</v>
+        <v>1200</v>
       </c>
       <c r="F96" s="14" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="G96" s="14" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="H96" s="18"/>
-      <c r="I96" s="18" t="s">
-        <v>294</v>
-      </c>
-      <c r="J96" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="K96" s="19" t="s">
-        <v>113</v>
-      </c>
+      <c r="I96" s="18"/>
+      <c r="J96" s="18"/>
+      <c r="K96" s="19"/>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>22</v>
-      </c>
-      <c r="B97" s="1">
-        <v>45626</v>
+        <v>24</v>
       </c>
       <c r="C97" t="s">
-        <v>289</v>
+        <v>208</v>
       </c>
       <c r="D97" s="1">
-        <v>45636</v>
+        <v>45562</v>
       </c>
       <c r="E97" s="4">
-        <v>270.25</v>
+        <v>263.89999999999998</v>
       </c>
       <c r="F97" t="s">
-        <v>290</v>
+        <v>209</v>
       </c>
       <c r="G97" t="s">
-        <v>291</v>
-      </c>
-      <c r="H97" t="s">
-        <v>292</v>
-      </c>
-      <c r="I97">
-        <v>60071014</v>
+        <v>210</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="I97" s="2" t="s">
+        <v>212</v>
       </c>
       <c r="J97" s="2" t="s">
-        <v>90</v>
+        <v>201</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C98" t="s">
-        <v>300</v>
+        <v>271</v>
       </c>
       <c r="D98" s="1">
-        <v>45638</v>
+        <v>45590</v>
       </c>
       <c r="E98" s="4">
-        <v>69.5</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F98" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="G98" t="s">
-        <v>30</v>
-      </c>
-      <c r="H98" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="I98" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="J98" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="K98" s="2" t="s">
-        <v>112</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H98" s="2"/>
+      <c r="I98" s="2"/>
+      <c r="J98" s="2"/>
+      <c r="K98" s="2"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>73</v>
-      </c>
-      <c r="B99" s="1">
-        <v>45646</v>
+        <v>17</v>
       </c>
       <c r="C99" t="s">
-        <v>303</v>
+        <v>277</v>
       </c>
       <c r="D99" s="1">
-        <v>45647</v>
+        <v>45590</v>
       </c>
       <c r="E99" s="4">
-        <v>39.950000000000003</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F99" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="G99" t="s">
-        <v>223</v>
-      </c>
-      <c r="H99" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="I99" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="J99" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K99" s="2" t="s">
-        <v>113</v>
-      </c>
+        <v>255</v>
+      </c>
+      <c r="H99" s="2"/>
+      <c r="I99" s="2"/>
+      <c r="J99" s="2"/>
+      <c r="K99" s="2"/>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>22</v>
-      </c>
-      <c r="B100" s="1">
-        <v>45646</v>
+        <v>24</v>
       </c>
       <c r="C100" t="s">
-        <v>297</v>
+        <v>260</v>
       </c>
       <c r="D100" s="1">
-        <v>45650</v>
+        <v>45590</v>
       </c>
       <c r="E100" s="4">
-        <v>426.55</v>
+        <v>1200</v>
       </c>
       <c r="F100" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="G100" t="s">
-        <v>62</v>
-      </c>
-      <c r="H100" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="I100" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="J100" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K100" s="2" t="s">
-        <v>113</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H100" s="2"/>
+      <c r="I100" s="2"/>
+      <c r="J100" s="2"/>
+      <c r="K100" s="2"/>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C101" t="s">
-        <v>273</v>
+        <v>286</v>
       </c>
       <c r="D101" s="1">
-        <v>45651</v>
+        <v>45618</v>
       </c>
       <c r="E101" s="4">
-        <f>1140*1.1</f>
-        <v>1254</v>
+        <v>68.08</v>
       </c>
       <c r="F101" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="G101" t="s">
-        <v>8</v>
-      </c>
-      <c r="H101" s="2"/>
-      <c r="I101" s="2"/>
-      <c r="J101" s="2"/>
-      <c r="K101" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="J101" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K101" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>17</v>
       </c>
       <c r="C102" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="D102" s="1">
-        <v>45651</v>
+        <v>45621</v>
       </c>
       <c r="E102" s="4">
         <f>1140*1.1</f>
         <v>1254</v>
       </c>
       <c r="F102" t="s">
-        <v>156</v>
+        <v>7</v>
       </c>
       <c r="G102" t="s">
-        <v>255</v>
+        <v>8</v>
       </c>
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
@@ -5004,22 +5047,23 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C103" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
       <c r="D103" s="1">
-        <v>45651</v>
+        <v>45621</v>
       </c>
       <c r="E103" s="4">
-        <v>1200</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F103" t="s">
-        <v>11</v>
+        <v>156</v>
       </c>
       <c r="G103" t="s">
-        <v>56</v>
+        <v>255</v>
       </c>
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
@@ -5028,169 +5072,149 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>22</v>
-      </c>
-      <c r="B104" s="1">
-        <v>45638</v>
+        <v>24</v>
       </c>
       <c r="C104" t="s">
-        <v>310</v>
+        <v>261</v>
       </c>
       <c r="D104" s="1">
-        <v>45653</v>
+        <v>45621</v>
       </c>
       <c r="E104" s="4">
-        <v>262.25</v>
+        <v>1200</v>
       </c>
       <c r="F104" t="s">
-        <v>185</v>
+        <v>11</v>
       </c>
       <c r="G104" t="s">
-        <v>186</v>
-      </c>
-      <c r="H104" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="I104" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="J104" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K104" s="2" t="s">
-        <v>113</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H104" s="2"/>
+      <c r="I104" s="2"/>
+      <c r="J104" s="2"/>
+      <c r="K104" s="2"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>22</v>
-      </c>
-      <c r="B105" s="1">
-        <v>45543</v>
+        <v>15</v>
       </c>
       <c r="C105" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="D105" s="1">
-        <v>45614</v>
+        <v>45638</v>
       </c>
       <c r="E105" s="4">
-        <v>86.75</v>
+        <v>69.5</v>
       </c>
       <c r="F105" t="s">
-        <v>314</v>
+        <v>29</v>
       </c>
       <c r="G105" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="I105" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="J105" s="2" t="s">
-        <v>90</v>
+        <v>302</v>
+      </c>
+      <c r="J105" s="6" t="s">
+        <v>111</v>
       </c>
       <c r="K105" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>22</v>
-      </c>
-      <c r="B106" s="1">
-        <v>45634</v>
+        <v>17</v>
       </c>
       <c r="C106" t="s">
-        <v>321</v>
+        <v>273</v>
       </c>
       <c r="D106" s="1">
-        <v>45665</v>
+        <v>45651</v>
       </c>
       <c r="E106" s="4">
-        <v>172.25</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F106" t="s">
-        <v>322</v>
+        <v>7</v>
       </c>
       <c r="G106" t="s">
-        <v>323</v>
+        <v>8</v>
       </c>
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
-      <c r="J106" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K106" s="2" t="s">
-        <v>113</v>
-      </c>
+      <c r="J106" s="2"/>
+      <c r="K106" s="2"/>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>73</v>
-      </c>
-      <c r="B107" s="1">
-        <v>45371</v>
+        <v>17</v>
       </c>
       <c r="C107" t="s">
-        <v>324</v>
+        <v>279</v>
       </c>
       <c r="D107" s="1">
-        <v>45323</v>
+        <v>45651</v>
       </c>
       <c r="E107" s="4">
-        <v>12.9</v>
+        <f>1140*1.1</f>
+        <v>1254</v>
       </c>
       <c r="F107" t="s">
-        <v>325</v>
+        <v>156</v>
+      </c>
+      <c r="G107" t="s">
+        <v>255</v>
       </c>
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
-      <c r="K107" s="2" t="s">
-        <v>226</v>
-      </c>
+      <c r="K107" s="2"/>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C108" t="s">
-        <v>326</v>
+        <v>262</v>
       </c>
       <c r="D108" s="1">
-        <v>45310</v>
+        <v>45651</v>
       </c>
       <c r="E108" s="4">
-        <v>42.54</v>
+        <v>1200</v>
       </c>
       <c r="F108" t="s">
-        <v>327</v>
+        <v>11</v>
+      </c>
+      <c r="G108" t="s">
+        <v>56</v>
       </c>
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>
-      <c r="K108" s="2" t="s">
-        <v>226</v>
-      </c>
+      <c r="K108" s="2"/>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>15</v>
       </c>
       <c r="C109" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D109" s="1">
-        <v>45330</v>
+        <v>45310</v>
       </c>
       <c r="E109" s="4">
-        <v>11.6</v>
+        <v>42.54</v>
       </c>
       <c r="F109" t="s">
-        <v>327</v>
+        <v>7</v>
       </c>
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
@@ -5201,23 +5225,19 @@
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>73</v>
-      </c>
-      <c r="B110" s="1">
-        <v>45333</v>
+        <v>15</v>
       </c>
       <c r="C110" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D110" s="1">
         <v>45330</v>
       </c>
       <c r="E110" s="4">
-        <f>36.16-11.6</f>
-        <v>24.559999999999995</v>
+        <v>11.6</v>
       </c>
       <c r="F110" t="s">
-        <v>327</v>
+        <v>7</v>
       </c>
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>
@@ -5231,7 +5251,7 @@
         <v>15</v>
       </c>
       <c r="C111" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D111" s="1">
         <v>45341</v>
@@ -5240,7 +5260,7 @@
         <v>61.32</v>
       </c>
       <c r="F111" t="s">
-        <v>327</v>
+        <v>7</v>
       </c>
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
@@ -5250,54 +5270,204 @@
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E112" s="4"/>
-    </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E113" s="4"/>
-    </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E114" s="4"/>
-    </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E115" s="4"/>
-    </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E116" s="4"/>
-    </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E117" s="4"/>
-    </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E118" s="4"/>
-    </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>15</v>
+      </c>
+      <c r="C112" t="s">
+        <v>331</v>
+      </c>
+      <c r="D112" s="1">
+        <v>45549</v>
+      </c>
+      <c r="E112" s="4">
+        <v>30.75</v>
+      </c>
+      <c r="F112" t="s">
+        <v>7</v>
+      </c>
+      <c r="H112" s="2"/>
+      <c r="I112" s="2"/>
+      <c r="J112" s="2"/>
+      <c r="K112" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>15</v>
+      </c>
+      <c r="C113" t="s">
+        <v>331</v>
+      </c>
+      <c r="D113" s="1">
+        <v>45583</v>
+      </c>
+      <c r="E113" s="4">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="F113" t="s">
+        <v>7</v>
+      </c>
+      <c r="H113" s="2"/>
+      <c r="I113" s="2"/>
+      <c r="J113" s="2"/>
+      <c r="K113" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>15</v>
+      </c>
+      <c r="C114" t="s">
+        <v>331</v>
+      </c>
+      <c r="D114" s="1">
+        <v>45542</v>
+      </c>
+      <c r="E114" s="4">
+        <v>14.3</v>
+      </c>
+      <c r="F114" t="s">
+        <v>7</v>
+      </c>
+      <c r="H114" s="2"/>
+      <c r="I114" s="2"/>
+      <c r="J114" s="2"/>
+      <c r="K114" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>15</v>
+      </c>
+      <c r="C115" t="s">
+        <v>331</v>
+      </c>
+      <c r="D115" s="1">
+        <v>45549</v>
+      </c>
+      <c r="E115" s="4">
+        <v>30.75</v>
+      </c>
+      <c r="F115" t="s">
+        <v>7</v>
+      </c>
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
+      <c r="J115" s="2"/>
+      <c r="K115" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>15</v>
+      </c>
+      <c r="C116" t="s">
+        <v>331</v>
+      </c>
+      <c r="D116" s="1">
+        <v>45400</v>
+      </c>
+      <c r="E116" s="4">
+        <v>34.450000000000003</v>
+      </c>
+      <c r="F116" t="s">
+        <v>7</v>
+      </c>
+      <c r="H116" s="2"/>
+      <c r="I116" s="2"/>
+      <c r="J116" s="2"/>
+      <c r="K116" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>15</v>
+      </c>
+      <c r="C117" t="s">
+        <v>331</v>
+      </c>
+      <c r="D117" s="1">
+        <v>45358</v>
+      </c>
+      <c r="E117" s="4">
+        <v>33.950000000000003</v>
+      </c>
+      <c r="F117" t="s">
+        <v>7</v>
+      </c>
+      <c r="H117" s="2"/>
+      <c r="I117" s="2"/>
+      <c r="J117" s="2"/>
+      <c r="K117" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>22</v>
+      </c>
+      <c r="B118" s="1">
+        <v>45625</v>
+      </c>
+      <c r="C118" t="s">
+        <v>332</v>
+      </c>
+      <c r="D118" s="1">
+        <v>45689</v>
+      </c>
+      <c r="E118" s="4">
+        <v>161.19999999999999</v>
+      </c>
+      <c r="F118" t="s">
+        <v>333</v>
+      </c>
+      <c r="G118" t="s">
+        <v>147</v>
+      </c>
+      <c r="H118" s="2"/>
+      <c r="I118">
+        <v>967</v>
+      </c>
+      <c r="J118" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K118" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E119" s="4"/>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E120" s="4"/>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E121" s="4"/>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E122" s="4"/>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E123" s="4"/>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E124" s="4"/>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E125" s="4"/>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E126" s="4"/>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E127" s="4"/>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E128" s="4"/>
     </row>
     <row r="129" spans="5:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Rechnung Crazy for Gelato
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D55AFE5-851A-44C9-9590-DC5E7C6E00F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579E152A-97FB-4F74-81B2-28DD280E09D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="337">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -1040,6 +1040,15 @@
   </si>
   <si>
     <t>Gehaltszahlung Betriebsleitung Nadia März 24</t>
+  </si>
+  <si>
+    <t>Gelati Kiosk für 2. saison 2024</t>
+  </si>
+  <si>
+    <t>Crazy for Gelato AG</t>
+  </si>
+  <si>
+    <t>Zilstrasse 40, 5722 Gränichen</t>
   </si>
 </sst>
 </file>
@@ -1241,8 +1250,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K119" totalsRowShown="0">
-  <autoFilter ref="A1:K119" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K120" totalsRowShown="0">
+  <autoFilter ref="A1:K120" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:K113">
     <sortCondition ref="D2:D119"/>
     <sortCondition ref="C2:C119"/>
@@ -1576,7 +1585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -1983,8 +1992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M217"/>
   <sheetViews>
-    <sheetView zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="G97" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K121" sqref="K121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5441,7 +5450,32 @@
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E120" s="4"/>
+      <c r="A120" t="s">
+        <v>15</v>
+      </c>
+      <c r="C120" t="s">
+        <v>334</v>
+      </c>
+      <c r="D120" s="1">
+        <v>45636</v>
+      </c>
+      <c r="E120" s="4">
+        <v>540</v>
+      </c>
+      <c r="F120" t="s">
+        <v>335</v>
+      </c>
+      <c r="G120" t="s">
+        <v>336</v>
+      </c>
+      <c r="H120" s="2"/>
+      <c r="I120" s="2"/>
+      <c r="J120" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K120" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E121" s="4"/>

</xml_diff>

<commit_message>
New feature: More than one film per day will be supported. Date and Suisa are used to determine
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E3369A-B267-412F-8C09-7319EDDC04D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC523572-A0D0-4E5F-B916-FA042DC01CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="4395" yWindow="1650" windowWidth="28770" windowHeight="15450" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>4407 Unterhalt</t>
+  </si>
+  <si>
+    <t>Suisanummer</t>
   </si>
 </sst>
 </file>
@@ -202,7 +205,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{27287C1A-B7AC-49C2-89D9-0074BB2DB80A}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -222,7 +225,13 @@
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
@@ -241,16 +250,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}" name="Table3" displayName="Table3" ref="A1:G2" totalsRowShown="0">
-  <autoFilter ref="A1:G2" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}" name="Table3" displayName="Table3" ref="A1:H2" totalsRowShown="0">
+  <autoFilter ref="A1:H2" xr:uid="{895BE82C-25E7-42D8-B99F-BB1A7DC4B1DC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H2">
     <sortCondition ref="A1:A2"/>
   </sortState>
-  <tableColumns count="7">
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3D23B81F-00E6-4787-9893-D2AE611E1A32}" name="Kategorie"/>
     <tableColumn id="2" xr3:uid="{4A3D2615-9D9C-4A35-9563-6454B477091D}" name="Bezeichnung"/>
-    <tableColumn id="5" xr3:uid="{CCC1A9CA-28D8-4BE0-BEDE-BE707C85139A}" name="Datum" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{DEF99A8A-2830-4960-A91D-1A789B2E195A}" name="Betrag" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{CCC1A9CA-28D8-4BE0-BEDE-BE707C85139A}" name="Datum" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{B572771D-D07E-4D8C-8302-8B1C2808427A}" name="Suisanummer" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{DEF99A8A-2830-4960-A91D-1A789B2E195A}" name="Betrag" dataDxfId="7"/>
     <tableColumn id="7" xr3:uid="{EC0FDCA3-B34E-4378-9B61-6671AF218B0B}" name="Firmennamen"/>
     <tableColumn id="8" xr3:uid="{359B982D-E085-4831-8FE0-859B1B4314AD}" name="Adresse"/>
     <tableColumn id="10" xr3:uid="{02367AEA-A5FC-4D0B-90AF-F9D0D56EB4A0}" name="Rechnungsnummer"/>
@@ -260,14 +270,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:J5" totalsRowShown="0">
-  <autoFilter ref="A1:J5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K5" totalsRowShown="0">
+  <autoFilter ref="A1:K5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K4">
     <sortCondition ref="A1:A4"/>
   </sortState>
-  <tableColumns count="10">
+  <tableColumns count="11">
     <tableColumn id="9" xr3:uid="{7720D0EA-5763-4F4F-82DA-8D34884933A7}" name="Kategorie"/>
-    <tableColumn id="8" xr3:uid="{12477251-A7BF-41F7-9734-91E55C44981E}" name="Spieldatum" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{12477251-A7BF-41F7-9734-91E55C44981E}" name="Spieldatum" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{90784966-A7C8-41A3-8EC0-117CDC7DFB09}" name="Suisanummer" dataDxfId="5"/>
     <tableColumn id="1" xr3:uid="{CADC5726-010C-420F-B3D1-E5B1B323B7D4}" name="Bezeichnung"/>
     <tableColumn id="2" xr3:uid="{48234371-EC10-4470-8D2A-22FC4E54CF28}" name="Datum" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{90883362-F5C5-4472-9591-164F8C364C6F}" name="Betrag" dataDxfId="3"/>
@@ -601,24 +612,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.28515625" customWidth="1"/>
     <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.42578125" customWidth="1"/>
+    <col min="3" max="4" width="15.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -628,16 +639,19 @@
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -663,485 +677,489 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
-  <dimension ref="A1:K114"/>
+  <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31" customWidth="1"/>
+    <col min="8" max="8" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>45682</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <f>1140*1.1</f>
         <v>1254</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="5"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K2" s="2"/>
+      <c r="L2" s="5"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>45713</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <f>1140*1.1</f>
         <v>1254</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>45682</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>1200</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>45671</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>40</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>26</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E35" s="3"/>
-    </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E36" s="3"/>
-    </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E37" s="3"/>
-    </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E38" s="3"/>
-    </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E39" s="3"/>
-    </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E40" s="3"/>
-    </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E41" s="3"/>
-    </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E43" s="3"/>
-    </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E44" s="3"/>
-    </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E45" s="3"/>
-    </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E46" s="3"/>
-    </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E47" s="3"/>
-    </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E48" s="3"/>
-    </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E49" s="3"/>
-    </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E50" s="3"/>
-    </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E51" s="3"/>
-    </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E52" s="3"/>
-    </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E53" s="3"/>
-    </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E54" s="3"/>
-    </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E55" s="3"/>
-    </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E56" s="3"/>
-    </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E57" s="3"/>
-    </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E58" s="3"/>
-    </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E59" s="3"/>
-    </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E60" s="3"/>
-    </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E61" s="3"/>
-    </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E62" s="3"/>
-    </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E63" s="3"/>
-    </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E64" s="3"/>
-    </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E65" s="3"/>
-    </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E66" s="3"/>
-    </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E67" s="3"/>
-    </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E68" s="3"/>
-    </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E69" s="3"/>
-    </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E70" s="3"/>
-    </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E71" s="3"/>
-    </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E72" s="3"/>
-    </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E73" s="3"/>
-    </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E74" s="3"/>
-    </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E75" s="3"/>
-    </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E76" s="3"/>
-    </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E77" s="3"/>
-    </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E78" s="3"/>
-    </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E79" s="3"/>
-    </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E80" s="3"/>
-    </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E81" s="3"/>
-    </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E82" s="3"/>
-    </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E83" s="3"/>
-    </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E84" s="3"/>
-    </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E85" s="3"/>
-    </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E86" s="3"/>
-    </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E87" s="3"/>
-    </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E88" s="3"/>
-    </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E89" s="3"/>
-    </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E90" s="3"/>
-    </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E91" s="3"/>
-    </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E92" s="3"/>
-    </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E93" s="3"/>
-    </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E94" s="3"/>
-    </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E95" s="3"/>
-    </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E96" s="3"/>
-    </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E97" s="3"/>
-    </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E98" s="3"/>
-    </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E99" s="3"/>
-    </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E100" s="3"/>
-    </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E101" s="3"/>
-    </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E102" s="3"/>
-    </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E103" s="3"/>
-    </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E104" s="3"/>
-    </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E105" s="3"/>
-    </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E106" s="3"/>
-    </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E107" s="3"/>
-    </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E108" s="3"/>
-    </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E109" s="3"/>
-    </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E110" s="3"/>
-    </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E111" s="3"/>
-    </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E112" s="3"/>
-    </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E113" s="3"/>
-    </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E114" s="3"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F45" s="3"/>
+    </row>
+    <row r="46" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="3"/>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F50" s="3"/>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F51" s="3"/>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F60" s="3"/>
+    </row>
+    <row r="61" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F65" s="3"/>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F66" s="3"/>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F67" s="3"/>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F68" s="3"/>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F69" s="3"/>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F70" s="3"/>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F71" s="3"/>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F72" s="3"/>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F73" s="3"/>
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F74" s="3"/>
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F75" s="3"/>
+    </row>
+    <row r="76" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F76" s="3"/>
+    </row>
+    <row r="77" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F77" s="3"/>
+    </row>
+    <row r="78" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F78" s="3"/>
+    </row>
+    <row r="79" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F79" s="3"/>
+    </row>
+    <row r="80" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F80" s="3"/>
+    </row>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F81" s="3"/>
+    </row>
+    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F82" s="3"/>
+    </row>
+    <row r="83" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F83" s="3"/>
+    </row>
+    <row r="84" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F84" s="3"/>
+    </row>
+    <row r="85" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F85" s="3"/>
+    </row>
+    <row r="86" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F86" s="3"/>
+    </row>
+    <row r="87" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F87" s="3"/>
+    </row>
+    <row r="88" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F88" s="3"/>
+    </row>
+    <row r="89" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F89" s="3"/>
+    </row>
+    <row r="90" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F90" s="3"/>
+    </row>
+    <row r="91" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F91" s="3"/>
+    </row>
+    <row r="92" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F92" s="3"/>
+    </row>
+    <row r="93" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F93" s="3"/>
+    </row>
+    <row r="94" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F94" s="3"/>
+    </row>
+    <row r="95" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F95" s="3"/>
+    </row>
+    <row r="96" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F96" s="3"/>
+    </row>
+    <row r="97" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F97" s="3"/>
+    </row>
+    <row r="98" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F98" s="3"/>
+    </row>
+    <row r="99" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F99" s="3"/>
+    </row>
+    <row r="100" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F100" s="3"/>
+    </row>
+    <row r="101" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F101" s="3"/>
+    </row>
+    <row r="102" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F102" s="3"/>
+    </row>
+    <row r="103" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F103" s="3"/>
+    </row>
+    <row r="104" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F104" s="3"/>
+    </row>
+    <row r="105" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F105" s="3"/>
+    </row>
+    <row r="106" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F106" s="3"/>
+    </row>
+    <row r="107" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F107" s="3"/>
+    </row>
+    <row r="108" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F108" s="3"/>
+    </row>
+    <row r="109" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F109" s="3"/>
+    </row>
+    <row r="110" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F110" s="3"/>
+    </row>
+    <row r="111" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F111" s="3"/>
+    </row>
+    <row r="112" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F112" s="3"/>
+    </row>
+    <row r="113" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F113" s="3"/>
+    </row>
+    <row r="114" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F114" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1162,7 +1180,7 @@
           <x14:formula1>
             <xm:f>Konten!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>J1:J1048576</xm:sqref>
+          <xm:sqref>K1:K1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1174,7 +1192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFEBA5D-FF22-4032-BB29-794CF56A632B}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Rechnung: Flow, Typisch Emil und Johan. Eintritte & kiosk 7.2.25 Der vierer
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC523572-A0D0-4E5F-B916-FA042DC01CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37392E8A-B0F7-42C2-9660-F40DD9B3C67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4395" yWindow="1650" windowWidth="28770" windowHeight="15450" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="6720" yWindow="3180" windowWidth="15684" windowHeight="11832" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -147,6 +147,51 @@
   </si>
   <si>
     <t>Suisanummer</t>
+  </si>
+  <si>
+    <t>1020.643</t>
+  </si>
+  <si>
+    <t>Film: Flow</t>
+  </si>
+  <si>
+    <t>Xenix Filmdistribution GmbH</t>
+  </si>
+  <si>
+    <t>Weberstrasse 21, CH 8004 Zürich</t>
+  </si>
+  <si>
+    <t>1020.514</t>
+  </si>
+  <si>
+    <t>Film: Everybody Hates Johan</t>
+  </si>
+  <si>
+    <t>Pathe Films AG</t>
+  </si>
+  <si>
+    <t>Neugasse 6, Postfach, 8031 Zürich</t>
+  </si>
+  <si>
+    <t>93 88771 00200 00000 06007 19602</t>
+  </si>
+  <si>
+    <t>60071960</t>
+  </si>
+  <si>
+    <t>1020.828</t>
+  </si>
+  <si>
+    <t>Film: Typisch Emil</t>
+  </si>
+  <si>
+    <t>Filmcoopi Zürich AG</t>
+  </si>
+  <si>
+    <t>Heinrichstrasse 114, 8005 Zürich</t>
+  </si>
+  <si>
+    <t>98 85900 00000 00000 00009 17792</t>
   </si>
 </sst>
 </file>
@@ -157,7 +202,7 @@
     <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +216,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -180,10 +231,49 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -193,17 +283,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{27287C1A-B7AC-49C2-89D9-0074BB2DB80A}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -270,8 +367,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K5" totalsRowShown="0">
-  <autoFilter ref="A1:K5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K8" totalsRowShown="0">
+  <autoFilter ref="A1:K8" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K4">
     <sortCondition ref="A1:A4"/>
   </sortState>
@@ -316,9 +413,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -356,7 +453,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -462,7 +559,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -614,22 +711,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.44140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.42578125" customWidth="1"/>
+    <col min="8" max="8" width="42.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -679,26 +776,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:L114"/>
   <sheetViews>
-    <sheetView zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" customWidth="1"/>
-    <col min="8" max="8" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -733,7 +830,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -758,7 +855,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -782,7 +879,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -805,7 +902,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -834,334 +931,429 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45676</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="1">
+        <v>45691</v>
+      </c>
+      <c r="F6" s="3">
+        <v>170</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2">
+        <v>48060</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45682</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="1">
+        <v>45692</v>
+      </c>
+      <c r="F7" s="3">
+        <v>181.6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="9">
+        <v>45667</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="9">
+        <v>45694</v>
+      </c>
+      <c r="F8" s="11">
+        <v>121</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="12">
+        <v>91779</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F51" s="3"/>
     </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F53" s="3"/>
     </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F54" s="3"/>
     </row>
-    <row r="55" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F55" s="3"/>
     </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F56" s="3"/>
     </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F57" s="3"/>
     </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F58" s="3"/>
     </row>
-    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F59" s="3"/>
     </row>
-    <row r="60" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F60" s="3"/>
     </row>
-    <row r="61" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F61" s="3"/>
     </row>
-    <row r="62" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F62" s="3"/>
     </row>
-    <row r="63" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F63" s="3"/>
     </row>
-    <row r="64" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F64" s="3"/>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F65" s="3"/>
     </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F66" s="3"/>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F67" s="3"/>
     </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F68" s="3"/>
     </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F69" s="3"/>
     </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F70" s="3"/>
     </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F71" s="3"/>
     </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F72" s="3"/>
     </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F73" s="3"/>
     </row>
-    <row r="74" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F74" s="3"/>
     </row>
-    <row r="75" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F75" s="3"/>
     </row>
-    <row r="76" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F76" s="3"/>
     </row>
-    <row r="77" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F77" s="3"/>
     </row>
-    <row r="78" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F78" s="3"/>
     </row>
-    <row r="79" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F79" s="3"/>
     </row>
-    <row r="80" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F80" s="3"/>
     </row>
-    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F81" s="3"/>
     </row>
-    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F82" s="3"/>
     </row>
-    <row r="83" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F83" s="3"/>
     </row>
-    <row r="84" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F84" s="3"/>
     </row>
-    <row r="85" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F85" s="3"/>
     </row>
-    <row r="86" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F86" s="3"/>
     </row>
-    <row r="87" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F87" s="3"/>
     </row>
-    <row r="88" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F88" s="3"/>
     </row>
-    <row r="89" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F89" s="3"/>
     </row>
-    <row r="90" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F90" s="3"/>
     </row>
-    <row r="91" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F91" s="3"/>
     </row>
-    <row r="92" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F92" s="3"/>
     </row>
-    <row r="93" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F93" s="3"/>
     </row>
-    <row r="94" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F94" s="3"/>
     </row>
-    <row r="95" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F95" s="3"/>
     </row>
-    <row r="96" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F96" s="3"/>
     </row>
-    <row r="97" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F97" s="3"/>
     </row>
-    <row r="98" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F98" s="3"/>
     </row>
-    <row r="99" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F99" s="3"/>
     </row>
-    <row r="100" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F100" s="3"/>
     </row>
-    <row r="101" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F101" s="3"/>
     </row>
-    <row r="102" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F102" s="3"/>
     </row>
-    <row r="103" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F103" s="3"/>
     </row>
-    <row r="104" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F104" s="3"/>
     </row>
-    <row r="105" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F105" s="3"/>
     </row>
-    <row r="106" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F106" s="3"/>
     </row>
-    <row r="107" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F107" s="3"/>
     </row>
-    <row r="108" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F108" s="3"/>
     </row>
-    <row r="109" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F109" s="3"/>
     </row>
-    <row r="110" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F110" s="3"/>
     </row>
-    <row r="111" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F111" s="3"/>
     </row>
-    <row r="112" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F112" s="3"/>
     </row>
-    <row r="113" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F113" s="3"/>
     </row>
-    <row r="114" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F114" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -1169,7 +1361,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{551055D3-EB54-4023-842C-CF79CAE47FBC}">
           <x14:formula1>
             <xm:f>dropdown!$A$2:$A$8</xm:f>
@@ -1196,48 +1388,48 @@
       <selection activeCell="D1" sqref="D1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1258,32 +1450,32 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Filmabrechnunng Weihnachten in der Schustergasse
</commit_message>
<xml_diff>
--- a/Input/Einnahmen und Ausgaben.xlsx
+++ b/Input/Einnahmen und Ausgaben.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DD56C5-43DA-4B2A-8C6B-07F77822186E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B412A982-D5B2-4876-9D39-F10A8CA42364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="18576" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
+    <workbookView xWindow="1344" yWindow="3324" windowWidth="15684" windowHeight="11832" activeTab="1" xr2:uid="{D194CBB7-18DA-440A-A6D7-06C22280DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Einnahmen" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="343">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -1055,6 +1055,18 @@
   </si>
   <si>
     <t>241166TS</t>
+  </si>
+  <si>
+    <t>Film: Weihnachten in der Schustergasse</t>
+  </si>
+  <si>
+    <t>Capeligth pictures OHG</t>
+  </si>
+  <si>
+    <t>Lessingstrasse 16, 16356 Ahresfelde</t>
+  </si>
+  <si>
+    <t>Rechnung 136 / 2024</t>
   </si>
 </sst>
 </file>
@@ -1256,8 +1268,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K120" totalsRowShown="0">
-  <autoFilter ref="A1:K120" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}" name="Table16" displayName="Table16" ref="A1:K121" totalsRowShown="0">
+  <autoFilter ref="A1:K121" xr:uid="{DECE9D5D-00D4-4490-AE11-80617FB82945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:K113">
     <sortCondition ref="D2:D119"/>
     <sortCondition ref="C2:C119"/>
@@ -1591,7 +1603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72045E-24F3-4DFF-AD02-E9648BA6850D}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+    <sheetView topLeftCell="D2" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -2024,8 +2036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D174BE7-BB11-4664-AEC1-AB301D6C9797}">
   <dimension ref="A1:M217"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E129" sqref="E129"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5510,7 +5522,37 @@
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E121" s="4"/>
+      <c r="A121" t="s">
+        <v>22</v>
+      </c>
+      <c r="B121" s="1">
+        <v>45641</v>
+      </c>
+      <c r="C121" t="s">
+        <v>339</v>
+      </c>
+      <c r="D121" s="1">
+        <v>45657</v>
+      </c>
+      <c r="E121" s="4">
+        <v>150</v>
+      </c>
+      <c r="F121" t="s">
+        <v>340</v>
+      </c>
+      <c r="G121" t="s">
+        <v>341</v>
+      </c>
+      <c r="H121" s="2"/>
+      <c r="I121" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="J121" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K121" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E122" s="4"/>

</xml_diff>